<commit_message>
update data april 4 2024
</commit_message>
<xml_diff>
--- a/pembayaran/Pembayaran.xlsx
+++ b/pembayaran/Pembayaran.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/277ffa1efc2bfcc1/Apartment Bintaro/Data Harian/BINTARO-APG/pembayaran/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="938" documentId="11_0B1D56BE9CDCCE836B02CE7A5FB0D4A9BBFD1C62" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{041CE381-6DB3-413F-BE8E-E34F00BCF28B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE676B13-7CC7-47E4-A985-8FC0BD1E4FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="74">
   <si>
     <t>Tanggal Pembayaran</t>
   </si>
@@ -726,8 +726,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="C80" sqref="C80"/>
+    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="110" workbookViewId="0">
+      <selection activeCell="B99" sqref="B99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3094,9 +3094,6 @@
       <c r="M100" s="1"/>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A101" s="6">
-        <v>45385</v>
-      </c>
       <c r="B101" t="s">
         <v>24</v>
       </c>
@@ -3152,23 +3149,105 @@
       <c r="M102" s="1"/>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A103" s="6">
+        <v>45385</v>
+      </c>
+      <c r="B103" t="s">
+        <v>24</v>
+      </c>
+      <c r="C103" t="s">
+        <v>25</v>
+      </c>
+      <c r="D103" s="6">
+        <v>45292</v>
+      </c>
+      <c r="E103" s="8">
+        <v>45384</v>
+      </c>
+      <c r="F103" s="1">
+        <v>789000</v>
+      </c>
+      <c r="G103" s="1">
+        <v>789000</v>
+      </c>
+      <c r="H103" s="1">
+        <v>93000</v>
+      </c>
       <c r="I103" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="J103" s="1">
+        <v>300000</v>
+      </c>
+      <c r="K103" s="1">
+        <f>G103+H103-J103</f>
+        <v>582000</v>
+      </c>
       <c r="M103" s="1"/>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A104" s="6">
+        <v>45386</v>
+      </c>
+      <c r="B104" t="s">
+        <v>57</v>
+      </c>
+      <c r="D104" s="6">
+        <v>45352</v>
+      </c>
+      <c r="E104" s="8">
+        <v>45384</v>
+      </c>
+      <c r="F104" s="1">
+        <v>27678000</v>
+      </c>
+      <c r="G104" s="1">
+        <v>27678000</v>
+      </c>
       <c r="I104" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="J104" s="1">
+        <v>20000000</v>
+      </c>
+      <c r="K104" s="1">
+        <f>G104+H104-J104</f>
+        <v>7678000</v>
+      </c>
       <c r="M104" s="1"/>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>14</v>
+      </c>
+      <c r="D105" s="6">
+        <v>45360</v>
+      </c>
+      <c r="E105" s="8">
+        <v>45384</v>
+      </c>
+      <c r="F105" s="1">
+        <v>35306000</v>
+      </c>
+      <c r="G105" s="1">
+        <v>35306000</v>
+      </c>
+      <c r="H105" s="1">
+        <f>K53+K83</f>
+        <v>19616000</v>
+      </c>
       <c r="I105" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
+      </c>
+      <c r="J105" s="1">
+        <v>30230000</v>
+      </c>
+      <c r="K105" s="1">
+        <f>G105+H105-J105</f>
+        <v>24692000</v>
       </c>
       <c r="M105" s="1"/>
     </row>

</xml_diff>

<commit_message>
update pembayaran purwadi & ipin
</commit_message>
<xml_diff>
--- a/pembayaran/Pembayaran.xlsx
+++ b/pembayaran/Pembayaran.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/277ffa1efc2bfcc1/Apartment Bintaro/Data Harian/BINTARO-APG/pembayaran/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bpsbi\OneDrive\Apartment Bintaro\Data Harian\BINTARO-APG\pembayaran\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE676B13-7CC7-47E4-A985-8FC0BD1E4FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32182262-DA5C-4AD4-AF8D-4F6823BD515F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="74">
   <si>
     <t>Tanggal Pembayaran</t>
   </si>
@@ -262,8 +262,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -301,7 +302,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -323,6 +324,12 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -384,8 +391,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}" name="Table1" displayName="Table1" ref="A1:M106" totalsRowShown="0" headerRowDxfId="10">
-  <autoFilter ref="A1:M106" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}" name="Table1" displayName="Table1" ref="A1:M108" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A1:M108" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{ADAEF761-889D-4642-B4B1-5AD983017E99}" name="Tanggal Pembayaran" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{1D148A0B-5DE6-485F-ABBF-15493C92DBA8}" name="Nama Mandor"/>
@@ -724,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O106"/>
+  <dimension ref="A1:O108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="110" workbookViewId="0">
-      <selection activeCell="B99" sqref="B99"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="110" workbookViewId="0">
+      <selection activeCell="G101" sqref="G101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3249,14 +3256,92 @@
         <f>G105+H105-J105</f>
         <v>24692000</v>
       </c>
+      <c r="L105" s="1">
+        <v>150000</v>
+      </c>
       <c r="M105" s="1"/>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A106" s="6">
+        <v>45387</v>
+      </c>
+      <c r="B106" t="s">
+        <v>54</v>
+      </c>
+      <c r="D106" s="6">
+        <v>45373</v>
+      </c>
+      <c r="E106" s="8">
+        <v>45386</v>
+      </c>
+      <c r="F106" s="1">
+        <v>3718000</v>
+      </c>
+      <c r="G106" s="1">
+        <v>3718000</v>
+      </c>
+      <c r="H106" s="1">
+        <v>0</v>
+      </c>
       <c r="I106" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
+      <c r="J106" s="1">
+        <v>3657000</v>
+      </c>
+      <c r="K106" s="1">
+        <f>G106+H106-J106</f>
+        <v>61000</v>
+      </c>
+      <c r="L106" s="1">
+        <v>100000</v>
+      </c>
       <c r="M106" s="1"/>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A107" s="9"/>
+      <c r="B107" t="s">
+        <v>28</v>
+      </c>
+      <c r="C107" t="s">
+        <v>67</v>
+      </c>
+      <c r="D107" s="9">
+        <v>45381</v>
+      </c>
+      <c r="E107" s="10">
+        <v>45386</v>
+      </c>
+      <c r="F107" s="1">
+        <v>225000</v>
+      </c>
+      <c r="G107" s="1">
+        <v>225000</v>
+      </c>
+      <c r="H107" s="1">
+        <v>0</v>
+      </c>
+      <c r="I107" s="1">
+        <f>F107-G107</f>
+        <v>0</v>
+      </c>
+      <c r="J107" s="1">
+        <v>225000</v>
+      </c>
+      <c r="K107" s="1">
+        <f>G107+H107-J107</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A108" s="9"/>
+      <c r="D108" s="9"/>
+      <c r="E108" s="10"/>
+      <c r="I108" s="1">
+        <f>F108-G108</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update 31 may 2024
</commit_message>
<xml_diff>
--- a/pembayaran/Pembayaran.xlsx
+++ b/pembayaran/Pembayaran.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/277ffa1efc2bfcc1/Apartment Bintaro/Data Harian/BINTARO-APG/pembayaran/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="252" documentId="8_{CE676B13-7CC7-47E4-A985-8FC0BD1E4FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EF3FCB7-9515-47F0-890B-CF554F30656B}"/>
+  <xr:revisionPtr revIDLastSave="420" documentId="8_{CE676B13-7CC7-47E4-A985-8FC0BD1E4FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{512DB859-446F-4F89-9B25-77DA3A1F3E26}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="94">
   <si>
     <t>Tanggal Pembayaran</t>
   </si>
@@ -108,7 +110,7 @@
     <t>Aroy</t>
   </si>
   <si>
-    <t>pembayaran pertama 13 des 2023</t>
+    <t>gabung tgl 13 des 2023</t>
   </si>
   <si>
     <t>Security</t>
@@ -186,63 +188,75 @@
     <t>Opik</t>
   </si>
   <si>
+    <t>gabung tgl 05 feb 2024</t>
+  </si>
+  <si>
+    <t>Turman</t>
+  </si>
+  <si>
+    <t>Sarana</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Diran</t>
+  </si>
+  <si>
+    <t>Sargani</t>
+  </si>
+  <si>
+    <t>gabung tgl  25 feb 2024</t>
+  </si>
+  <si>
+    <t>Purwadi</t>
+  </si>
+  <si>
+    <t>lunas tgl 25 feb 2024</t>
+  </si>
+  <si>
+    <t>Parjo</t>
+  </si>
+  <si>
+    <t>Manggi</t>
+  </si>
+  <si>
+    <t>lunas tgl 17 mar 2024</t>
+  </si>
+  <si>
+    <t>gabung  tgl 11 mar 2024</t>
+  </si>
+  <si>
+    <t>Saiman</t>
+  </si>
+  <si>
+    <t>lunas tgl 29 mar 2024</t>
+  </si>
+  <si>
+    <t>Nano</t>
+  </si>
+  <si>
+    <t>Rizal</t>
+  </si>
+  <si>
+    <t>Firman</t>
+  </si>
+  <si>
+    <t>Mugo</t>
+  </si>
+  <si>
+    <t>Faisal</t>
+  </si>
+  <si>
     <t>belum lunas</t>
   </si>
   <si>
-    <t>Turman</t>
-  </si>
-  <si>
-    <t>Sarana</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Diran</t>
-  </si>
-  <si>
-    <t>Sargani</t>
-  </si>
-  <si>
-    <t>Purwadi</t>
-  </si>
-  <si>
-    <t>lunas tgl 25 feb 2024</t>
-  </si>
-  <si>
-    <t>Parjo</t>
-  </si>
-  <si>
-    <t>Manggi</t>
-  </si>
-  <si>
-    <t>lunas tgl 17 mar 2024</t>
-  </si>
-  <si>
-    <t>Saiman</t>
-  </si>
-  <si>
-    <t>lunas tgl 29 mar 2024</t>
-  </si>
-  <si>
-    <t>Nano</t>
-  </si>
-  <si>
-    <t>Rizal</t>
-  </si>
-  <si>
-    <t>Firman</t>
-  </si>
-  <si>
-    <t>Mugo</t>
-  </si>
-  <si>
-    <t>Faisal</t>
-  </si>
-  <si>
     <t>Rosiin</t>
   </si>
   <si>
+    <t>gabung tgl 04 apr 2024</t>
+  </si>
+  <si>
     <t>Ipin</t>
   </si>
   <si>
@@ -267,30 +281,53 @@
     <t>gabung tgl  05 apr 2024</t>
   </si>
   <si>
+    <t>lunas tgl 02 mei 2024</t>
+  </si>
+  <si>
     <t>gabung tgl 03 apr 2024</t>
   </si>
   <si>
+    <t>lunas tgl 27 apr 2024</t>
+  </si>
+  <si>
+    <t>gabung tgl 04 mei 2024</t>
+  </si>
+  <si>
+    <t>lunas tgl 04 mei 2024</t>
+  </si>
+  <si>
+    <t>gabung tgl 15 mei 2024</t>
+  </si>
+  <si>
     <t>Alvian</t>
   </si>
   <si>
     <t>Dede</t>
   </si>
   <si>
-    <t>lunas tgl 27 apr 2024</t>
-  </si>
-  <si>
-    <t>lunas tgl 02 mei 2024</t>
+    <t>gabung tgl 18 mei 2024</t>
+  </si>
+  <si>
+    <t>Aceng</t>
+  </si>
+  <si>
+    <t>Fatoni</t>
+  </si>
+  <si>
+    <t>Haji Skun</t>
+  </si>
+  <si>
+    <t>Amin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,7 +363,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -348,12 +385,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -386,15 +417,15 @@
       <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="right"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
@@ -418,8 +449,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}" name="Table1" displayName="Table1" ref="A1:N106" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A1:N106" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}" name="Table1" displayName="Table1" ref="A1:N124" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A1:N124" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{ADAEF761-889D-4642-B4B1-5AD983017E99}" name="Tanggal Pembayaran" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{1D148A0B-5DE6-485F-ABBF-15493C92DBA8}" name="Nama Mandor"/>
@@ -430,7 +461,7 @@
     <tableColumn id="7" xr3:uid="{8424FE3E-B023-4FE2-AF52-93DAEEA191A0}" name="Tertagih" dataDxfId="6"/>
     <tableColumn id="4" xr3:uid="{4517E20A-4B2D-4011-9A2E-1E60F705359A}" name="Kurang Sebelumnya" dataDxfId="5"/>
     <tableColumn id="13" xr3:uid="{25384B78-313F-40B0-AA79-73F412F48A23}" name="Beda Tagihan" dataDxfId="4">
-      <calculatedColumnFormula>F2-G2</calculatedColumnFormula>
+      <calculatedColumnFormula>G2-F2</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{923A0758-378C-4EF9-BEC9-0DB21D69B2B6}" name="Pembayaran" dataDxfId="3"/>
     <tableColumn id="14" xr3:uid="{92AA36DD-3FF7-4461-B3D5-7E2605084332}" name="Kurang Bayar Sekarang" dataDxfId="2">
@@ -763,13 +794,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P106"/>
+  <dimension ref="A1:P124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScale="110" workbookViewId="0">
-      <selection activeCell="N79" sqref="N79"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="110" workbookViewId="0">
+      <selection activeCell="J125" sqref="J125"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
@@ -782,7 +813,7 @@
     <col min="15" max="15" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -826,7 +857,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="6">
         <v>45233</v>
       </c>
@@ -843,8 +874,8 @@
         <v>2702000</v>
       </c>
       <c r="I2" s="1">
-        <f t="shared" ref="I2:I33" si="0">F2-G2</f>
-        <v>-2702000</v>
+        <f t="shared" ref="I2:I33" si="0">G2-F2</f>
+        <v>2702000</v>
       </c>
       <c r="J2" s="1">
         <v>2702000</v>
@@ -858,7 +889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="6">
         <v>45234</v>
       </c>
@@ -876,7 +907,7 @@
       </c>
       <c r="I3" s="1">
         <f t="shared" si="0"/>
-        <v>-13654000</v>
+        <v>13654000</v>
       </c>
       <c r="J3" s="1">
         <v>13654000</v>
@@ -890,7 +921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="6">
         <v>45248</v>
       </c>
@@ -908,7 +939,7 @@
       </c>
       <c r="I4" s="1">
         <f t="shared" si="0"/>
-        <v>-11649000</v>
+        <v>11649000</v>
       </c>
       <c r="J4" s="1">
         <v>6450000</v>
@@ -925,7 +956,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -943,7 +974,7 @@
       </c>
       <c r="I5" s="1">
         <f t="shared" si="0"/>
-        <v>-545000</v>
+        <v>545000</v>
       </c>
       <c r="J5" s="1">
         <v>545000</v>
@@ -957,7 +988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="C6" t="s">
         <v>19</v>
       </c>
@@ -972,7 +1003,7 @@
       </c>
       <c r="I6" s="1">
         <f t="shared" si="0"/>
-        <v>-448000</v>
+        <v>448000</v>
       </c>
       <c r="J6" s="1">
         <v>448000</v>
@@ -986,7 +1017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="C7" t="s">
         <v>20</v>
       </c>
@@ -1001,7 +1032,7 @@
       </c>
       <c r="I7" s="1">
         <f t="shared" si="0"/>
-        <v>-96000</v>
+        <v>96000</v>
       </c>
       <c r="J7" s="1">
         <v>96000</v>
@@ -1015,7 +1046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="C8" t="s">
         <v>21</v>
       </c>
@@ -1030,7 +1061,7 @@
       </c>
       <c r="I8" s="1">
         <f t="shared" si="0"/>
-        <v>-101000</v>
+        <v>101000</v>
       </c>
       <c r="J8" s="1">
         <v>101000</v>
@@ -1044,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -1062,7 +1093,7 @@
       </c>
       <c r="I9" s="1">
         <f t="shared" si="0"/>
-        <v>-53000</v>
+        <v>53000</v>
       </c>
       <c r="J9" s="1">
         <v>53000</v>
@@ -1076,7 +1107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -1091,7 +1122,7 @@
       </c>
       <c r="I10" s="1">
         <f t="shared" si="0"/>
-        <v>-10846000</v>
+        <v>10846000</v>
       </c>
       <c r="J10" s="1">
         <v>10846000</v>
@@ -1105,7 +1136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -1120,7 +1151,7 @@
       </c>
       <c r="I11" s="1">
         <f t="shared" si="0"/>
-        <v>-9355000</v>
+        <v>9355000</v>
       </c>
       <c r="J11" s="1">
         <v>5355000</v>
@@ -1137,7 +1168,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -1173,7 +1204,7 @@
       </c>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="C13" t="s">
         <v>27</v>
       </c>
@@ -1206,7 +1237,7 @@
       </c>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="C14" t="s">
         <v>28</v>
       </c>
@@ -1221,7 +1252,7 @@
       </c>
       <c r="I14" s="1">
         <f t="shared" si="0"/>
-        <v>-380000</v>
+        <v>380000</v>
       </c>
       <c r="J14" s="1">
         <v>380000</v>
@@ -1236,7 +1267,7 @@
       </c>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="6">
         <v>45252</v>
       </c>
@@ -1257,7 +1288,7 @@
       </c>
       <c r="I15" s="1">
         <f t="shared" si="0"/>
-        <v>-394000</v>
+        <v>394000</v>
       </c>
       <c r="J15" s="1">
         <v>394000</v>
@@ -1273,7 +1304,7 @@
       <c r="N15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="6">
         <v>45261</v>
       </c>
@@ -1291,7 +1322,7 @@
       </c>
       <c r="I16" s="1">
         <f t="shared" si="0"/>
-        <v>-5768000</v>
+        <v>5768000</v>
       </c>
       <c r="J16" s="1">
         <v>5768000</v>
@@ -1309,7 +1340,7 @@
       </c>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -1327,7 +1358,7 @@
       </c>
       <c r="I17" s="1">
         <f t="shared" si="0"/>
-        <v>-14697000</v>
+        <v>14697000</v>
       </c>
       <c r="J17" s="1">
         <v>16697000</v>
@@ -1347,7 +1378,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" s="6">
         <v>45273</v>
       </c>
@@ -1369,7 +1400,7 @@
       </c>
       <c r="I18" s="1">
         <f t="shared" si="0"/>
-        <v>-14425000</v>
+        <v>14425000</v>
       </c>
       <c r="J18" s="1">
         <v>7000000</v>
@@ -1386,7 +1417,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19" s="6">
         <v>45275</v>
       </c>
@@ -1403,11 +1434,11 @@
         <v>21027000</v>
       </c>
       <c r="H19" s="1">
-        <v>2000000</v>
+        <v>4000000</v>
       </c>
       <c r="I19" s="1">
         <f t="shared" si="0"/>
-        <v>-21027000</v>
+        <v>21027000</v>
       </c>
       <c r="J19" s="1">
         <v>17545000</v>
@@ -1418,7 +1449,7 @@
       </c>
       <c r="L19" s="1">
         <f t="shared" si="2"/>
-        <v>5482000</v>
+        <v>7482000</v>
       </c>
       <c r="M19" s="1">
         <v>100000</v>
@@ -1427,7 +1458,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="B20" t="s">
         <v>23</v>
       </c>
@@ -1442,7 +1473,7 @@
       </c>
       <c r="I20" s="1">
         <f t="shared" si="0"/>
-        <v>-4912000</v>
+        <v>4912000</v>
       </c>
       <c r="J20" s="1">
         <v>4912000</v>
@@ -1460,7 +1491,7 @@
       </c>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="B21" t="s">
         <v>34</v>
       </c>
@@ -1478,7 +1509,7 @@
       </c>
       <c r="I21" s="1">
         <f t="shared" si="0"/>
-        <v>-163000</v>
+        <v>163000</v>
       </c>
       <c r="J21" s="1">
         <v>0</v>
@@ -1495,7 +1526,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="C22" t="s">
         <v>37</v>
       </c>
@@ -1510,7 +1541,7 @@
       </c>
       <c r="I22" s="1">
         <f t="shared" si="0"/>
-        <v>-177000</v>
+        <v>177000</v>
       </c>
       <c r="J22" s="1">
         <v>9</v>
@@ -1527,7 +1558,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="6">
         <v>45277</v>
       </c>
@@ -1548,7 +1579,7 @@
       </c>
       <c r="I23" s="1">
         <f t="shared" si="0"/>
-        <v>-524000</v>
+        <v>524000</v>
       </c>
       <c r="J23" s="1">
         <v>524000</v>
@@ -1563,7 +1594,7 @@
       </c>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="B24" t="s">
         <v>25</v>
       </c>
@@ -1581,7 +1612,7 @@
       </c>
       <c r="I24" s="1">
         <f t="shared" si="0"/>
-        <v>-105000</v>
+        <v>105000</v>
       </c>
       <c r="J24" s="1">
         <v>105000</v>
@@ -1596,7 +1627,7 @@
       </c>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="B25" t="s">
         <v>17</v>
       </c>
@@ -1614,7 +1645,7 @@
       </c>
       <c r="I25" s="1">
         <f t="shared" si="0"/>
-        <v>-398000</v>
+        <v>398000</v>
       </c>
       <c r="J25" s="1">
         <v>398000</v>
@@ -1629,7 +1660,7 @@
       </c>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="C26" t="s">
         <v>39</v>
       </c>
@@ -1644,7 +1675,7 @@
       </c>
       <c r="I26" s="1">
         <f t="shared" si="0"/>
-        <v>-521000</v>
+        <v>521000</v>
       </c>
       <c r="J26" s="1">
         <v>521000</v>
@@ -1659,7 +1690,7 @@
       </c>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="C27" t="s">
         <v>40</v>
       </c>
@@ -1674,7 +1705,7 @@
       </c>
       <c r="I27" s="1">
         <f t="shared" si="0"/>
-        <v>-165000</v>
+        <v>165000</v>
       </c>
       <c r="J27" s="1">
         <v>165000</v>
@@ -1689,7 +1720,7 @@
       </c>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="B28" t="s">
         <v>15</v>
       </c>
@@ -1707,7 +1738,7 @@
       </c>
       <c r="I28" s="1">
         <f t="shared" si="0"/>
-        <v>-18320000</v>
+        <v>18320000</v>
       </c>
       <c r="J28" s="1">
         <v>16600000</v>
@@ -1727,7 +1758,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="6">
         <v>45289</v>
       </c>
@@ -1748,7 +1779,7 @@
       </c>
       <c r="I29" s="1">
         <f t="shared" si="0"/>
-        <v>-18125000</v>
+        <v>18125000</v>
       </c>
       <c r="J29" s="1">
         <v>17889000</v>
@@ -1765,7 +1796,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="B30" t="s">
         <v>14</v>
       </c>
@@ -1783,7 +1814,7 @@
       </c>
       <c r="I30" s="1">
         <f t="shared" si="0"/>
-        <v>-17409000</v>
+        <v>17409000</v>
       </c>
       <c r="J30" s="1">
         <f>14909000+5482000</f>
@@ -1804,7 +1835,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14">
       <c r="A31" s="6">
         <v>45290</v>
       </c>
@@ -1825,7 +1856,7 @@
       </c>
       <c r="I31" s="1">
         <f t="shared" si="0"/>
-        <v>-288000</v>
+        <v>288000</v>
       </c>
       <c r="J31" s="1">
         <v>288000</v>
@@ -1840,7 +1871,7 @@
       </c>
       <c r="N31" s="1"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14">
       <c r="C32" t="s">
         <v>44</v>
       </c>
@@ -1855,7 +1886,7 @@
       </c>
       <c r="I32" s="1">
         <f t="shared" si="0"/>
-        <v>-230000</v>
+        <v>230000</v>
       </c>
       <c r="J32" s="1">
         <v>230000</v>
@@ -1870,7 +1901,7 @@
       </c>
       <c r="N32" s="1"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16">
       <c r="C33" t="s">
         <v>45</v>
       </c>
@@ -1885,7 +1916,7 @@
       </c>
       <c r="I33" s="1">
         <f t="shared" si="0"/>
-        <v>-225000</v>
+        <v>225000</v>
       </c>
       <c r="J33" s="1">
         <v>225000</v>
@@ -1900,7 +1931,7 @@
       </c>
       <c r="N33" s="1"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16">
       <c r="C34" t="s">
         <v>46</v>
       </c>
@@ -1914,8 +1945,8 @@
         <v>147000</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" ref="I34:I65" si="3">F34-G34</f>
-        <v>-147000</v>
+        <f t="shared" ref="I34:I65" si="3">G34-F34</f>
+        <v>147000</v>
       </c>
       <c r="J34" s="1">
         <v>147000</v>
@@ -1930,7 +1961,7 @@
       </c>
       <c r="N34" s="1"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16">
       <c r="C35" t="s">
         <v>47</v>
       </c>
@@ -1945,7 +1976,7 @@
       </c>
       <c r="I35" s="1">
         <f t="shared" si="3"/>
-        <v>-60000</v>
+        <v>60000</v>
       </c>
       <c r="J35" s="1">
         <v>60000</v>
@@ -1960,7 +1991,7 @@
       </c>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16">
       <c r="C36" t="s">
         <v>48</v>
       </c>
@@ -1975,7 +2006,7 @@
       </c>
       <c r="I36" s="1">
         <f t="shared" si="3"/>
-        <v>-147000</v>
+        <v>147000</v>
       </c>
       <c r="J36" s="1">
         <v>147000</v>
@@ -1991,7 +2022,7 @@
       <c r="N36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16">
       <c r="A37" s="6">
         <v>45305</v>
       </c>
@@ -2012,7 +2043,7 @@
       </c>
       <c r="I37" s="1">
         <f t="shared" si="3"/>
-        <v>-19307000</v>
+        <v>19307000</v>
       </c>
       <c r="J37" s="1">
         <f>16675000+2500000</f>
@@ -2033,7 +2064,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16">
       <c r="A38" s="6">
         <v>45309</v>
       </c>
@@ -2054,7 +2085,7 @@
       </c>
       <c r="I38" s="1">
         <f t="shared" si="3"/>
-        <v>-511000</v>
+        <v>511000</v>
       </c>
       <c r="J38" s="1">
         <v>511000</v>
@@ -2069,7 +2100,7 @@
       </c>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16">
       <c r="A39" s="6">
         <v>45312</v>
       </c>
@@ -2090,7 +2121,7 @@
       </c>
       <c r="I39" s="1">
         <f t="shared" si="3"/>
-        <v>-960000</v>
+        <v>960000</v>
       </c>
       <c r="J39" s="1">
         <v>960000</v>
@@ -2105,7 +2136,7 @@
       </c>
       <c r="N39" s="1"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16">
       <c r="C40" t="s">
         <v>47</v>
       </c>
@@ -2120,7 +2151,7 @@
       </c>
       <c r="I40" s="1">
         <f t="shared" si="3"/>
-        <v>-325000</v>
+        <v>325000</v>
       </c>
       <c r="J40" s="1">
         <v>325000</v>
@@ -2135,7 +2166,7 @@
       </c>
       <c r="N40" s="1"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16">
       <c r="C41" t="s">
         <v>46</v>
       </c>
@@ -2150,7 +2181,7 @@
       </c>
       <c r="I41" s="1">
         <f t="shared" si="3"/>
-        <v>-667000</v>
+        <v>667000</v>
       </c>
       <c r="J41" s="1">
         <v>667000</v>
@@ -2165,7 +2196,7 @@
       </c>
       <c r="N41" s="1"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16">
       <c r="C42" t="s">
         <v>48</v>
       </c>
@@ -2180,7 +2211,7 @@
       </c>
       <c r="I42" s="1">
         <f t="shared" si="3"/>
-        <v>-22000</v>
+        <v>22000</v>
       </c>
       <c r="J42" s="1">
         <v>22000</v>
@@ -2195,7 +2226,7 @@
       </c>
       <c r="N42" s="1"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16">
       <c r="C43" t="s">
         <v>45</v>
       </c>
@@ -2210,7 +2241,7 @@
       </c>
       <c r="I43" s="1">
         <f t="shared" si="3"/>
-        <v>-721000</v>
+        <v>721000</v>
       </c>
       <c r="J43" s="1">
         <v>721000</v>
@@ -2225,7 +2256,7 @@
       </c>
       <c r="N43" s="1"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16">
       <c r="C44" t="s">
         <v>44</v>
       </c>
@@ -2240,7 +2271,7 @@
       </c>
       <c r="I44" s="1">
         <f t="shared" si="3"/>
-        <v>-471000</v>
+        <v>471000</v>
       </c>
       <c r="J44" s="1">
         <v>471000</v>
@@ -2255,7 +2286,7 @@
       </c>
       <c r="N44" s="1"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16">
       <c r="C45" t="s">
         <v>39</v>
       </c>
@@ -2270,7 +2301,7 @@
       </c>
       <c r="I45" s="1">
         <f t="shared" si="3"/>
-        <v>-256000</v>
+        <v>256000</v>
       </c>
       <c r="J45" s="1">
         <v>256000</v>
@@ -2285,7 +2316,7 @@
       </c>
       <c r="N45" s="1"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16">
       <c r="C46" t="s">
         <v>49</v>
       </c>
@@ -2300,7 +2331,7 @@
       </c>
       <c r="I46" s="1">
         <f t="shared" si="3"/>
-        <v>-554000</v>
+        <v>554000</v>
       </c>
       <c r="J46" s="1">
         <v>554000</v>
@@ -2315,7 +2346,7 @@
       </c>
       <c r="N46" s="1"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16">
       <c r="B47" t="s">
         <v>15</v>
       </c>
@@ -2332,8 +2363,8 @@
         <v>14580000</v>
       </c>
       <c r="I47" s="1">
-        <f>F47-G47</f>
-        <v>-19842000</v>
+        <f t="shared" si="3"/>
+        <v>19842000</v>
       </c>
       <c r="J47" s="1">
         <f>4042000+14580000</f>
@@ -2354,7 +2385,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16">
       <c r="A48" s="6">
         <v>45316</v>
       </c>
@@ -2375,7 +2406,7 @@
       </c>
       <c r="I48" s="1">
         <f t="shared" si="3"/>
-        <v>-72000</v>
+        <v>72000</v>
       </c>
       <c r="J48" s="1">
         <v>72000</v>
@@ -2390,7 +2421,7 @@
       </c>
       <c r="N48" s="1"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16">
       <c r="C49" t="s">
         <v>51</v>
       </c>
@@ -2405,7 +2436,7 @@
       </c>
       <c r="I49" s="1">
         <f t="shared" si="3"/>
-        <v>-2748000</v>
+        <v>2748000</v>
       </c>
       <c r="J49" s="1">
         <v>2748000</v>
@@ -2420,7 +2451,7 @@
       </c>
       <c r="N49" s="1"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16">
       <c r="C50" t="s">
         <v>52</v>
       </c>
@@ -2435,7 +2466,7 @@
       </c>
       <c r="I50" s="1">
         <f t="shared" si="3"/>
-        <v>-66000</v>
+        <v>66000</v>
       </c>
       <c r="J50" s="1">
         <v>66000</v>
@@ -2450,7 +2481,7 @@
       </c>
       <c r="N50" s="1"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16">
       <c r="C51" t="s">
         <v>54</v>
       </c>
@@ -2465,7 +2496,7 @@
       </c>
       <c r="I51" s="1">
         <f t="shared" si="3"/>
-        <v>-1319000</v>
+        <v>1319000</v>
       </c>
       <c r="J51" s="1">
         <v>1319000</v>
@@ -2480,7 +2511,7 @@
       </c>
       <c r="N51" s="1"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16">
       <c r="C52" t="s">
         <v>55</v>
       </c>
@@ -2492,7 +2523,7 @@
       </c>
       <c r="I52" s="1">
         <f t="shared" si="3"/>
-        <v>-506000</v>
+        <v>506000</v>
       </c>
       <c r="J52" s="1">
         <v>506000</v>
@@ -2507,7 +2538,7 @@
       </c>
       <c r="N52" s="1"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16">
       <c r="C53" t="s">
         <v>38</v>
       </c>
@@ -2516,7 +2547,7 @@
       </c>
       <c r="I53" s="1">
         <f t="shared" si="3"/>
-        <v>-1589000</v>
+        <v>1589000</v>
       </c>
       <c r="J53" s="1">
         <v>1589000</v>
@@ -2531,7 +2562,7 @@
       </c>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16">
       <c r="C54" t="s">
         <v>19</v>
       </c>
@@ -2540,7 +2571,7 @@
       </c>
       <c r="I54" s="1">
         <f t="shared" si="3"/>
-        <v>-624000</v>
+        <v>624000</v>
       </c>
       <c r="J54" s="1">
         <v>624000</v>
@@ -2555,7 +2586,7 @@
       </c>
       <c r="N54" s="1"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16">
       <c r="C55" t="s">
         <v>18</v>
       </c>
@@ -2564,7 +2595,7 @@
       </c>
       <c r="I55" s="1">
         <f t="shared" si="3"/>
-        <v>-618000</v>
+        <v>618000</v>
       </c>
       <c r="J55" s="1">
         <v>618000</v>
@@ -2579,7 +2610,7 @@
       </c>
       <c r="N55" s="1"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16">
       <c r="A56" s="6">
         <v>45318</v>
       </c>
@@ -2600,7 +2631,7 @@
       </c>
       <c r="I56" s="1">
         <f t="shared" si="3"/>
-        <v>-39879000</v>
+        <v>39879000</v>
       </c>
       <c r="J56" s="1">
         <f>39879000+2632000</f>
@@ -2619,7 +2650,7 @@
       </c>
       <c r="N56" s="1"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16">
       <c r="B57" t="s">
         <v>34</v>
       </c>
@@ -2646,7 +2677,7 @@
       </c>
       <c r="N57" s="1"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16">
       <c r="C58" t="s">
         <v>37</v>
       </c>
@@ -2670,7 +2701,7 @@
       </c>
       <c r="N58" s="1"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16">
       <c r="A59" s="6">
         <v>45319</v>
       </c>
@@ -2691,7 +2722,7 @@
       </c>
       <c r="I59" s="1">
         <f t="shared" si="3"/>
-        <v>-163000</v>
+        <v>163000</v>
       </c>
       <c r="J59" s="1">
         <v>163000</v>
@@ -2706,7 +2737,7 @@
       </c>
       <c r="N59" s="1"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16">
       <c r="C60" t="s">
         <v>49</v>
       </c>
@@ -2721,7 +2752,7 @@
       </c>
       <c r="I60" s="1">
         <f t="shared" si="3"/>
-        <v>-416000</v>
+        <v>416000</v>
       </c>
       <c r="J60" s="1">
         <v>416000</v>
@@ -2737,7 +2768,7 @@
       <c r="N60" s="1"/>
       <c r="P60" s="1"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16">
       <c r="A61" s="6">
         <v>45327</v>
       </c>
@@ -2758,7 +2789,7 @@
       </c>
       <c r="I61" s="1">
         <f t="shared" si="3"/>
-        <v>-16540000</v>
+        <v>16540000</v>
       </c>
       <c r="J61" s="1">
         <v>16540000</v>
@@ -2775,15 +2806,15 @@
         <v>100000</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16">
       <c r="A62" s="6">
         <v>45332</v>
       </c>
       <c r="B62" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D62" s="6">
         <v>45318</v>
@@ -2796,7 +2827,7 @@
       </c>
       <c r="I62" s="1">
         <f t="shared" si="3"/>
-        <v>-28447000</v>
+        <v>28447000</v>
       </c>
       <c r="J62" s="1">
         <v>27519000</v>
@@ -2813,15 +2844,15 @@
         <v>150000</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16">
       <c r="A63" s="6">
         <v>45339</v>
       </c>
       <c r="B63" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D63" s="6">
         <v>45298</v>
@@ -2834,7 +2865,7 @@
       </c>
       <c r="I63" s="1">
         <f t="shared" si="3"/>
-        <v>-864000</v>
+        <v>864000</v>
       </c>
       <c r="J63" s="1">
         <v>864000</v>
@@ -2849,7 +2880,7 @@
       </c>
       <c r="N63" s="1"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16">
       <c r="B64" t="s">
         <v>29</v>
       </c>
@@ -2862,12 +2893,15 @@
       <c r="E64" s="8">
         <v>45333</v>
       </c>
+      <c r="F64" s="1">
+        <v>484000</v>
+      </c>
       <c r="G64" s="1">
         <v>484000</v>
       </c>
       <c r="I64" s="1">
         <f t="shared" si="3"/>
-        <v>-484000</v>
+        <v>0</v>
       </c>
       <c r="J64" s="1">
         <v>484000</v>
@@ -2882,12 +2916,12 @@
       </c>
       <c r="N64" s="1"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16">
       <c r="A65" s="6">
         <v>45341</v>
       </c>
       <c r="B65" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D65" s="6">
         <v>45321</v>
@@ -2900,7 +2934,7 @@
       </c>
       <c r="I65" s="1">
         <f t="shared" si="3"/>
-        <v>-6146000</v>
+        <v>6146000</v>
       </c>
       <c r="J65" s="1">
         <v>5000000</v>
@@ -2914,10 +2948,10 @@
         <v>1146000</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16">
       <c r="A66" s="6">
         <v>45347</v>
       </c>
@@ -2937,8 +2971,8 @@
         <v>15800000</v>
       </c>
       <c r="I66" s="1">
-        <f t="shared" ref="I66:I101" si="6">F66-G66</f>
-        <v>-21096000</v>
+        <f t="shared" ref="I66:I97" si="6">G66-F66</f>
+        <v>21096000</v>
       </c>
       <c r="J66" s="1">
         <v>21096000</v>
@@ -2955,12 +2989,12 @@
         <v>200000</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16">
       <c r="B67" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D67" s="6">
         <v>45331</v>
@@ -2976,7 +3010,7 @@
       </c>
       <c r="I67" s="1">
         <f t="shared" si="6"/>
-        <v>-6925000</v>
+        <v>6925000</v>
       </c>
       <c r="J67" s="1">
         <f>6925000+928000</f>
@@ -2996,7 +3030,7 @@
       <c r="N67" s="1"/>
       <c r="P67" s="1"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16">
       <c r="A68" s="6">
         <v>45352</v>
       </c>
@@ -3004,7 +3038,7 @@
         <v>29</v>
       </c>
       <c r="C68" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D68" s="6">
         <v>45316</v>
@@ -3017,7 +3051,7 @@
       </c>
       <c r="I68" s="1">
         <f t="shared" si="6"/>
-        <v>-958000</v>
+        <v>958000</v>
       </c>
       <c r="J68" s="1">
         <v>908000</v>
@@ -3031,15 +3065,15 @@
         <v>50000</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16">
       <c r="B69" t="s">
         <v>34</v>
       </c>
       <c r="C69" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D69" s="6">
         <v>45315</v>
@@ -3052,7 +3086,7 @@
       </c>
       <c r="I69" s="1">
         <f t="shared" si="6"/>
-        <v>-1516000</v>
+        <v>1516000</v>
       </c>
       <c r="J69" s="1">
         <v>1516000</v>
@@ -3067,9 +3101,9 @@
       </c>
       <c r="N69" s="1"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16">
       <c r="C70" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D70" s="6">
         <v>45315</v>
@@ -3082,7 +3116,7 @@
       </c>
       <c r="I70" s="1">
         <f t="shared" si="6"/>
-        <v>-492000</v>
+        <v>492000</v>
       </c>
       <c r="J70" s="1">
         <v>492000</v>
@@ -3097,9 +3131,9 @@
       </c>
       <c r="N70" s="1"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16">
       <c r="C71" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D71" s="6">
         <v>45315</v>
@@ -3112,7 +3146,7 @@
       </c>
       <c r="I71" s="1">
         <f t="shared" si="6"/>
-        <v>-1267000</v>
+        <v>1267000</v>
       </c>
       <c r="J71" s="1">
         <v>1267000</v>
@@ -3127,9 +3161,9 @@
       </c>
       <c r="N71" s="1"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16">
       <c r="C72" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D72" s="6">
         <v>45324</v>
@@ -3142,7 +3176,7 @@
       </c>
       <c r="I72" s="1">
         <f t="shared" si="6"/>
-        <v>-1016000</v>
+        <v>1016000</v>
       </c>
       <c r="J72" s="1">
         <v>1016000</v>
@@ -3157,7 +3191,7 @@
       </c>
       <c r="N72" s="1"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16">
       <c r="A73" s="6">
         <v>45354</v>
       </c>
@@ -3165,7 +3199,7 @@
         <v>29</v>
       </c>
       <c r="C73" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D73" s="6">
         <v>45316</v>
@@ -3178,7 +3212,7 @@
       </c>
       <c r="I73" s="1">
         <f t="shared" si="6"/>
-        <v>-847000</v>
+        <v>847000</v>
       </c>
       <c r="J73" s="1">
         <v>812000</v>
@@ -3192,10 +3226,10 @@
         <v>35000</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16">
       <c r="A74" s="6">
         <v>45358</v>
       </c>
@@ -3203,7 +3237,7 @@
         <v>34</v>
       </c>
       <c r="C74" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="D74" s="6">
         <v>45200</v>
@@ -3216,7 +3250,7 @@
       </c>
       <c r="I74" s="1">
         <f t="shared" si="6"/>
-        <v>-4019000</v>
+        <v>4019000</v>
       </c>
       <c r="J74" s="1">
         <v>4019000</v>
@@ -3234,12 +3268,12 @@
       </c>
       <c r="N74" s="1"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16">
       <c r="A75" s="6">
         <v>45361</v>
       </c>
       <c r="B75" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D75" s="6">
         <v>45345</v>
@@ -3252,7 +3286,7 @@
       </c>
       <c r="I75" s="1">
         <f t="shared" si="6"/>
-        <v>-6027000</v>
+        <v>6027000</v>
       </c>
       <c r="J75" s="1">
         <v>6027000</v>
@@ -3267,7 +3301,7 @@
       </c>
       <c r="N75" s="1"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16">
       <c r="A76" s="6">
         <v>45362</v>
       </c>
@@ -3288,7 +3322,7 @@
       </c>
       <c r="I76" s="1">
         <f t="shared" si="6"/>
-        <v>-20242000</v>
+        <v>20242000</v>
       </c>
       <c r="J76" s="1">
         <v>16426000</v>
@@ -3305,10 +3339,10 @@
         <v>200000</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16">
       <c r="A77" s="6">
         <v>45366</v>
       </c>
@@ -3316,7 +3350,7 @@
         <v>29</v>
       </c>
       <c r="C77" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D77" s="6">
         <v>45359</v>
@@ -3329,7 +3363,7 @@
       </c>
       <c r="I77" s="1">
         <f t="shared" si="6"/>
-        <v>-316000</v>
+        <v>316000</v>
       </c>
       <c r="J77" s="1">
         <v>316000</v>
@@ -3344,9 +3378,9 @@
       </c>
       <c r="N77" s="1"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16">
       <c r="C78" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D78" s="6">
         <v>45331</v>
@@ -3354,12 +3388,15 @@
       <c r="E78" s="8">
         <v>45336</v>
       </c>
+      <c r="F78" s="1">
+        <v>166000</v>
+      </c>
       <c r="G78" s="1">
         <v>166000</v>
       </c>
       <c r="I78" s="1">
         <f t="shared" si="6"/>
-        <v>-166000</v>
+        <v>0</v>
       </c>
       <c r="J78" s="1">
         <v>166000</v>
@@ -3375,12 +3412,12 @@
       <c r="N78" s="1"/>
       <c r="P78" s="1"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16">
       <c r="A79" s="6">
         <v>45368</v>
       </c>
       <c r="B79" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D79" s="6">
         <v>45338</v>
@@ -3396,7 +3433,7 @@
       </c>
       <c r="I79" s="1">
         <f t="shared" si="6"/>
-        <v>-13131000</v>
+        <v>13131000</v>
       </c>
       <c r="J79" s="1">
         <f>13131000+1146000</f>
@@ -3415,7 +3452,7 @@
       </c>
       <c r="N79" s="1"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16">
       <c r="A80" s="6">
         <v>45374</v>
       </c>
@@ -3423,7 +3460,7 @@
         <v>25</v>
       </c>
       <c r="C80" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D80" s="6">
         <v>45328</v>
@@ -3454,7 +3491,7 @@
       </c>
       <c r="N80" s="1"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16">
       <c r="C81" t="s">
         <v>27</v>
       </c>
@@ -3487,9 +3524,9 @@
       </c>
       <c r="N81" s="1"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16">
       <c r="C82" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D82" s="6">
         <v>45331</v>
@@ -3520,9 +3557,9 @@
       </c>
       <c r="N82" s="1"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16">
       <c r="B83" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D83" s="6">
         <v>45359</v>
@@ -3556,12 +3593,12 @@
       </c>
       <c r="N83" s="1"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16">
       <c r="B84" t="s">
         <v>34</v>
       </c>
       <c r="C84" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="D84" s="6">
         <v>45307</v>
@@ -3591,15 +3628,15 @@
         <v>686000</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16">
       <c r="A85" s="6">
         <v>45376</v>
       </c>
       <c r="B85" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="D85" s="6">
         <v>45328</v>
@@ -3630,9 +3667,9 @@
       </c>
       <c r="N85" s="1"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16">
       <c r="B86" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D86" s="6">
         <v>45323</v>
@@ -3665,10 +3702,10 @@
         <v>100000</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16">
       <c r="A87" s="6">
         <v>45380</v>
       </c>
@@ -3707,12 +3744,12 @@
       </c>
       <c r="N87" s="1"/>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16">
       <c r="B88" t="s">
         <v>29</v>
       </c>
       <c r="C88" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D88" s="6">
         <v>45367</v>
@@ -3743,9 +3780,9 @@
       </c>
       <c r="N88" s="1"/>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16">
       <c r="C89" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D89" s="6">
         <v>45352</v>
@@ -3782,7 +3819,7 @@
       </c>
       <c r="P89" s="1"/>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16">
       <c r="A90" s="6">
         <v>45383</v>
       </c>
@@ -3790,7 +3827,7 @@
         <v>25</v>
       </c>
       <c r="C90" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="D90" s="6">
         <v>45352</v>
@@ -3821,12 +3858,12 @@
       </c>
       <c r="N90" s="1"/>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16">
       <c r="B91" t="s">
         <v>34</v>
       </c>
       <c r="C91" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D91" s="6">
         <v>45351</v>
@@ -3857,9 +3894,9 @@
       </c>
       <c r="N91" s="1"/>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16">
       <c r="C92" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D92" s="6">
         <v>45351</v>
@@ -3890,9 +3927,9 @@
       </c>
       <c r="N92" s="1"/>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16">
       <c r="C93" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D93" s="6">
         <v>45351</v>
@@ -3923,7 +3960,7 @@
       </c>
       <c r="N93" s="1"/>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16">
       <c r="B94" t="s">
         <v>25</v>
       </c>
@@ -3941,7 +3978,7 @@
       </c>
       <c r="I94" s="1">
         <f t="shared" si="6"/>
-        <v>-562000</v>
+        <v>562000</v>
       </c>
       <c r="J94" s="1">
         <v>469000</v>
@@ -3955,10 +3992,10 @@
         <v>93000</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16">
       <c r="C95" t="s">
         <v>28</v>
       </c>
@@ -3968,12 +4005,15 @@
       <c r="E95" s="8">
         <v>45310</v>
       </c>
+      <c r="F95" s="1">
+        <v>1056000</v>
+      </c>
       <c r="G95" s="1">
         <v>1056000</v>
       </c>
       <c r="I95" s="1">
         <f t="shared" si="6"/>
-        <v>-1056000</v>
+        <v>0</v>
       </c>
       <c r="J95" s="1">
         <v>805000</v>
@@ -3987,11 +4027,11 @@
         <v>251000</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="P95" s="1"/>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16">
       <c r="A96" s="6">
         <v>45385</v>
       </c>
@@ -4032,15 +4072,15 @@
         <v>582000</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="97" spans="1:14">
       <c r="A97" s="6">
         <v>45386</v>
       </c>
       <c r="B97" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D97" s="6">
         <v>45352</v>
@@ -4070,10 +4110,10 @@
         <v>7678000</v>
       </c>
       <c r="N97" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="98" spans="1:14">
       <c r="B98" t="s">
         <v>15</v>
       </c>
@@ -4093,14 +4133,14 @@
         <v>19616000</v>
       </c>
       <c r="I98" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="I98:I122" si="9">G98-F98</f>
         <v>0</v>
       </c>
       <c r="J98" s="1">
         <v>30230000</v>
       </c>
       <c r="K98" s="1">
-        <f t="shared" ref="K98:K101" si="9">G98-J98</f>
+        <f t="shared" ref="K98:K101" si="10">G98-J98</f>
         <v>5076000</v>
       </c>
       <c r="L98" s="1">
@@ -4111,15 +4151,15 @@
         <v>150000</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="99" spans="1:14">
       <c r="A99" s="6">
         <v>45387</v>
       </c>
       <c r="B99" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D99" s="6">
         <v>45373</v>
@@ -4134,14 +4174,14 @@
         <v>3718000</v>
       </c>
       <c r="I99" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J99" s="1">
         <v>3657000</v>
       </c>
       <c r="K99" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>61000</v>
       </c>
       <c r="L99" s="1">
@@ -4152,15 +4192,15 @@
         <v>100000</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="100" spans="1:14">
       <c r="B100" t="s">
         <v>29</v>
       </c>
       <c r="C100" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="D100" s="6">
         <v>45381</v>
@@ -4175,14 +4215,14 @@
         <v>225000</v>
       </c>
       <c r="I100" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J100" s="1">
         <v>225000</v>
       </c>
       <c r="K100" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="L100" s="1">
@@ -4190,9 +4230,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14">
       <c r="B101" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D101" s="6">
         <v>45376</v>
@@ -4210,14 +4250,14 @@
         <v>5729000</v>
       </c>
       <c r="I101" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J101" s="1">
         <v>10000000</v>
       </c>
       <c r="K101" s="1">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-4416000</v>
       </c>
       <c r="L101" s="1">
@@ -4225,23 +4265,23 @@
         <v>1313000</v>
       </c>
       <c r="N101" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A102" s="9">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="102" spans="1:14">
+      <c r="A102" s="6">
         <v>45408</v>
       </c>
       <c r="B102" t="s">
         <v>25</v>
       </c>
       <c r="C102" t="s">
-        <v>78</v>
-      </c>
-      <c r="D102" s="9">
+        <v>87</v>
+      </c>
+      <c r="D102" s="6">
         <v>45378</v>
       </c>
-      <c r="E102" s="10">
+      <c r="E102" s="8">
         <v>45406</v>
       </c>
       <c r="F102" s="1">
@@ -4254,7 +4294,7 @@
         <v>0</v>
       </c>
       <c r="I102" s="1">
-        <f>F102-G102</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J102" s="1">
@@ -4269,20 +4309,20 @@
         <v>141000</v>
       </c>
       <c r="N102" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A103" s="9">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="103" spans="1:14">
+      <c r="A103" s="6">
         <v>45409</v>
       </c>
       <c r="B103" t="s">
-        <v>59</v>
-      </c>
-      <c r="D103" s="9">
+        <v>60</v>
+      </c>
+      <c r="D103" s="6">
         <v>45384</v>
       </c>
-      <c r="E103" s="10">
+      <c r="E103" s="8">
         <v>45384</v>
       </c>
       <c r="F103" s="1">
@@ -4295,7 +4335,7 @@
         <v>7678000</v>
       </c>
       <c r="I103" s="1">
-        <f>F103-G103</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J103" s="1">
@@ -4310,17 +4350,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A104" s="9">
+    <row r="104" spans="1:14">
+      <c r="A104" s="6">
         <v>45410</v>
       </c>
       <c r="B104" t="s">
         <v>27</v>
       </c>
-      <c r="D104" s="9">
+      <c r="D104" s="6">
         <v>45401</v>
       </c>
-      <c r="E104" s="10">
+      <c r="E104" s="8">
         <v>45409</v>
       </c>
       <c r="F104" s="1">
@@ -4330,7 +4370,7 @@
         <v>6440000</v>
       </c>
       <c r="I104" s="1">
-        <f>F104-G104</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J104" s="1">
@@ -4345,17 +4385,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A105" s="9">
+    <row r="105" spans="1:14">
+      <c r="A105" s="6">
         <v>45412</v>
       </c>
       <c r="B105" t="s">
-        <v>79</v>
-      </c>
-      <c r="D105" s="9">
+        <v>88</v>
+      </c>
+      <c r="D105" s="6">
         <v>45403</v>
       </c>
-      <c r="E105" s="10">
+      <c r="E105" s="8">
         <v>45411</v>
       </c>
       <c r="F105" s="1">
@@ -4365,7 +4405,7 @@
         <v>3641000</v>
       </c>
       <c r="I105" s="1">
-        <f>F105-G105</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J105" s="1">
@@ -4380,48 +4420,711 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A106" s="9">
-        <v>45414</v>
+    <row r="106" spans="1:14">
+      <c r="A106" s="6">
+        <v>45413</v>
       </c>
       <c r="B106" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C106" t="s">
-        <v>61</v>
-      </c>
-      <c r="D106" s="9">
-        <v>45380</v>
-      </c>
-      <c r="E106" s="10">
+        <v>65</v>
+      </c>
+      <c r="D106" s="6">
+        <v>45383</v>
+      </c>
+      <c r="E106" s="8">
         <v>45411</v>
       </c>
       <c r="F106" s="1">
-        <v>790000</v>
+        <v>829000</v>
       </c>
       <c r="G106" s="1">
-        <v>790000</v>
-      </c>
-      <c r="H106" s="1">
-        <v>11000</v>
+        <v>829000</v>
       </c>
       <c r="I106" s="1">
-        <f>F106-G106</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="J106" s="1">
-        <v>700000</v>
+        <v>829000</v>
       </c>
       <c r="K106" s="1">
         <f>G106-J106</f>
-        <v>90000</v>
+        <v>0</v>
       </c>
       <c r="L106" s="1">
         <f>G106-J106+H106</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:14">
+      <c r="C107" t="s">
+        <v>67</v>
+      </c>
+      <c r="D107" s="6">
+        <v>45383</v>
+      </c>
+      <c r="E107" s="8">
+        <v>45411</v>
+      </c>
+      <c r="F107" s="1">
+        <v>739000</v>
+      </c>
+      <c r="G107" s="1">
+        <v>739000</v>
+      </c>
+      <c r="I107" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J107" s="1">
+        <v>739000</v>
+      </c>
+      <c r="K107" s="1">
+        <f>G107-J107</f>
+        <v>0</v>
+      </c>
+      <c r="L107" s="1">
+        <f>G107-J107+H107</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14">
+      <c r="C108" t="s">
+        <v>68</v>
+      </c>
+      <c r="D108" s="6">
+        <v>45383</v>
+      </c>
+      <c r="E108" s="8">
+        <v>45411</v>
+      </c>
+      <c r="F108" s="1">
+        <v>641000</v>
+      </c>
+      <c r="G108" s="1">
+        <v>641000</v>
+      </c>
+      <c r="I108" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J108" s="1">
+        <v>641000</v>
+      </c>
+      <c r="K108" s="1">
+        <f>G108-J108</f>
+        <v>0</v>
+      </c>
+      <c r="L108" s="1">
+        <f>G108-J108+H108</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14">
+      <c r="A109" s="6">
+        <v>45414</v>
+      </c>
+      <c r="B109" t="s">
+        <v>29</v>
+      </c>
+      <c r="C109" t="s">
+        <v>63</v>
+      </c>
+      <c r="D109" s="6">
+        <v>45380</v>
+      </c>
+      <c r="E109" s="8">
+        <v>45411</v>
+      </c>
+      <c r="F109" s="1">
+        <v>790000</v>
+      </c>
+      <c r="G109" s="1">
+        <v>790000</v>
+      </c>
+      <c r="H109" s="1">
+        <v>11000</v>
+      </c>
+      <c r="I109" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J109" s="1">
+        <v>700000</v>
+      </c>
+      <c r="K109" s="1">
+        <f>G109-J109</f>
+        <v>90000</v>
+      </c>
+      <c r="L109" s="1">
+        <f>G109-J109+H109</f>
         <v>101000</v>
       </c>
-      <c r="N106" t="s">
-        <v>50</v>
+      <c r="N109" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14">
+      <c r="A110" s="6">
+        <v>45416</v>
+      </c>
+      <c r="B110" t="s">
+        <v>15</v>
+      </c>
+      <c r="D110" s="6">
+        <v>45385</v>
+      </c>
+      <c r="E110" s="8">
+        <v>45412</v>
+      </c>
+      <c r="F110" s="1">
+        <v>28729000</v>
+      </c>
+      <c r="G110" s="1">
+        <v>28729000</v>
+      </c>
+      <c r="H110" s="1">
+        <v>24692000</v>
+      </c>
+      <c r="I110" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J110" s="1">
+        <v>24000000</v>
+      </c>
+      <c r="K110" s="1">
+        <f>G110-J110</f>
+        <v>4729000</v>
+      </c>
+      <c r="L110" s="1">
+        <f>G110-J110+H110</f>
+        <v>29421000</v>
+      </c>
+      <c r="M110" s="1">
+        <v>200000</v>
+      </c>
+      <c r="N110" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14">
+      <c r="B111" t="s">
+        <v>57</v>
+      </c>
+      <c r="D111" s="6">
+        <v>45387</v>
+      </c>
+      <c r="E111" s="8">
+        <v>45414</v>
+      </c>
+      <c r="F111" s="1">
+        <v>10042000</v>
+      </c>
+      <c r="G111" s="1">
+        <v>10042000</v>
+      </c>
+      <c r="H111" s="1">
+        <v>61000</v>
+      </c>
+      <c r="I111" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J111" s="1">
+        <v>10103000</v>
+      </c>
+      <c r="K111" s="1">
+        <f>G111-J111</f>
+        <v>-61000</v>
+      </c>
+      <c r="L111" s="1">
+        <f>G111-J111+H111</f>
+        <v>0</v>
+      </c>
+      <c r="M111" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14">
+      <c r="A112" s="6">
+        <v>45417</v>
+      </c>
+      <c r="B112" t="s">
+        <v>25</v>
+      </c>
+      <c r="C112" t="s">
+        <v>27</v>
+      </c>
+      <c r="D112" s="6">
+        <v>45381</v>
+      </c>
+      <c r="E112" s="8">
+        <v>45411</v>
+      </c>
+      <c r="F112" s="1">
+        <v>436000</v>
+      </c>
+      <c r="G112" s="1">
+        <v>436000</v>
+      </c>
+      <c r="I112" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J112" s="1">
+        <v>436000</v>
+      </c>
+      <c r="K112" s="1">
+        <f>G112-J112</f>
+        <v>0</v>
+      </c>
+      <c r="L112" s="1">
+        <f>G112-J112+H112</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:14">
+      <c r="A113" s="6">
+        <v>45420</v>
+      </c>
+      <c r="B113" t="s">
+        <v>90</v>
+      </c>
+      <c r="D113" s="6">
+        <v>45399</v>
+      </c>
+      <c r="E113" s="8">
+        <v>45407</v>
+      </c>
+      <c r="F113" s="1">
+        <v>5355000</v>
+      </c>
+      <c r="G113" s="1">
+        <v>5355000</v>
+      </c>
+      <c r="I113" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J113" s="1">
+        <v>5355000</v>
+      </c>
+      <c r="K113" s="1">
+        <f>G113-J113</f>
+        <v>0</v>
+      </c>
+      <c r="L113" s="1">
+        <f>G113-J113+H113</f>
+        <v>0</v>
+      </c>
+      <c r="M113" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14">
+      <c r="A114" s="6">
+        <v>45424</v>
+      </c>
+      <c r="B114" t="s">
+        <v>91</v>
+      </c>
+      <c r="D114" s="6">
+        <v>45404</v>
+      </c>
+      <c r="E114" s="8">
+        <v>45418</v>
+      </c>
+      <c r="F114" s="1">
+        <v>4243000</v>
+      </c>
+      <c r="G114" s="1">
+        <v>4243000</v>
+      </c>
+      <c r="I114" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J114" s="1">
+        <v>4243000</v>
+      </c>
+      <c r="K114" s="1">
+        <f>G114-J114</f>
+        <v>0</v>
+      </c>
+      <c r="L114" s="1">
+        <f>G114-J114+H114</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:14">
+      <c r="A115" s="6">
+        <v>45427</v>
+      </c>
+      <c r="B115" t="s">
+        <v>88</v>
+      </c>
+      <c r="D115" s="6">
+        <v>45412</v>
+      </c>
+      <c r="E115" s="8">
+        <v>45422</v>
+      </c>
+      <c r="F115" s="1">
+        <v>4482000</v>
+      </c>
+      <c r="G115" s="1">
+        <v>4482000</v>
+      </c>
+      <c r="I115" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J115" s="1">
+        <v>4482000</v>
+      </c>
+      <c r="K115" s="1">
+        <f>G115-J115</f>
+        <v>0</v>
+      </c>
+      <c r="L115" s="1">
+        <f>G115-J115+H115</f>
+        <v>0</v>
+      </c>
+      <c r="M115" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14">
+      <c r="B116" t="s">
+        <v>79</v>
+      </c>
+      <c r="D116" s="6">
+        <v>45387</v>
+      </c>
+      <c r="E116" s="8">
+        <v>45423</v>
+      </c>
+      <c r="F116" s="1">
+        <v>11539000</v>
+      </c>
+      <c r="G116" s="1">
+        <v>11539000</v>
+      </c>
+      <c r="H116" s="1">
+        <v>1313000</v>
+      </c>
+      <c r="I116" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J116" s="1">
+        <v>7852000</v>
+      </c>
+      <c r="K116" s="1">
+        <f>G116-J116</f>
+        <v>3687000</v>
+      </c>
+      <c r="L116" s="1">
+        <f>G116-J116+H116</f>
+        <v>5000000</v>
+      </c>
+      <c r="M116" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="117" spans="1:14">
+      <c r="A117" s="6">
+        <v>45430</v>
+      </c>
+      <c r="B117" t="s">
+        <v>57</v>
+      </c>
+      <c r="D117" s="6">
+        <v>45415</v>
+      </c>
+      <c r="E117" s="8">
+        <v>45428</v>
+      </c>
+      <c r="F117" s="1">
+        <v>6951000</v>
+      </c>
+      <c r="G117" s="1">
+        <v>6951000</v>
+      </c>
+      <c r="I117" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J117" s="1">
+        <v>6951000</v>
+      </c>
+      <c r="K117" s="1">
+        <f>G117-J117</f>
+        <v>0</v>
+      </c>
+      <c r="L117" s="1">
+        <f>G117-J117+H117</f>
+        <v>0</v>
+      </c>
+      <c r="M117" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14">
+      <c r="B118" t="s">
+        <v>92</v>
+      </c>
+      <c r="D118" s="6">
+        <v>45412</v>
+      </c>
+      <c r="E118" s="8">
+        <v>45421</v>
+      </c>
+      <c r="F118" s="1">
+        <v>9523000</v>
+      </c>
+      <c r="G118" s="1">
+        <v>9523000</v>
+      </c>
+      <c r="I118" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J118" s="1">
+        <v>6000000</v>
+      </c>
+      <c r="K118" s="1">
+        <f>G118-J118</f>
+        <v>3523000</v>
+      </c>
+      <c r="L118" s="1">
+        <f>G118-J118+H118</f>
+        <v>3523000</v>
+      </c>
+      <c r="N118" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="119" spans="1:14">
+      <c r="B119" t="s">
+        <v>15</v>
+      </c>
+      <c r="D119" s="6">
+        <v>45413</v>
+      </c>
+      <c r="E119" s="8">
+        <v>45428</v>
+      </c>
+      <c r="F119" s="1">
+        <v>26820000</v>
+      </c>
+      <c r="G119" s="1">
+        <v>26820000</v>
+      </c>
+      <c r="H119" s="1">
+        <v>29421000</v>
+      </c>
+      <c r="I119" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J119" s="1">
+        <v>21000000</v>
+      </c>
+      <c r="K119" s="1">
+        <f>G119-J119</f>
+        <v>5820000</v>
+      </c>
+      <c r="L119" s="1">
+        <f>G119-J119+H119</f>
+        <v>35241000</v>
+      </c>
+      <c r="M119" s="1">
+        <v>100000</v>
+      </c>
+      <c r="N119" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="120" spans="1:14">
+      <c r="A120" s="6">
+        <v>45434</v>
+      </c>
+      <c r="B120" t="s">
+        <v>91</v>
+      </c>
+      <c r="D120" s="6">
+        <v>45419</v>
+      </c>
+      <c r="E120" s="8">
+        <v>45430</v>
+      </c>
+      <c r="F120" s="1">
+        <v>4529000</v>
+      </c>
+      <c r="G120" s="1">
+        <v>4529000</v>
+      </c>
+      <c r="I120" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J120" s="1">
+        <v>4529000</v>
+      </c>
+      <c r="K120" s="1">
+        <f>G120-J120</f>
+        <v>0</v>
+      </c>
+      <c r="L120" s="1">
+        <f>G120-J120+H120</f>
+        <v>0</v>
+      </c>
+      <c r="M120" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14">
+      <c r="B121" t="s">
+        <v>90</v>
+      </c>
+      <c r="D121" s="6">
+        <v>45408</v>
+      </c>
+      <c r="E121" s="8">
+        <v>45422</v>
+      </c>
+      <c r="F121" s="1">
+        <v>6107000</v>
+      </c>
+      <c r="G121" s="1">
+        <v>6107000</v>
+      </c>
+      <c r="I121" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J121" s="1">
+        <v>6107000</v>
+      </c>
+      <c r="K121" s="1">
+        <f>G121-J121</f>
+        <v>0</v>
+      </c>
+      <c r="L121" s="1">
+        <f>G121-J121+H121</f>
+        <v>0</v>
+      </c>
+      <c r="M121" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14">
+      <c r="B122" t="s">
+        <v>27</v>
+      </c>
+      <c r="D122" s="6">
+        <v>45410</v>
+      </c>
+      <c r="E122" s="8">
+        <v>45423</v>
+      </c>
+      <c r="F122" s="1">
+        <v>6673000</v>
+      </c>
+      <c r="G122" s="1">
+        <v>6673000</v>
+      </c>
+      <c r="I122" s="1">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J122" s="1">
+        <v>6673000</v>
+      </c>
+      <c r="K122" s="1">
+        <f>G122-J122</f>
+        <v>0</v>
+      </c>
+      <c r="L122" s="1">
+        <f>G122-J122+H122</f>
+        <v>0</v>
+      </c>
+      <c r="M122" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14">
+      <c r="A123" s="6">
+        <v>45437</v>
+      </c>
+      <c r="B123" t="s">
+        <v>93</v>
+      </c>
+      <c r="D123" s="6">
+        <v>45418</v>
+      </c>
+      <c r="E123" s="8">
+        <v>45430</v>
+      </c>
+      <c r="F123" s="1">
+        <v>1108000</v>
+      </c>
+      <c r="G123" s="1">
+        <v>1108000</v>
+      </c>
+      <c r="I123" s="1">
+        <f>G123-F123</f>
+        <v>0</v>
+      </c>
+      <c r="J123" s="1">
+        <v>1108000</v>
+      </c>
+      <c r="K123" s="1">
+        <f>G123-J123</f>
+        <v>0</v>
+      </c>
+      <c r="L123" s="1">
+        <f>G123-J123+H123</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:14">
+      <c r="A124" s="6">
+        <v>45443</v>
+      </c>
+      <c r="B124" t="s">
+        <v>88</v>
+      </c>
+      <c r="D124" s="6">
+        <v>45423</v>
+      </c>
+      <c r="E124" s="8">
+        <v>45436</v>
+      </c>
+      <c r="F124" s="1">
+        <v>7200000</v>
+      </c>
+      <c r="G124" s="1">
+        <v>7200000</v>
+      </c>
+      <c r="I124" s="1">
+        <f>G124-F124</f>
+        <v>0</v>
+      </c>
+      <c r="J124" s="1">
+        <v>7200000</v>
+      </c>
+      <c r="K124" s="1">
+        <f>G124-J124</f>
+        <v>0</v>
+      </c>
+      <c r="L124" s="1">
+        <f>G124-J124+H124</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 9 juni -list utang
</commit_message>
<xml_diff>
--- a/pembayaran/Pembayaran.xlsx
+++ b/pembayaran/Pembayaran.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27804"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/277ffa1efc2bfcc1/Apartment Bintaro/Data Harian/BINTARO-APG/pembayaran/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="14_{1E7DE582-8E6A-4088-84FC-1A8DF5B9EF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{57D4EF30-3431-4FF1-BE74-1B9606E7333A}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="14_{1E7DE582-8E6A-4088-84FC-1A8DF5B9EF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0DB0D9C-75F9-44A1-A5E8-E8A601017E81}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="96">
   <si>
     <t>Tanggal Pembayaran</t>
   </si>
@@ -316,12 +318,6 @@
   </si>
   <si>
     <t>Amin</t>
-  </si>
-  <si>
-    <t>perorangan</t>
-  </si>
-  <si>
-    <t>perorngan</t>
   </si>
   <si>
     <t>30/04/2024</t>
@@ -334,11 +330,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -374,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -396,12 +391,6 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -434,15 +423,15 @@
       <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="right"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
@@ -466,8 +455,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}" name="Table1" displayName="Table1" ref="A1:N132" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A1:N132" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}" name="Table1" displayName="Table1" ref="A1:N134" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A1:N134" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{ADAEF761-889D-4642-B4B1-5AD983017E99}" name="Tanggal Pembayaran" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{1D148A0B-5DE6-485F-ABBF-15493C92DBA8}" name="Nama Mandor"/>
@@ -811,13 +800,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P132"/>
+  <dimension ref="A1:P134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="110" workbookViewId="0">
-      <selection activeCell="A133" sqref="A133"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="H137" sqref="H137"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
@@ -830,7 +819,7 @@
     <col min="15" max="15" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -874,7 +863,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16">
       <c r="A2" s="6">
         <v>45233</v>
       </c>
@@ -906,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16">
       <c r="A3" s="6">
         <v>45234</v>
       </c>
@@ -938,7 +927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16">
       <c r="A4" s="6">
         <v>45248</v>
       </c>
@@ -973,7 +962,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16">
       <c r="B5" t="s">
         <v>17</v>
       </c>
@@ -1005,7 +994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16">
       <c r="C6" t="s">
         <v>19</v>
       </c>
@@ -1034,7 +1023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16">
       <c r="C7" t="s">
         <v>20</v>
       </c>
@@ -1063,7 +1052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16">
       <c r="C8" t="s">
         <v>21</v>
       </c>
@@ -1092,7 +1081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16">
       <c r="B9" t="s">
         <v>15</v>
       </c>
@@ -1124,7 +1113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16">
       <c r="B10" t="s">
         <v>23</v>
       </c>
@@ -1153,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -1185,7 +1174,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -1221,7 +1210,7 @@
       </c>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16">
       <c r="C13" t="s">
         <v>27</v>
       </c>
@@ -1254,7 +1243,7 @@
       </c>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16">
       <c r="C14" t="s">
         <v>28</v>
       </c>
@@ -1284,7 +1273,7 @@
       </c>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16">
       <c r="A15" s="6">
         <v>45252</v>
       </c>
@@ -1321,7 +1310,7 @@
       <c r="N15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16">
       <c r="A16" s="6">
         <v>45261</v>
       </c>
@@ -1357,7 +1346,7 @@
       </c>
       <c r="N16" s="1"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -1395,7 +1384,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14">
       <c r="A18" s="6">
         <v>45273</v>
       </c>
@@ -1434,7 +1423,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19" s="6">
         <v>45275</v>
       </c>
@@ -1475,7 +1464,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="B20" t="s">
         <v>23</v>
       </c>
@@ -1508,7 +1497,7 @@
       </c>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="B21" t="s">
         <v>34</v>
       </c>
@@ -1543,7 +1532,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="C22" t="s">
         <v>37</v>
       </c>
@@ -1575,7 +1564,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="6">
         <v>45277</v>
       </c>
@@ -1611,7 +1600,7 @@
       </c>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="B24" t="s">
         <v>25</v>
       </c>
@@ -1644,7 +1633,7 @@
       </c>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="B25" t="s">
         <v>17</v>
       </c>
@@ -1677,7 +1666,7 @@
       </c>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="C26" t="s">
         <v>39</v>
       </c>
@@ -1707,7 +1696,7 @@
       </c>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="C27" t="s">
         <v>40</v>
       </c>
@@ -1737,7 +1726,7 @@
       </c>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="B28" t="s">
         <v>15</v>
       </c>
@@ -1775,7 +1764,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="6">
         <v>45289</v>
       </c>
@@ -1813,7 +1802,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="B30" t="s">
         <v>14</v>
       </c>
@@ -1852,7 +1841,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14">
       <c r="A31" s="6">
         <v>45290</v>
       </c>
@@ -1888,7 +1877,7 @@
       </c>
       <c r="N31" s="1"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14">
       <c r="C32" t="s">
         <v>44</v>
       </c>
@@ -1918,7 +1907,7 @@
       </c>
       <c r="N32" s="1"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16">
       <c r="C33" t="s">
         <v>45</v>
       </c>
@@ -1948,7 +1937,7 @@
       </c>
       <c r="N33" s="1"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16">
       <c r="C34" t="s">
         <v>46</v>
       </c>
@@ -1978,7 +1967,7 @@
       </c>
       <c r="N34" s="1"/>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16">
       <c r="C35" t="s">
         <v>47</v>
       </c>
@@ -2008,7 +1997,7 @@
       </c>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16">
       <c r="C36" t="s">
         <v>48</v>
       </c>
@@ -2039,7 +2028,7 @@
       <c r="N36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16">
       <c r="A37" s="6">
         <v>45305</v>
       </c>
@@ -2081,7 +2070,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16">
       <c r="A38" s="6">
         <v>45309</v>
       </c>
@@ -2117,7 +2106,7 @@
       </c>
       <c r="N38" s="1"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16">
       <c r="A39" s="6">
         <v>45312</v>
       </c>
@@ -2153,7 +2142,7 @@
       </c>
       <c r="N39" s="1"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16">
       <c r="C40" t="s">
         <v>47</v>
       </c>
@@ -2183,7 +2172,7 @@
       </c>
       <c r="N40" s="1"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16">
       <c r="C41" t="s">
         <v>46</v>
       </c>
@@ -2213,7 +2202,7 @@
       </c>
       <c r="N41" s="1"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16">
       <c r="C42" t="s">
         <v>48</v>
       </c>
@@ -2243,7 +2232,7 @@
       </c>
       <c r="N42" s="1"/>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16">
       <c r="C43" t="s">
         <v>45</v>
       </c>
@@ -2273,7 +2262,7 @@
       </c>
       <c r="N43" s="1"/>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16">
       <c r="C44" t="s">
         <v>44</v>
       </c>
@@ -2303,7 +2292,7 @@
       </c>
       <c r="N44" s="1"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16">
       <c r="C45" t="s">
         <v>39</v>
       </c>
@@ -2333,7 +2322,7 @@
       </c>
       <c r="N45" s="1"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16">
       <c r="C46" t="s">
         <v>49</v>
       </c>
@@ -2363,7 +2352,7 @@
       </c>
       <c r="N46" s="1"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16">
       <c r="B47" t="s">
         <v>15</v>
       </c>
@@ -2402,7 +2391,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16">
       <c r="A48" s="6">
         <v>45316</v>
       </c>
@@ -2438,7 +2427,7 @@
       </c>
       <c r="N48" s="1"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16">
       <c r="C49" t="s">
         <v>51</v>
       </c>
@@ -2468,7 +2457,7 @@
       </c>
       <c r="N49" s="1"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16">
       <c r="C50" t="s">
         <v>52</v>
       </c>
@@ -2498,7 +2487,7 @@
       </c>
       <c r="N50" s="1"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16">
       <c r="C51" t="s">
         <v>54</v>
       </c>
@@ -2528,7 +2517,7 @@
       </c>
       <c r="N51" s="1"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16">
       <c r="C52" t="s">
         <v>55</v>
       </c>
@@ -2555,7 +2544,7 @@
       </c>
       <c r="N52" s="1"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16">
       <c r="C53" t="s">
         <v>38</v>
       </c>
@@ -2579,7 +2568,7 @@
       </c>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16">
       <c r="C54" t="s">
         <v>19</v>
       </c>
@@ -2603,7 +2592,7 @@
       </c>
       <c r="N54" s="1"/>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16">
       <c r="C55" t="s">
         <v>18</v>
       </c>
@@ -2627,7 +2616,7 @@
       </c>
       <c r="N55" s="1"/>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16">
       <c r="A56" s="6">
         <v>45318</v>
       </c>
@@ -2667,7 +2656,7 @@
       </c>
       <c r="N56" s="1"/>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16">
       <c r="B57" t="s">
         <v>34</v>
       </c>
@@ -2694,7 +2683,7 @@
       </c>
       <c r="N57" s="1"/>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16">
       <c r="C58" t="s">
         <v>37</v>
       </c>
@@ -2718,7 +2707,7 @@
       </c>
       <c r="N58" s="1"/>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16">
       <c r="A59" s="6">
         <v>45319</v>
       </c>
@@ -2754,7 +2743,7 @@
       </c>
       <c r="N59" s="1"/>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16">
       <c r="C60" t="s">
         <v>49</v>
       </c>
@@ -2785,7 +2774,7 @@
       <c r="N60" s="1"/>
       <c r="P60" s="1"/>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16">
       <c r="A61" s="6">
         <v>45327</v>
       </c>
@@ -2826,7 +2815,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16">
       <c r="A62" s="6">
         <v>45332</v>
       </c>
@@ -2864,7 +2853,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16">
       <c r="A63" s="6">
         <v>45339</v>
       </c>
@@ -2897,7 +2886,7 @@
       </c>
       <c r="N63" s="1"/>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16">
       <c r="B64" t="s">
         <v>29</v>
       </c>
@@ -2933,7 +2922,7 @@
       </c>
       <c r="N64" s="1"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16">
       <c r="A65" s="6">
         <v>45341</v>
       </c>
@@ -2968,7 +2957,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16">
       <c r="A66" s="6">
         <v>45347</v>
       </c>
@@ -3009,7 +2998,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16">
       <c r="B67" t="s">
         <v>57</v>
       </c>
@@ -3047,7 +3036,7 @@
       <c r="N67" s="1"/>
       <c r="P67" s="1"/>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16">
       <c r="A68" s="6">
         <v>45352</v>
       </c>
@@ -3085,7 +3074,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16">
       <c r="B69" t="s">
         <v>34</v>
       </c>
@@ -3118,7 +3107,7 @@
       </c>
       <c r="N69" s="1"/>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16">
       <c r="C70" t="s">
         <v>66</v>
       </c>
@@ -3148,7 +3137,7 @@
       </c>
       <c r="N70" s="1"/>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16">
       <c r="C71" t="s">
         <v>67</v>
       </c>
@@ -3178,7 +3167,7 @@
       </c>
       <c r="N71" s="1"/>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16">
       <c r="C72" t="s">
         <v>68</v>
       </c>
@@ -3208,7 +3197,7 @@
       </c>
       <c r="N72" s="1"/>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16">
       <c r="A73" s="6">
         <v>45354</v>
       </c>
@@ -3246,7 +3235,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16">
       <c r="A74" s="6">
         <v>45358</v>
       </c>
@@ -3285,7 +3274,7 @@
       </c>
       <c r="N74" s="1"/>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16">
       <c r="A75" s="6">
         <v>45361</v>
       </c>
@@ -3318,7 +3307,7 @@
       </c>
       <c r="N75" s="1"/>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16">
       <c r="A76" s="6">
         <v>45362</v>
       </c>
@@ -3359,7 +3348,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16">
       <c r="A77" s="6">
         <v>45366</v>
       </c>
@@ -3395,7 +3384,7 @@
       </c>
       <c r="N77" s="1"/>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16">
       <c r="C78" t="s">
         <v>74</v>
       </c>
@@ -3429,7 +3418,7 @@
       <c r="N78" s="1"/>
       <c r="P78" s="1"/>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16">
       <c r="A79" s="6">
         <v>45368</v>
       </c>
@@ -3469,7 +3458,7 @@
       </c>
       <c r="N79" s="1"/>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16">
       <c r="A80" s="6">
         <v>45374</v>
       </c>
@@ -3508,7 +3497,7 @@
       </c>
       <c r="N80" s="1"/>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16">
       <c r="C81" t="s">
         <v>27</v>
       </c>
@@ -3541,7 +3530,7 @@
       </c>
       <c r="N81" s="1"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16">
       <c r="C82" t="s">
         <v>76</v>
       </c>
@@ -3574,7 +3563,7 @@
       </c>
       <c r="N82" s="1"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16">
       <c r="B83" t="s">
         <v>57</v>
       </c>
@@ -3610,7 +3599,7 @@
       </c>
       <c r="N83" s="1"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16">
       <c r="B84" t="s">
         <v>34</v>
       </c>
@@ -3648,7 +3637,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16">
       <c r="A85" s="6">
         <v>45376</v>
       </c>
@@ -3684,7 +3673,7 @@
       </c>
       <c r="N85" s="1"/>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16">
       <c r="B86" t="s">
         <v>79</v>
       </c>
@@ -3722,7 +3711,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16">
       <c r="A87" s="6">
         <v>45380</v>
       </c>
@@ -3761,7 +3750,7 @@
       </c>
       <c r="N87" s="1"/>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16">
       <c r="B88" t="s">
         <v>29</v>
       </c>
@@ -3797,7 +3786,7 @@
       </c>
       <c r="N88" s="1"/>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16">
       <c r="C89" t="s">
         <v>63</v>
       </c>
@@ -3836,7 +3825,7 @@
       </c>
       <c r="P89" s="1"/>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16">
       <c r="A90" s="6">
         <v>45383</v>
       </c>
@@ -3875,7 +3864,7 @@
       </c>
       <c r="N90" s="1"/>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16">
       <c r="B91" t="s">
         <v>34</v>
       </c>
@@ -3911,7 +3900,7 @@
       </c>
       <c r="N91" s="1"/>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16">
       <c r="C92" t="s">
         <v>67</v>
       </c>
@@ -3944,7 +3933,7 @@
       </c>
       <c r="N92" s="1"/>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16">
       <c r="C93" t="s">
         <v>68</v>
       </c>
@@ -3977,7 +3966,7 @@
       </c>
       <c r="N93" s="1"/>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16">
       <c r="B94" t="s">
         <v>25</v>
       </c>
@@ -4012,7 +4001,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16">
       <c r="C95" t="s">
         <v>28</v>
       </c>
@@ -4048,7 +4037,7 @@
       </c>
       <c r="P95" s="1"/>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16">
       <c r="A96" s="6">
         <v>45385</v>
       </c>
@@ -4092,7 +4081,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14">
       <c r="A97" s="6">
         <v>45386</v>
       </c>
@@ -4130,7 +4119,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14">
       <c r="B98" t="s">
         <v>15</v>
       </c>
@@ -4171,7 +4160,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14">
       <c r="A99" s="6">
         <v>45387</v>
       </c>
@@ -4212,7 +4201,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14">
       <c r="B100" t="s">
         <v>29</v>
       </c>
@@ -4247,7 +4236,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14">
       <c r="B101" t="s">
         <v>79</v>
       </c>
@@ -4285,7 +4274,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14">
       <c r="A102" s="6">
         <v>45408</v>
       </c>
@@ -4329,7 +4318,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14">
       <c r="A103" s="6">
         <v>45409</v>
       </c>
@@ -4367,7 +4356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14">
       <c r="A104" s="6">
         <v>45410</v>
       </c>
@@ -4402,7 +4391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14">
       <c r="A105" s="6">
         <v>45412</v>
       </c>
@@ -4437,7 +4426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14">
       <c r="A106" s="6">
         <v>45413</v>
       </c>
@@ -4475,7 +4464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14">
       <c r="C107" t="s">
         <v>67</v>
       </c>
@@ -4507,7 +4496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14">
       <c r="C108" t="s">
         <v>68</v>
       </c>
@@ -4539,7 +4528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14">
       <c r="A109" s="6">
         <v>45414</v>
       </c>
@@ -4583,7 +4572,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14">
       <c r="A110" s="6">
         <v>45416</v>
       </c>
@@ -4627,7 +4616,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14">
       <c r="B111" t="s">
         <v>57</v>
       </c>
@@ -4665,7 +4654,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14">
       <c r="A112" s="6">
         <v>45417</v>
       </c>
@@ -4703,7 +4692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14">
       <c r="A113" s="6">
         <v>45420</v>
       </c>
@@ -4741,7 +4730,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14">
       <c r="A114" s="6">
         <v>45424</v>
       </c>
@@ -4776,7 +4765,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14">
       <c r="A115" s="6">
         <v>45427</v>
       </c>
@@ -4814,7 +4803,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14">
       <c r="B116" t="s">
         <v>79</v>
       </c>
@@ -4852,7 +4841,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14">
       <c r="A117" s="6">
         <v>45430</v>
       </c>
@@ -4890,7 +4879,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14">
       <c r="B118" t="s">
         <v>92</v>
       </c>
@@ -4925,7 +4914,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14">
       <c r="B119" t="s">
         <v>15</v>
       </c>
@@ -4966,7 +4955,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14">
       <c r="A120" s="6">
         <v>45434</v>
       </c>
@@ -5004,7 +4993,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14">
       <c r="B121" t="s">
         <v>90</v>
       </c>
@@ -5039,7 +5028,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14">
       <c r="B122" t="s">
         <v>27</v>
       </c>
@@ -5074,7 +5063,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14">
       <c r="A123" s="6">
         <v>45437</v>
       </c>
@@ -5109,7 +5098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14">
       <c r="A124" s="6">
         <v>45443</v>
       </c>
@@ -5144,7 +5133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14">
       <c r="A125" s="6">
         <v>45444</v>
       </c>
@@ -5182,10 +5171,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A126" s="6">
-        <v>45444</v>
-      </c>
+    <row r="126" spans="1:14">
       <c r="B126" t="s">
         <v>25</v>
       </c>
@@ -5220,20 +5206,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A127" s="9">
-        <v>45444</v>
-      </c>
+    <row r="127" spans="1:14">
       <c r="B127" t="s">
-        <v>95</v>
+        <v>34</v>
       </c>
       <c r="C127" t="s">
         <v>67</v>
       </c>
-      <c r="D127" s="9">
+      <c r="D127" s="6">
         <v>191509</v>
       </c>
-      <c r="E127" s="10">
+      <c r="E127" s="8">
         <v>45442</v>
       </c>
       <c r="F127" s="1">
@@ -5258,21 +5241,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A128" s="9">
-        <v>45444</v>
-      </c>
-      <c r="B128" t="s">
-        <v>94</v>
-      </c>
+    <row r="128" spans="1:14">
       <c r="C128" t="s">
         <v>65</v>
       </c>
-      <c r="D128" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E128" s="10" t="s">
-        <v>97</v>
+      <c r="D128" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="E128" s="8" t="s">
+        <v>95</v>
       </c>
       <c r="F128" s="1">
         <v>2441000</v>
@@ -5296,17 +5273,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A129" s="9">
-        <v>45444</v>
-      </c>
+    <row r="129" spans="1:13">
       <c r="B129" t="s">
         <v>79</v>
       </c>
-      <c r="D129" s="9">
+      <c r="D129" s="6">
         <v>45424</v>
       </c>
-      <c r="E129" s="10">
+      <c r="E129" s="8">
         <v>45442</v>
       </c>
       <c r="F129" s="1">
@@ -5337,17 +5311,14 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A130" s="9">
-        <v>45444</v>
-      </c>
+    <row r="130" spans="1:13">
       <c r="B130" t="s">
         <v>60</v>
       </c>
-      <c r="D130" s="9">
+      <c r="D130" s="6">
         <v>45401</v>
       </c>
-      <c r="E130" s="10">
+      <c r="E130" s="8">
         <v>45415</v>
       </c>
       <c r="F130" s="1">
@@ -5372,20 +5343,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A131" s="9">
-        <v>45444</v>
-      </c>
+    <row r="131" spans="1:13">
       <c r="B131" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
       <c r="C131" t="s">
         <v>68</v>
       </c>
-      <c r="D131" s="9">
+      <c r="D131" s="6">
         <v>45412</v>
       </c>
-      <c r="E131" s="10">
+      <c r="E131" s="8">
         <v>45442</v>
       </c>
       <c r="F131" s="1">
@@ -5410,17 +5378,14 @@
         <v>429000</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A132" s="9">
-        <v>45444</v>
-      </c>
+    <row r="132" spans="1:13">
       <c r="B132" t="s">
         <v>93</v>
       </c>
-      <c r="D132" s="9">
+      <c r="D132" s="6">
         <v>45431</v>
       </c>
-      <c r="E132" s="10">
+      <c r="E132" s="8">
         <v>45442</v>
       </c>
       <c r="F132" s="1">
@@ -5443,6 +5408,82 @@
       <c r="L132" s="1">
         <f t="shared" si="15"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13">
+      <c r="A133" s="6">
+        <v>45450</v>
+      </c>
+      <c r="B133" t="s">
+        <v>90</v>
+      </c>
+      <c r="D133" s="6">
+        <v>45423</v>
+      </c>
+      <c r="E133" s="8">
+        <v>45436</v>
+      </c>
+      <c r="F133" s="1">
+        <v>5049000</v>
+      </c>
+      <c r="G133" s="1">
+        <v>3448000</v>
+      </c>
+      <c r="I133" s="1">
+        <f>G133-F133</f>
+        <v>-1601000</v>
+      </c>
+      <c r="J133" s="1">
+        <v>3448000</v>
+      </c>
+      <c r="K133" s="1">
+        <f>G133-J133</f>
+        <v>0</v>
+      </c>
+      <c r="L133" s="1">
+        <f>G133-J133+H133</f>
+        <v>0</v>
+      </c>
+      <c r="M133" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13">
+      <c r="B134" t="s">
+        <v>92</v>
+      </c>
+      <c r="D134" s="6">
+        <v>45422</v>
+      </c>
+      <c r="E134" s="8">
+        <v>45435</v>
+      </c>
+      <c r="F134" s="1">
+        <v>16778000</v>
+      </c>
+      <c r="G134" s="1">
+        <v>16778000</v>
+      </c>
+      <c r="H134" s="1">
+        <v>3523000</v>
+      </c>
+      <c r="I134" s="1">
+        <f>G134-F134</f>
+        <v>0</v>
+      </c>
+      <c r="J134" s="1">
+        <v>18000000</v>
+      </c>
+      <c r="K134" s="1">
+        <f>G134-J134</f>
+        <v>-1222000</v>
+      </c>
+      <c r="L134" s="1">
+        <f>G134-J134+H134</f>
+        <v>2301000</v>
+      </c>
+      <c r="M134" s="1">
+        <v>100000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 30 juni 2024
</commit_message>
<xml_diff>
--- a/pembayaran/Pembayaran.xlsx
+++ b/pembayaran/Pembayaran.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27809"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/277ffa1efc2bfcc1/Apartment Bintaro/Data Harian/BINTARO-APG/pembayaran/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="14_{1E7DE582-8E6A-4088-84FC-1A8DF5B9EF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{240C770A-C94E-420E-8EA7-8EB06AE23FE0}"/>
+  <xr:revisionPtr revIDLastSave="292" documentId="14_{1E7DE582-8E6A-4088-84FC-1A8DF5B9EF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4F5FEA7-649E-4B2E-88FE-42879FEE7A24}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="104">
   <si>
     <t>Tanggal Pembayaran</t>
   </si>
@@ -287,6 +287,9 @@
     <t>gabung tgl 03 apr 2024</t>
   </si>
   <si>
+    <t>gabung tgl 28 juni 2024</t>
+  </si>
+  <si>
     <t>lunas tgl 27 apr 2024</t>
   </si>
   <si>
@@ -302,6 +305,9 @@
     <t>Alvian</t>
   </si>
   <si>
+    <t>gabung tgl 26 juni 2024</t>
+  </si>
+  <si>
     <t>Dede</t>
   </si>
   <si>
@@ -324,6 +330,24 @@
   </si>
   <si>
     <t>30/05/2024</t>
+  </si>
+  <si>
+    <t>lunas tgl 01 juli 2024</t>
+  </si>
+  <si>
+    <t>Eko &amp; Sarana</t>
+  </si>
+  <si>
+    <t>lunas tgl 28 juni 2024</t>
+  </si>
+  <si>
+    <t>lunas tgl 26 juni 2024</t>
+  </si>
+  <si>
+    <t>Ujang P</t>
+  </si>
+  <si>
+    <t>lunas</t>
   </si>
 </sst>
 </file>
@@ -455,8 +479,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}" name="Table1" displayName="Table1" ref="A1:N135" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A1:N135" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}" name="Table1" displayName="Table1" ref="A1:N160" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A1:N160" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{ADAEF761-889D-4642-B4B1-5AD983017E99}" name="Tanggal Pembayaran" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{1D148A0B-5DE6-485F-ABBF-15493C92DBA8}" name="Nama Mandor"/>
@@ -800,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P135"/>
+  <dimension ref="A1:P160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="110" workbookViewId="0">
-      <selection activeCell="N130" sqref="N130"/>
+    <sheetView tabSelected="1" topLeftCell="F125" zoomScale="110" workbookViewId="0">
+      <selection activeCell="N140" sqref="N140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4078,7 +4102,7 @@
         <v>582000</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:14">
@@ -4116,7 +4140,7 @@
         <v>7678000</v>
       </c>
       <c r="N97" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="98" spans="1:14">
@@ -4157,7 +4181,7 @@
         <v>150000</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="99" spans="1:14">
@@ -4198,7 +4222,7 @@
         <v>100000</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="100" spans="1:14">
@@ -4271,7 +4295,7 @@
         <v>1313000</v>
       </c>
       <c r="N101" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="102" spans="1:14">
@@ -4282,7 +4306,7 @@
         <v>25</v>
       </c>
       <c r="C102" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D102" s="6">
         <v>45378</v>
@@ -4315,7 +4339,7 @@
         <v>141000</v>
       </c>
       <c r="N102" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
     </row>
     <row r="103" spans="1:14">
@@ -4396,7 +4420,7 @@
         <v>45412</v>
       </c>
       <c r="B105" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D105" s="6">
         <v>45403</v>
@@ -4613,7 +4637,7 @@
         <v>200000</v>
       </c>
       <c r="N110" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="111" spans="1:14">
@@ -4697,7 +4721,7 @@
         <v>45420</v>
       </c>
       <c r="B113" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D113" s="6">
         <v>45399</v>
@@ -4735,7 +4759,7 @@
         <v>45424</v>
       </c>
       <c r="B114" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D114" s="6">
         <v>45404</v>
@@ -4770,7 +4794,7 @@
         <v>45427</v>
       </c>
       <c r="B115" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D115" s="6">
         <v>45412</v>
@@ -4881,7 +4905,7 @@
     </row>
     <row r="118" spans="1:14">
       <c r="B118" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D118" s="6">
         <v>45412</v>
@@ -4960,7 +4984,7 @@
         <v>45434</v>
       </c>
       <c r="B120" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D120" s="6">
         <v>45419</v>
@@ -4995,7 +5019,7 @@
     </row>
     <row r="121" spans="1:14">
       <c r="B121" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D121" s="6">
         <v>45408</v>
@@ -5068,7 +5092,7 @@
         <v>45437</v>
       </c>
       <c r="B123" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D123" s="6">
         <v>45418</v>
@@ -5103,7 +5127,7 @@
         <v>45443</v>
       </c>
       <c r="B124" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D124" s="6">
         <v>45423</v>
@@ -5246,10 +5270,10 @@
         <v>65</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F128" s="1">
         <v>2441000</v>
@@ -5381,12 +5405,12 @@
         <v>429000</v>
       </c>
       <c r="N131" t="s">
-        <v>70</v>
+        <v>98</v>
       </c>
     </row>
     <row r="132" spans="1:14">
       <c r="B132" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D132" s="6">
         <v>45431</v>
@@ -5421,7 +5445,7 @@
         <v>45450</v>
       </c>
       <c r="B133" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D133" s="6">
         <v>45423</v>
@@ -5456,7 +5480,7 @@
     </row>
     <row r="134" spans="1:14">
       <c r="B134" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D134" s="6">
         <v>45422</v>
@@ -5492,7 +5516,7 @@
         <v>100000</v>
       </c>
       <c r="N134" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
     </row>
     <row r="135" spans="1:14">
@@ -5531,6 +5555,986 @@
       </c>
       <c r="M135" s="1">
         <v>100000</v>
+      </c>
+    </row>
+    <row r="136" spans="1:14">
+      <c r="A136" s="6">
+        <v>45456</v>
+      </c>
+      <c r="B136" t="s">
+        <v>93</v>
+      </c>
+      <c r="D136" s="6">
+        <v>45431</v>
+      </c>
+      <c r="E136" s="8">
+        <v>45444</v>
+      </c>
+      <c r="F136" s="1">
+        <v>5367000</v>
+      </c>
+      <c r="G136" s="1">
+        <v>5367000</v>
+      </c>
+      <c r="I136" s="1">
+        <f t="shared" ref="I136:I144" si="16">G136-F136</f>
+        <v>0</v>
+      </c>
+      <c r="J136" s="1">
+        <v>5367000</v>
+      </c>
+      <c r="K136" s="1">
+        <f t="shared" ref="K136:K144" si="17">G136-J136</f>
+        <v>0</v>
+      </c>
+      <c r="L136" s="1">
+        <f t="shared" ref="L136:L144" si="18">G136-J136+H136</f>
+        <v>0</v>
+      </c>
+      <c r="M136" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="137" spans="1:14">
+      <c r="B137" t="s">
+        <v>90</v>
+      </c>
+      <c r="D137" s="6">
+        <v>45437</v>
+      </c>
+      <c r="E137" s="8">
+        <v>45452</v>
+      </c>
+      <c r="F137" s="1">
+        <v>7273000</v>
+      </c>
+      <c r="G137" s="1">
+        <v>7273000</v>
+      </c>
+      <c r="I137" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J137" s="1">
+        <v>7080000</v>
+      </c>
+      <c r="K137" s="1">
+        <f t="shared" si="17"/>
+        <v>193000</v>
+      </c>
+      <c r="L137" s="1">
+        <f t="shared" si="18"/>
+        <v>193000</v>
+      </c>
+      <c r="M137" s="1">
+        <v>100000</v>
+      </c>
+      <c r="N137" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="138" spans="1:14">
+      <c r="A138" s="6">
+        <v>45457</v>
+      </c>
+      <c r="B138" t="s">
+        <v>57</v>
+      </c>
+      <c r="D138" s="6">
+        <v>45443</v>
+      </c>
+      <c r="E138" s="8">
+        <v>45456</v>
+      </c>
+      <c r="F138" s="1">
+        <v>1692000</v>
+      </c>
+      <c r="G138" s="1">
+        <v>1692000</v>
+      </c>
+      <c r="I138" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J138" s="1">
+        <v>1692000</v>
+      </c>
+      <c r="K138" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="L138" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="M138" s="1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="139" spans="1:14">
+      <c r="B139" t="s">
+        <v>29</v>
+      </c>
+      <c r="C139" t="s">
+        <v>99</v>
+      </c>
+      <c r="D139" s="6">
+        <v>45231</v>
+      </c>
+      <c r="E139" s="8">
+        <v>45373</v>
+      </c>
+      <c r="F139" s="1">
+        <v>2514000</v>
+      </c>
+      <c r="G139" s="1">
+        <v>2514000</v>
+      </c>
+      <c r="I139" s="1">
+        <f>G139-F139</f>
+        <v>0</v>
+      </c>
+      <c r="J139" s="1">
+        <v>1500000</v>
+      </c>
+      <c r="K139" s="1">
+        <f>G139-J139</f>
+        <v>1014000</v>
+      </c>
+      <c r="L139" s="1">
+        <f>G139-J139+H139</f>
+        <v>1014000</v>
+      </c>
+      <c r="N139" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="140" spans="1:14">
+      <c r="A140" s="6">
+        <v>45458</v>
+      </c>
+      <c r="B140" t="s">
+        <v>60</v>
+      </c>
+      <c r="D140" s="6">
+        <v>45416</v>
+      </c>
+      <c r="E140" s="8">
+        <v>45447</v>
+      </c>
+      <c r="F140" s="1">
+        <v>36606000</v>
+      </c>
+      <c r="G140" s="1">
+        <v>36606000</v>
+      </c>
+      <c r="I140" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J140" s="1">
+        <v>30000000</v>
+      </c>
+      <c r="K140" s="1">
+        <f t="shared" si="17"/>
+        <v>6606000</v>
+      </c>
+      <c r="L140" s="1">
+        <f t="shared" si="18"/>
+        <v>6606000</v>
+      </c>
+      <c r="M140" s="1">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="141" spans="1:14">
+      <c r="A141" s="6">
+        <v>45459</v>
+      </c>
+      <c r="B141" t="s">
+        <v>79</v>
+      </c>
+      <c r="D141" s="6">
+        <v>45443</v>
+      </c>
+      <c r="E141" s="8">
+        <v>45456</v>
+      </c>
+      <c r="F141" s="1">
+        <v>6131000</v>
+      </c>
+      <c r="G141" s="1">
+        <v>6131000</v>
+      </c>
+      <c r="H141" s="1">
+        <v>3763000</v>
+      </c>
+      <c r="I141" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J141" s="1">
+        <v>6000000</v>
+      </c>
+      <c r="K141" s="1">
+        <f t="shared" si="17"/>
+        <v>131000</v>
+      </c>
+      <c r="L141" s="1">
+        <f t="shared" si="18"/>
+        <v>3894000</v>
+      </c>
+      <c r="M141" s="1">
+        <v>100000</v>
+      </c>
+      <c r="N141" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="142" spans="1:14">
+      <c r="A142" s="6">
+        <v>45463</v>
+      </c>
+      <c r="B142" t="s">
+        <v>93</v>
+      </c>
+      <c r="D142" s="6">
+        <v>45445</v>
+      </c>
+      <c r="E142" s="8">
+        <v>45458</v>
+      </c>
+      <c r="F142" s="1">
+        <v>5481000</v>
+      </c>
+      <c r="G142" s="1">
+        <v>5481000</v>
+      </c>
+      <c r="I142" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J142" s="1">
+        <v>5481000</v>
+      </c>
+      <c r="K142" s="1">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="L142" s="1">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="M142" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="143" spans="1:14">
+      <c r="A143" s="6">
+        <v>45466</v>
+      </c>
+      <c r="B143" t="s">
+        <v>92</v>
+      </c>
+      <c r="D143" s="6">
+        <v>45437</v>
+      </c>
+      <c r="E143" s="8">
+        <v>45451</v>
+      </c>
+      <c r="F143" s="1">
+        <v>4103000</v>
+      </c>
+      <c r="G143" s="1">
+        <v>5704000</v>
+      </c>
+      <c r="I143" s="1">
+        <f t="shared" si="16"/>
+        <v>1601000</v>
+      </c>
+      <c r="J143" s="1">
+        <v>2000000</v>
+      </c>
+      <c r="K143" s="1">
+        <f t="shared" si="17"/>
+        <v>3704000</v>
+      </c>
+      <c r="L143" s="1">
+        <f t="shared" si="18"/>
+        <v>3704000</v>
+      </c>
+      <c r="M143" s="1">
+        <v>50000</v>
+      </c>
+      <c r="N143" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="144" spans="1:14">
+      <c r="B144" t="s">
+        <v>19</v>
+      </c>
+      <c r="D144" s="6">
+        <v>45447</v>
+      </c>
+      <c r="E144" s="8">
+        <v>45464</v>
+      </c>
+      <c r="F144" s="1">
+        <v>2043000</v>
+      </c>
+      <c r="G144" s="1">
+        <v>2043000</v>
+      </c>
+      <c r="I144" s="1">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J144" s="1">
+        <v>1823000</v>
+      </c>
+      <c r="K144" s="1">
+        <f t="shared" si="17"/>
+        <v>220000</v>
+      </c>
+      <c r="L144" s="1">
+        <f t="shared" si="18"/>
+        <v>220000</v>
+      </c>
+      <c r="N144" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="145" spans="1:14">
+      <c r="B145" t="s">
+        <v>27</v>
+      </c>
+      <c r="D145" s="6">
+        <v>45438</v>
+      </c>
+      <c r="E145" s="8">
+        <v>45450</v>
+      </c>
+      <c r="F145" s="1">
+        <v>3086000</v>
+      </c>
+      <c r="G145" s="1">
+        <v>3086000</v>
+      </c>
+      <c r="I145" s="1">
+        <f>G145-F145</f>
+        <v>0</v>
+      </c>
+      <c r="J145" s="1">
+        <v>3086000</v>
+      </c>
+      <c r="K145" s="1">
+        <f>G145-J145</f>
+        <v>0</v>
+      </c>
+      <c r="L145" s="1">
+        <f>G145-J145+H145</f>
+        <v>0</v>
+      </c>
+      <c r="M145" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14">
+      <c r="A146" s="6">
+        <v>45468</v>
+      </c>
+      <c r="B146" t="s">
+        <v>15</v>
+      </c>
+      <c r="D146" s="6">
+        <v>45429</v>
+      </c>
+      <c r="E146" s="8">
+        <v>45442</v>
+      </c>
+      <c r="F146" s="1">
+        <v>4202000</v>
+      </c>
+      <c r="G146" s="1">
+        <v>4202000</v>
+      </c>
+      <c r="H146" s="1">
+        <v>35241000</v>
+      </c>
+      <c r="I146" s="1">
+        <f>G146-F146</f>
+        <v>0</v>
+      </c>
+      <c r="J146" s="1">
+        <v>4202000</v>
+      </c>
+      <c r="K146" s="1">
+        <f>G146-J146</f>
+        <v>0</v>
+      </c>
+      <c r="L146" s="1">
+        <f>G146-J146+H146</f>
+        <v>35241000</v>
+      </c>
+      <c r="M146" s="1">
+        <v>50000</v>
+      </c>
+      <c r="N146" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="147" spans="1:14">
+      <c r="A147" s="6">
+        <v>45469</v>
+      </c>
+      <c r="B147" t="s">
+        <v>15</v>
+      </c>
+      <c r="D147" s="6">
+        <v>45443</v>
+      </c>
+      <c r="E147" s="8">
+        <v>45467</v>
+      </c>
+      <c r="F147" s="1">
+        <v>15635000</v>
+      </c>
+      <c r="G147" s="1">
+        <v>15635000</v>
+      </c>
+      <c r="H147" s="1">
+        <v>35241000</v>
+      </c>
+      <c r="I147" s="1">
+        <f>G147-F147</f>
+        <v>0</v>
+      </c>
+      <c r="J147" s="1">
+        <v>14676000</v>
+      </c>
+      <c r="K147" s="1">
+        <f>G147-J147</f>
+        <v>959000</v>
+      </c>
+      <c r="L147" s="1">
+        <f>G147-J147+H147</f>
+        <v>36200000</v>
+      </c>
+      <c r="M147" s="1">
+        <v>150000</v>
+      </c>
+      <c r="N147" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="148" spans="1:14">
+      <c r="B148" t="s">
+        <v>94</v>
+      </c>
+      <c r="D148" s="6">
+        <v>45436</v>
+      </c>
+      <c r="E148" s="8">
+        <v>45449</v>
+      </c>
+      <c r="F148" s="1">
+        <v>13492000</v>
+      </c>
+      <c r="G148" s="1">
+        <v>13492000</v>
+      </c>
+      <c r="H148" s="1">
+        <v>2301000</v>
+      </c>
+      <c r="I148" s="1">
+        <f>G148-F148</f>
+        <v>0</v>
+      </c>
+      <c r="J148" s="1">
+        <v>14293000</v>
+      </c>
+      <c r="K148" s="1">
+        <f>G148-J148</f>
+        <v>-801000</v>
+      </c>
+      <c r="L148" s="1">
+        <f>G148-J148+H148</f>
+        <v>1500000</v>
+      </c>
+      <c r="M148" s="1">
+        <v>150000</v>
+      </c>
+      <c r="N148" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="149" spans="1:14">
+      <c r="B149" t="s">
+        <v>92</v>
+      </c>
+      <c r="D149" s="6">
+        <v>45437</v>
+      </c>
+      <c r="E149" s="8">
+        <v>45451</v>
+      </c>
+      <c r="F149" s="1">
+        <v>0</v>
+      </c>
+      <c r="G149" s="1">
+        <v>0</v>
+      </c>
+      <c r="H149" s="1">
+        <v>3704000</v>
+      </c>
+      <c r="I149" s="1">
+        <f>G149-F149</f>
+        <v>0</v>
+      </c>
+      <c r="J149" s="1">
+        <v>3704000</v>
+      </c>
+      <c r="K149" s="1">
+        <f>G149-J149</f>
+        <v>-3704000</v>
+      </c>
+      <c r="L149" s="1">
+        <f>G149-J149+H149</f>
+        <v>0</v>
+      </c>
+      <c r="M149" s="1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="150" spans="1:14">
+      <c r="A150" s="6">
+        <v>45470</v>
+      </c>
+      <c r="B150" t="s">
+        <v>25</v>
+      </c>
+      <c r="C150" t="s">
+        <v>88</v>
+      </c>
+      <c r="D150" s="6">
+        <v>45407</v>
+      </c>
+      <c r="E150" s="8">
+        <v>45470</v>
+      </c>
+      <c r="F150" s="1">
+        <v>1134000</v>
+      </c>
+      <c r="G150" s="1">
+        <v>1134000</v>
+      </c>
+      <c r="H150" s="1">
+        <v>141000</v>
+      </c>
+      <c r="I150" s="1">
+        <f>G150-F150</f>
+        <v>0</v>
+      </c>
+      <c r="J150" s="1">
+        <v>200000</v>
+      </c>
+      <c r="K150" s="1">
+        <f>G150-J150</f>
+        <v>934000</v>
+      </c>
+      <c r="L150" s="1">
+        <f>G150-J150+H150</f>
+        <v>1075000</v>
+      </c>
+      <c r="N150" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14">
+      <c r="A151" s="6">
+        <v>45471</v>
+      </c>
+      <c r="B151" t="s">
+        <v>29</v>
+      </c>
+      <c r="C151" t="s">
+        <v>102</v>
+      </c>
+      <c r="D151" s="6">
+        <v>45463</v>
+      </c>
+      <c r="E151" s="8">
+        <v>45470</v>
+      </c>
+      <c r="F151" s="1">
+        <v>314000</v>
+      </c>
+      <c r="G151" s="1">
+        <v>314000</v>
+      </c>
+      <c r="I151" s="1">
+        <f>G151-F151</f>
+        <v>0</v>
+      </c>
+      <c r="J151" s="1">
+        <v>314000</v>
+      </c>
+      <c r="K151" s="1">
+        <f>G151-J151</f>
+        <v>0</v>
+      </c>
+      <c r="L151" s="1">
+        <f>G151-J151+H151</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14">
+      <c r="C152" t="s">
+        <v>99</v>
+      </c>
+      <c r="D152" s="6">
+        <v>45231</v>
+      </c>
+      <c r="E152" s="8">
+        <v>45373</v>
+      </c>
+      <c r="F152" s="1">
+        <v>0</v>
+      </c>
+      <c r="G152" s="1">
+        <v>0</v>
+      </c>
+      <c r="H152" s="1">
+        <v>1014000</v>
+      </c>
+      <c r="I152" s="1">
+        <f>G152-F152</f>
+        <v>0</v>
+      </c>
+      <c r="J152" s="1">
+        <v>1014000</v>
+      </c>
+      <c r="K152" s="1">
+        <f>G152-J152</f>
+        <v>-1014000</v>
+      </c>
+      <c r="L152" s="1">
+        <f>G152-J152+H152</f>
+        <v>0</v>
+      </c>
+      <c r="M152" s="1">
+        <v>14000</v>
+      </c>
+      <c r="N152" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14">
+      <c r="B153" t="s">
+        <v>25</v>
+      </c>
+      <c r="C153" t="s">
+        <v>26</v>
+      </c>
+      <c r="D153" s="6">
+        <v>45385</v>
+      </c>
+      <c r="E153" s="8">
+        <v>45471</v>
+      </c>
+      <c r="F153" s="1">
+        <v>554000</v>
+      </c>
+      <c r="G153" s="1">
+        <v>554000</v>
+      </c>
+      <c r="H153" s="1">
+        <v>582000</v>
+      </c>
+      <c r="I153" s="1">
+        <f>G153-F153</f>
+        <v>0</v>
+      </c>
+      <c r="J153" s="1">
+        <v>500000</v>
+      </c>
+      <c r="K153" s="1">
+        <f>G153-J153</f>
+        <v>54000</v>
+      </c>
+      <c r="L153" s="1">
+        <f>G153-J153+H153</f>
+        <v>636000</v>
+      </c>
+      <c r="N153" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14">
+      <c r="A154" s="6">
+        <v>45473</v>
+      </c>
+      <c r="B154" t="s">
+        <v>57</v>
+      </c>
+      <c r="D154" s="6">
+        <v>45457</v>
+      </c>
+      <c r="E154" s="8">
+        <v>45471</v>
+      </c>
+      <c r="F154" s="1">
+        <v>1129000</v>
+      </c>
+      <c r="G154" s="1">
+        <v>1129000</v>
+      </c>
+      <c r="I154" s="1">
+        <f>G154-F154</f>
+        <v>0</v>
+      </c>
+      <c r="J154" s="1">
+        <v>1129000</v>
+      </c>
+      <c r="K154" s="1">
+        <f>G154-J154</f>
+        <v>0</v>
+      </c>
+      <c r="L154" s="1">
+        <f>G154-J154+H154</f>
+        <v>0</v>
+      </c>
+      <c r="M154" s="1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14">
+      <c r="A155" s="6">
+        <v>45474</v>
+      </c>
+      <c r="B155" t="s">
+        <v>93</v>
+      </c>
+      <c r="D155" s="6">
+        <v>45459</v>
+      </c>
+      <c r="E155" s="8">
+        <v>45472</v>
+      </c>
+      <c r="F155" s="1">
+        <v>5896000</v>
+      </c>
+      <c r="G155" s="1">
+        <v>5896000</v>
+      </c>
+      <c r="I155" s="1">
+        <f>G155-F155</f>
+        <v>0</v>
+      </c>
+      <c r="J155" s="1">
+        <v>5896000</v>
+      </c>
+      <c r="K155" s="1">
+        <f>G155-J155</f>
+        <v>0</v>
+      </c>
+      <c r="L155" s="1">
+        <f>G155-J155+H155</f>
+        <v>0</v>
+      </c>
+      <c r="M155" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14">
+      <c r="B156" t="s">
+        <v>34</v>
+      </c>
+      <c r="C156" t="s">
+        <v>67</v>
+      </c>
+      <c r="D156" s="6">
+        <v>45443</v>
+      </c>
+      <c r="E156" s="8">
+        <v>45473</v>
+      </c>
+      <c r="F156" s="1">
+        <v>2196000</v>
+      </c>
+      <c r="G156" s="1">
+        <v>2212000</v>
+      </c>
+      <c r="I156" s="1">
+        <f>G156-F156</f>
+        <v>16000</v>
+      </c>
+      <c r="J156" s="1">
+        <v>2212000</v>
+      </c>
+      <c r="K156" s="1">
+        <f>G156-J156</f>
+        <v>0</v>
+      </c>
+      <c r="L156" s="1">
+        <f>G156-J156+H156</f>
+        <v>0</v>
+      </c>
+      <c r="M156" s="1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14">
+      <c r="C157" t="s">
+        <v>65</v>
+      </c>
+      <c r="D157" s="6">
+        <v>45443</v>
+      </c>
+      <c r="E157" s="8">
+        <v>45473</v>
+      </c>
+      <c r="F157" s="1">
+        <v>2105000</v>
+      </c>
+      <c r="G157" s="1">
+        <v>2113000</v>
+      </c>
+      <c r="I157" s="1">
+        <f>G157-F157</f>
+        <v>8000</v>
+      </c>
+      <c r="J157" s="1">
+        <v>2113000</v>
+      </c>
+      <c r="K157" s="1">
+        <f>G157-J157</f>
+        <v>0</v>
+      </c>
+      <c r="L157" s="1">
+        <f>G157-J157+H157</f>
+        <v>0</v>
+      </c>
+      <c r="M157" s="1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14">
+      <c r="C158" t="s">
+        <v>68</v>
+      </c>
+      <c r="D158" s="6">
+        <v>45443</v>
+      </c>
+      <c r="E158" s="8">
+        <v>45473</v>
+      </c>
+      <c r="F158" s="1">
+        <v>1611000</v>
+      </c>
+      <c r="G158" s="1">
+        <v>1611000</v>
+      </c>
+      <c r="H158" s="1">
+        <v>429000</v>
+      </c>
+      <c r="I158" s="1">
+        <f>G158-F158</f>
+        <v>0</v>
+      </c>
+      <c r="J158" s="1">
+        <v>2040000</v>
+      </c>
+      <c r="K158" s="1">
+        <f>G158-J158</f>
+        <v>-429000</v>
+      </c>
+      <c r="L158" s="1">
+        <f>G158-J158+H158</f>
+        <v>0</v>
+      </c>
+      <c r="M158" s="1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14">
+      <c r="B159" t="s">
+        <v>79</v>
+      </c>
+      <c r="D159" s="6">
+        <v>45457</v>
+      </c>
+      <c r="E159" s="8">
+        <v>45473</v>
+      </c>
+      <c r="F159" s="1">
+        <v>6839000</v>
+      </c>
+      <c r="G159" s="1">
+        <v>6839000</v>
+      </c>
+      <c r="H159" s="1">
+        <v>3894000</v>
+      </c>
+      <c r="I159" s="1">
+        <f>G159-F159</f>
+        <v>0</v>
+      </c>
+      <c r="J159" s="1">
+        <v>9000000</v>
+      </c>
+      <c r="K159" s="1">
+        <f>G159-J159</f>
+        <v>-2161000</v>
+      </c>
+      <c r="L159" s="1">
+        <f>G159-J159+H159</f>
+        <v>1733000</v>
+      </c>
+      <c r="M159" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="160" spans="1:14">
+      <c r="A160" s="6">
+        <v>45475</v>
+      </c>
+      <c r="B160" t="s">
+        <v>60</v>
+      </c>
+      <c r="D160" s="6">
+        <v>45448</v>
+      </c>
+      <c r="E160" s="8">
+        <v>45465</v>
+      </c>
+      <c r="F160" s="1">
+        <v>15148000</v>
+      </c>
+      <c r="G160" s="1">
+        <v>15148000</v>
+      </c>
+      <c r="H160" s="1">
+        <v>6606000</v>
+      </c>
+      <c r="I160" s="1">
+        <f>G160-F160</f>
+        <v>0</v>
+      </c>
+      <c r="J160" s="1">
+        <v>20000000</v>
+      </c>
+      <c r="K160" s="1">
+        <f>G160-J160</f>
+        <v>-4852000</v>
+      </c>
+      <c r="L160" s="1">
+        <f>G160-J160+H160</f>
+        <v>1754000</v>
+      </c>
+      <c r="M160" s="1">
+        <v>150000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update tanpa data list hutang
</commit_message>
<xml_diff>
--- a/pembayaran/Pembayaran.xlsx
+++ b/pembayaran/Pembayaran.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27904"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/277ffa1efc2bfcc1/Apartment Bintaro/Data Harian/BINTARO-APG/pembayaran/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="292" documentId="14_{1E7DE582-8E6A-4088-84FC-1A8DF5B9EF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D4F5FEA7-649E-4B2E-88FE-42879FEE7A24}"/>
+  <xr:revisionPtr revIDLastSave="481" documentId="14_{1E7DE582-8E6A-4088-84FC-1A8DF5B9EF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9538201F-2349-4DFB-B66E-5BA66FBDFEA8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="118">
   <si>
     <t>Tanggal Pembayaran</t>
   </si>
@@ -83,6 +83,9 @@
     <t>Eko</t>
   </si>
   <si>
+    <t>November</t>
+  </si>
+  <si>
     <t>Subadi</t>
   </si>
   <si>
@@ -131,6 +134,9 @@
     <t>Safety R</t>
   </si>
   <si>
+    <t>December</t>
+  </si>
+  <si>
     <t>lunas tgl 15 des 2023</t>
   </si>
   <si>
@@ -185,6 +191,9 @@
     <t>Rijam</t>
   </si>
   <si>
+    <t>January</t>
+  </si>
+  <si>
     <t>Opik</t>
   </si>
   <si>
@@ -209,6 +218,9 @@
     <t>gabung tgl  25 feb 2024</t>
   </si>
   <si>
+    <t>February</t>
+  </si>
+  <si>
     <t>Purwadi</t>
   </si>
   <si>
@@ -233,6 +245,9 @@
     <t>lunas tgl 29 mar 2024</t>
   </si>
   <si>
+    <t>Maret</t>
+  </si>
+  <si>
     <t>Nano</t>
   </si>
   <si>
@@ -284,6 +299,9 @@
     <t>lunas tgl 02 mei 2024</t>
   </si>
   <si>
+    <t>April</t>
+  </si>
+  <si>
     <t>gabung tgl 03 apr 2024</t>
   </si>
   <si>
@@ -311,6 +329,9 @@
     <t>Dede</t>
   </si>
   <si>
+    <t>May</t>
+  </si>
+  <si>
     <t>gabung tgl 18 mei 2024</t>
   </si>
   <si>
@@ -326,6 +347,9 @@
     <t>Amin</t>
   </si>
   <si>
+    <t>June</t>
+  </si>
+  <si>
     <t>30/04/2024</t>
   </si>
   <si>
@@ -335,6 +359,9 @@
     <t>lunas tgl 01 juli 2024</t>
   </si>
   <si>
+    <t>gabung  tgl 08 juli 2024</t>
+  </si>
+  <si>
     <t>Eko &amp; Sarana</t>
   </si>
   <si>
@@ -344,10 +371,25 @@
     <t>lunas tgl 26 juni 2024</t>
   </si>
   <si>
+    <t>gabung tgl 25 juni 2024</t>
+  </si>
+  <si>
+    <t>gabung tgl 08 juli 2024</t>
+  </si>
+  <si>
     <t>Ujang P</t>
   </si>
   <si>
     <t>lunas</t>
+  </si>
+  <si>
+    <t>July</t>
+  </si>
+  <si>
+    <t>Hasani</t>
+  </si>
+  <si>
+    <t>Jaenudin</t>
   </si>
 </sst>
 </file>
@@ -479,8 +521,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}" name="Table1" displayName="Table1" ref="A1:N160" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A1:N160" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}" name="Table1" displayName="Table1" ref="A1:N170" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A1:N170" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{ADAEF761-889D-4642-B4B1-5AD983017E99}" name="Tanggal Pembayaran" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{1D148A0B-5DE6-485F-ABBF-15493C92DBA8}" name="Nama Mandor"/>
@@ -824,10 +866,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P160"/>
+  <dimension ref="A1:Q170"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F125" zoomScale="110" workbookViewId="0">
-      <selection activeCell="N140" sqref="N140"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="110" workbookViewId="0">
+      <selection activeCell="E147" sqref="E147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -841,9 +883,10 @@
     <col min="13" max="13" width="17.28515625" style="1" customWidth="1"/>
     <col min="14" max="14" width="23.28515625" customWidth="1"/>
     <col min="15" max="15" width="15" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -887,7 +930,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" s="6">
         <v>45233</v>
       </c>
@@ -918,13 +961,20 @@
         <f t="shared" ref="L2:L33" si="2">G2-J2+H2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="P2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q2" s="1">
+        <f>SUM(J2:J15)</f>
+        <v>41282000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="6">
         <v>45234</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="6">
         <v>45222</v>
@@ -950,13 +1000,20 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="P3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="1">
+        <f>SUM(M2:M15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="6">
         <v>45248</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="6">
         <v>45234</v>
@@ -983,15 +1040,15 @@
         <v>5199000</v>
       </c>
       <c r="N4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="B5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D5" s="6">
         <v>45226</v>
@@ -1018,9 +1075,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:17">
       <c r="C6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D6" s="6">
         <v>45229</v>
@@ -1047,9 +1104,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:17">
       <c r="C7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="6">
         <v>45240</v>
@@ -1076,9 +1133,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:17">
       <c r="C8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" s="6">
         <v>45241</v>
@@ -1105,12 +1162,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:17">
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" s="6">
         <v>45234</v>
@@ -1137,9 +1194,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:17">
       <c r="B10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D10" s="6">
         <v>45229</v>
@@ -1166,7 +1223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:17">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -1195,15 +1252,15 @@
         <v>4000000</v>
       </c>
       <c r="N11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="B12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" s="6">
         <v>45227</v>
@@ -1234,9 +1291,9 @@
       </c>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:17">
       <c r="C13" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D13" s="6">
         <v>45225</v>
@@ -1267,9 +1324,9 @@
       </c>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:17">
       <c r="C14" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D14" s="6">
         <v>45224</v>
@@ -1297,15 +1354,15 @@
       </c>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:17">
       <c r="A15" s="6">
         <v>45252</v>
       </c>
       <c r="B15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D15" s="6">
         <v>45233</v>
@@ -1334,12 +1391,12 @@
       <c r="N15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:17">
       <c r="A16" s="6">
         <v>45261</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D16" s="6">
         <v>45247</v>
@@ -1369,8 +1426,15 @@
         <v>100000</v>
       </c>
       <c r="N16" s="1"/>
-    </row>
-    <row r="17" spans="1:14">
+      <c r="P16" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q16" s="1">
+        <f>SUM(J16:J36)</f>
+        <v>109612000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -1405,15 +1469,22 @@
         <v>100000</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+        <v>33</v>
+      </c>
+      <c r="P17" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q17" s="1">
+        <f>SUM(M16:M36)</f>
+        <v>700000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" s="6">
         <v>45273</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D18" s="6">
         <v>45248</v>
@@ -1444,10 +1515,10 @@
         <v>12624000</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" s="6">
         <v>45275</v>
       </c>
@@ -1485,12 +1556,12 @@
         <v>100000</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="B20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D20" s="6">
         <v>45261</v>
@@ -1521,12 +1592,12 @@
       </c>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:17">
       <c r="B21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D21" s="6">
         <v>45272</v>
@@ -1553,12 +1624,12 @@
         <v>163000</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="C22" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D22" s="6">
         <v>45272</v>
@@ -1574,29 +1645,29 @@
         <v>177000</v>
       </c>
       <c r="J22" s="1">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="K22" s="1">
         <f t="shared" si="1"/>
-        <v>176991</v>
+        <v>177000</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" si="2"/>
-        <v>176991</v>
+        <v>177000</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" s="6">
         <v>45277</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D23" s="6">
         <v>45253</v>
@@ -1624,12 +1695,12 @@
       </c>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:17">
       <c r="B24" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D24" s="6">
         <v>45230</v>
@@ -1657,12 +1728,12 @@
       </c>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:17">
       <c r="B25" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D25" s="6">
         <v>45256</v>
@@ -1690,9 +1761,9 @@
       </c>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:17">
       <c r="C26" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D26" s="6">
         <v>45256</v>
@@ -1720,9 +1791,9 @@
       </c>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:17">
       <c r="C27" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D27" s="6">
         <v>45258</v>
@@ -1750,9 +1821,9 @@
       </c>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:17">
       <c r="B28" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D28" s="6">
         <v>45261</v>
@@ -1785,15 +1856,15 @@
         <v>200000</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29" s="6">
         <v>45289</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D29" s="6">
         <v>45276</v>
@@ -1823,10 +1894,10 @@
         <v>14580000</v>
       </c>
       <c r="N29" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="B30" t="s">
         <v>14</v>
       </c>
@@ -1862,18 +1933,18 @@
         <v>100000</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31" s="6">
         <v>45290</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D31" s="6">
         <v>45287</v>
@@ -1901,9 +1972,9 @@
       </c>
       <c r="N31" s="1"/>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:17">
       <c r="C32" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D32" s="6">
         <v>45287</v>
@@ -1931,9 +2002,9 @@
       </c>
       <c r="N32" s="1"/>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:17">
       <c r="C33" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D33" s="6">
         <v>45287</v>
@@ -1961,9 +2032,9 @@
       </c>
       <c r="N33" s="1"/>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:17">
       <c r="C34" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D34" s="6">
         <v>45287</v>
@@ -1991,9 +2062,9 @@
       </c>
       <c r="N34" s="1"/>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:17">
       <c r="C35" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D35" s="6">
         <v>45287</v>
@@ -2021,9 +2092,9 @@
       </c>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:17">
       <c r="C36" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D36" s="6">
         <v>45287</v>
@@ -2052,7 +2123,7 @@
       <c r="N36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:17">
       <c r="A37" s="6">
         <v>45305</v>
       </c>
@@ -2091,18 +2162,25 @@
         <v>100000</v>
       </c>
       <c r="N37" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16">
+        <v>38</v>
+      </c>
+      <c r="P37" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q37" s="1">
+        <f>SUM(J37:J60)</f>
+        <v>93256000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38" s="6">
         <v>45309</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C38" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D38" s="6">
         <v>45267</v>
@@ -2129,16 +2207,23 @@
         <v>0</v>
       </c>
       <c r="N38" s="1"/>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="P38" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q38" s="1">
+        <f>SUM(M37:M60)</f>
+        <v>400000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39" s="6">
         <v>45312</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C39" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D39" s="6">
         <v>45289</v>
@@ -2166,9 +2251,9 @@
       </c>
       <c r="N39" s="1"/>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:17">
       <c r="C40" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D40" s="6">
         <v>45289</v>
@@ -2196,9 +2281,9 @@
       </c>
       <c r="N40" s="1"/>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:17">
       <c r="C41" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D41" s="6">
         <v>45289</v>
@@ -2226,9 +2311,9 @@
       </c>
       <c r="N41" s="1"/>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:17">
       <c r="C42" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D42" s="6">
         <v>45289</v>
@@ -2256,9 +2341,9 @@
       </c>
       <c r="N42" s="1"/>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:17">
       <c r="C43" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D43" s="6">
         <v>45289</v>
@@ -2286,9 +2371,9 @@
       </c>
       <c r="N43" s="1"/>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:17">
       <c r="C44" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D44" s="6">
         <v>45289</v>
@@ -2316,9 +2401,9 @@
       </c>
       <c r="N44" s="1"/>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:17">
       <c r="C45" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D45" s="6">
         <v>45289</v>
@@ -2346,9 +2431,9 @@
       </c>
       <c r="N45" s="1"/>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:17">
       <c r="C46" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D46" s="6">
         <v>45289</v>
@@ -2376,9 +2461,9 @@
       </c>
       <c r="N46" s="1"/>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:17">
       <c r="B47" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D47" s="6">
         <v>45288</v>
@@ -2412,18 +2497,18 @@
         <v>100000</v>
       </c>
       <c r="N47" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17">
       <c r="A48" s="6">
         <v>45316</v>
       </c>
       <c r="B48" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C48" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D48" s="6">
         <v>45226</v>
@@ -2451,9 +2536,9 @@
       </c>
       <c r="N48" s="1"/>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:17">
       <c r="C49" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D49" s="6">
         <v>45229</v>
@@ -2481,15 +2566,15 @@
       </c>
       <c r="N49" s="1"/>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:17">
       <c r="C50" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D50" s="6">
         <v>45230</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G50" s="1">
         <v>66000</v>
@@ -2511,15 +2596,15 @@
       </c>
       <c r="N50" s="1"/>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:17">
       <c r="C51" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D51" s="6">
         <v>45226</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G51" s="1">
         <v>1319000</v>
@@ -2541,12 +2626,12 @@
       </c>
       <c r="N51" s="1"/>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:17">
       <c r="C52" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G52" s="1">
         <v>506000</v>
@@ -2568,9 +2653,9 @@
       </c>
       <c r="N52" s="1"/>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:17">
       <c r="C53" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G53" s="1">
         <v>1589000</v>
@@ -2592,9 +2677,9 @@
       </c>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:17">
       <c r="C54" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G54" s="1">
         <v>624000</v>
@@ -2616,9 +2701,9 @@
       </c>
       <c r="N54" s="1"/>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:17">
       <c r="C55" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G55" s="1">
         <v>618000</v>
@@ -2640,7 +2725,7 @@
       </c>
       <c r="N55" s="1"/>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:17">
       <c r="A56" s="6">
         <v>45318</v>
       </c>
@@ -2680,12 +2765,12 @@
       </c>
       <c r="N56" s="1"/>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:17">
       <c r="B57" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C57" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H57" s="1">
         <v>163000</v>
@@ -2707,9 +2792,9 @@
       </c>
       <c r="N57" s="1"/>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:17">
       <c r="C58" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H58" s="1">
         <v>177000</v>
@@ -2731,15 +2816,15 @@
       </c>
       <c r="N58" s="1"/>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:17">
       <c r="A59" s="6">
         <v>45319</v>
       </c>
       <c r="B59" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C59" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D59" s="6">
         <v>45307</v>
@@ -2767,9 +2852,9 @@
       </c>
       <c r="N59" s="1"/>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:17">
       <c r="C60" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D60" s="6">
         <v>45305</v>
@@ -2798,12 +2883,12 @@
       <c r="N60" s="1"/>
       <c r="P60" s="1"/>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:17">
       <c r="A61" s="6">
         <v>45327</v>
       </c>
       <c r="B61" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D61" s="6">
         <v>45310</v>
@@ -2836,15 +2921,22 @@
         <v>100000</v>
       </c>
       <c r="N61" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="62" spans="1:16">
+        <v>59</v>
+      </c>
+      <c r="P61" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q61" s="1">
+        <f>SUM(J61:J67)</f>
+        <v>79356000</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17">
       <c r="A62" s="6">
         <v>45332</v>
       </c>
       <c r="B62" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D62" s="6">
         <v>45318</v>
@@ -2874,15 +2966,22 @@
         <v>150000</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16">
+        <v>62</v>
+      </c>
+      <c r="P62" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q62" s="1">
+        <f>SUM(M61:M67)</f>
+        <v>550000</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17">
       <c r="A63" s="6">
         <v>45339</v>
       </c>
       <c r="B63" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D63" s="6">
         <v>45298</v>
@@ -2910,12 +3009,12 @@
       </c>
       <c r="N63" s="1"/>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:17">
       <c r="B64" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C64" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D64" s="6">
         <v>45310</v>
@@ -2946,12 +3045,12 @@
       </c>
       <c r="N64" s="1"/>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:17">
       <c r="A65" s="6">
         <v>45341</v>
       </c>
       <c r="B65" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D65" s="6">
         <v>45321</v>
@@ -2978,15 +3077,15 @@
         <v>1146000</v>
       </c>
       <c r="N65" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="66" spans="1:16">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17">
       <c r="A66" s="6">
         <v>45347</v>
       </c>
       <c r="B66" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D66" s="6">
         <v>45325</v>
@@ -3019,12 +3118,12 @@
         <v>200000</v>
       </c>
       <c r="N66" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17">
       <c r="B67" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D67" s="6">
         <v>45331</v>
@@ -3060,15 +3159,15 @@
       <c r="N67" s="1"/>
       <c r="P67" s="1"/>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:17">
       <c r="A68" s="6">
         <v>45352</v>
       </c>
       <c r="B68" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C68" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D68" s="6">
         <v>45316</v>
@@ -3095,15 +3194,22 @@
         <v>50000</v>
       </c>
       <c r="N68" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="69" spans="1:16">
+        <v>68</v>
+      </c>
+      <c r="P68" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q68" s="1">
+        <f>SUM(J68:J89)</f>
+        <v>74431000</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17">
       <c r="B69" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C69" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D69" s="6">
         <v>45315</v>
@@ -3130,10 +3236,17 @@
         <v>0</v>
       </c>
       <c r="N69" s="1"/>
-    </row>
-    <row r="70" spans="1:16">
+      <c r="P69" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q69" s="1">
+        <f>SUM(M68:M89)</f>
+        <v>600000</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17">
       <c r="C70" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="D70" s="6">
         <v>45315</v>
@@ -3161,9 +3274,9 @@
       </c>
       <c r="N70" s="1"/>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:17">
       <c r="C71" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D71" s="6">
         <v>45315</v>
@@ -3191,9 +3304,9 @@
       </c>
       <c r="N71" s="1"/>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:17">
       <c r="C72" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D72" s="6">
         <v>45324</v>
@@ -3221,15 +3334,15 @@
       </c>
       <c r="N72" s="1"/>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:17">
       <c r="A73" s="6">
         <v>45354</v>
       </c>
       <c r="B73" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C73" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="D73" s="6">
         <v>45316</v>
@@ -3256,18 +3369,18 @@
         <v>35000</v>
       </c>
       <c r="N73" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17">
       <c r="A74" s="6">
         <v>45358</v>
       </c>
       <c r="B74" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C74" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="D74" s="6">
         <v>45200</v>
@@ -3298,12 +3411,12 @@
       </c>
       <c r="N74" s="1"/>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:17">
       <c r="A75" s="6">
         <v>45361</v>
       </c>
       <c r="B75" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D75" s="6">
         <v>45345</v>
@@ -3331,12 +3444,12 @@
       </c>
       <c r="N75" s="1"/>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:17">
       <c r="A76" s="6">
         <v>45362</v>
       </c>
       <c r="B76" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D76" s="6">
         <v>45345</v>
@@ -3369,18 +3482,18 @@
         <v>200000</v>
       </c>
       <c r="N76" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="77" spans="1:17">
       <c r="A77" s="6">
         <v>45366</v>
       </c>
       <c r="B77" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C77" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D77" s="6">
         <v>45359</v>
@@ -3388,13 +3501,12 @@
       <c r="E77" s="8">
         <v>45366</v>
       </c>
+      <c r="F77" s="1">
+        <v>316000</v>
+      </c>
       <c r="G77" s="1">
         <v>316000</v>
       </c>
-      <c r="I77" s="1">
-        <f t="shared" si="6"/>
-        <v>316000</v>
-      </c>
       <c r="J77" s="1">
         <v>316000</v>
       </c>
@@ -3408,9 +3520,9 @@
       </c>
       <c r="N77" s="1"/>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:17">
       <c r="C78" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="D78" s="6">
         <v>45331</v>
@@ -3442,12 +3554,12 @@
       <c r="N78" s="1"/>
       <c r="P78" s="1"/>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:17">
       <c r="A79" s="6">
         <v>45368</v>
       </c>
       <c r="B79" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D79" s="6">
         <v>45338</v>
@@ -3482,15 +3594,15 @@
       </c>
       <c r="N79" s="1"/>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:17">
       <c r="A80" s="6">
         <v>45374</v>
       </c>
       <c r="B80" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C80" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D80" s="6">
         <v>45328</v>
@@ -3521,9 +3633,9 @@
       </c>
       <c r="N80" s="1"/>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:17">
       <c r="C81" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D81" s="6">
         <v>45261</v>
@@ -3554,9 +3666,9 @@
       </c>
       <c r="N81" s="1"/>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:17">
       <c r="C82" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D82" s="6">
         <v>45331</v>
@@ -3587,9 +3699,9 @@
       </c>
       <c r="N82" s="1"/>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:17">
       <c r="B83" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D83" s="6">
         <v>45359</v>
@@ -3623,12 +3735,12 @@
       </c>
       <c r="N83" s="1"/>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:17">
       <c r="B84" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C84" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="D84" s="6">
         <v>45307</v>
@@ -3658,15 +3770,15 @@
         <v>686000</v>
       </c>
       <c r="N84" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="85" spans="1:16">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:17">
       <c r="A85" s="6">
         <v>45376</v>
       </c>
       <c r="B85" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D85" s="6">
         <v>45328</v>
@@ -3697,9 +3809,9 @@
       </c>
       <c r="N85" s="1"/>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:17">
       <c r="B86" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D86" s="6">
         <v>45323</v>
@@ -3732,18 +3844,18 @@
         <v>100000</v>
       </c>
       <c r="N86" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:17">
       <c r="A87" s="6">
         <v>45380</v>
       </c>
       <c r="B87" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C87" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D87" s="6">
         <v>45352</v>
@@ -3774,12 +3886,12 @@
       </c>
       <c r="N87" s="1"/>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:17">
       <c r="B88" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C88" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D88" s="6">
         <v>45367</v>
@@ -3788,14 +3900,14 @@
         <v>45380</v>
       </c>
       <c r="F88" s="1">
-        <v>600000</v>
+        <v>608000</v>
       </c>
       <c r="G88" s="1">
         <v>600000</v>
       </c>
       <c r="I88" s="1">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>-8000</v>
       </c>
       <c r="J88" s="1">
         <v>600000</v>
@@ -3810,9 +3922,9 @@
       </c>
       <c r="N88" s="1"/>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:17">
       <c r="C89" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D89" s="6">
         <v>45352</v>
@@ -3845,19 +3957,19 @@
         <v>11000</v>
       </c>
       <c r="N89" s="1" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="P89" s="1"/>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:17">
       <c r="A90" s="6">
         <v>45383</v>
       </c>
       <c r="B90" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C90" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="D90" s="6">
         <v>45352</v>
@@ -3887,13 +3999,20 @@
         <v>0</v>
       </c>
       <c r="N90" s="1"/>
-    </row>
-    <row r="91" spans="1:16">
+      <c r="P90" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q90" s="1">
+        <f>SUM(J90:J105)</f>
+        <v>89108000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:17">
       <c r="B91" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C91" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D91" s="6">
         <v>45351</v>
@@ -3923,10 +4042,17 @@
         <v>0</v>
       </c>
       <c r="N91" s="1"/>
-    </row>
-    <row r="92" spans="1:16">
+      <c r="P91" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q91" s="1">
+        <f>SUM(M90:M105)</f>
+        <v>250000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:17">
       <c r="C92" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D92" s="6">
         <v>45351</v>
@@ -3957,9 +4083,9 @@
       </c>
       <c r="N92" s="1"/>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:17">
       <c r="C93" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D93" s="6">
         <v>45351</v>
@@ -3990,12 +4116,12 @@
       </c>
       <c r="N93" s="1"/>
     </row>
-    <row r="94" spans="1:16">
+    <row r="94" spans="1:17">
       <c r="B94" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C94" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D94" s="6">
         <v>45231</v>
@@ -4022,12 +4148,12 @@
         <v>93000</v>
       </c>
       <c r="N94" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="95" spans="1:16">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17">
       <c r="C95" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D95" s="6">
         <v>45246</v>
@@ -4057,19 +4183,19 @@
         <v>251000</v>
       </c>
       <c r="N95" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="P95" s="1"/>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:17">
       <c r="A96" s="6">
         <v>45385</v>
       </c>
       <c r="B96" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C96" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D96" s="6">
         <v>45292</v>
@@ -4102,15 +4228,15 @@
         <v>582000</v>
       </c>
       <c r="N96" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="97" spans="1:14">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17">
       <c r="A97" s="6">
         <v>45386</v>
       </c>
       <c r="B97" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D97" s="6">
         <v>45352</v>
@@ -4140,12 +4266,12 @@
         <v>7678000</v>
       </c>
       <c r="N97" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="98" spans="1:14">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17">
       <c r="B98" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D98" s="6">
         <v>45360</v>
@@ -4181,15 +4307,15 @@
         <v>150000</v>
       </c>
       <c r="N98" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="99" spans="1:14">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17">
       <c r="A99" s="6">
         <v>45387</v>
       </c>
       <c r="B99" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D99" s="6">
         <v>45373</v>
@@ -4222,15 +4348,15 @@
         <v>100000</v>
       </c>
       <c r="N99" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="100" spans="1:14">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="100" spans="1:17">
       <c r="B100" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C100" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="D100" s="6">
         <v>45381</v>
@@ -4260,9 +4386,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:14">
+    <row r="101" spans="1:17">
       <c r="B101" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D101" s="6">
         <v>45376</v>
@@ -4295,18 +4421,18 @@
         <v>1313000</v>
       </c>
       <c r="N101" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="102" spans="1:14">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="102" spans="1:17">
       <c r="A102" s="6">
         <v>45408</v>
       </c>
       <c r="B102" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C102" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D102" s="6">
         <v>45378</v>
@@ -4339,15 +4465,15 @@
         <v>141000</v>
       </c>
       <c r="N102" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="103" spans="1:14">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="103" spans="1:17">
       <c r="A103" s="6">
         <v>45409</v>
       </c>
       <c r="B103" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D103" s="6">
         <v>45384</v>
@@ -4380,12 +4506,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:14">
+    <row r="104" spans="1:17">
       <c r="A104" s="6">
         <v>45410</v>
       </c>
       <c r="B104" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D104" s="6">
         <v>45401</v>
@@ -4415,12 +4541,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:14">
+    <row r="105" spans="1:17">
       <c r="A105" s="6">
         <v>45412</v>
       </c>
       <c r="B105" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D105" s="6">
         <v>45403</v>
@@ -4450,15 +4576,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:14">
+    <row r="106" spans="1:17">
       <c r="A106" s="6">
         <v>45413</v>
       </c>
       <c r="B106" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C106" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D106" s="6">
         <v>45383</v>
@@ -4487,10 +4613,17 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:14">
+      <c r="P106" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q106" s="1">
+        <f>SUM(J106:J124)</f>
+        <v>118948000</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17">
       <c r="C107" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D107" s="6">
         <v>45383</v>
@@ -4519,10 +4652,17 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:14">
+      <c r="P107" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q107" s="1">
+        <f>SUM(M106:M124)</f>
+        <v>1100000</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17">
       <c r="C108" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D108" s="6">
         <v>45383</v>
@@ -4552,15 +4692,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:14">
+    <row r="109" spans="1:17">
       <c r="A109" s="6">
         <v>45414</v>
       </c>
       <c r="B109" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C109" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D109" s="6">
         <v>45380</v>
@@ -4593,15 +4733,15 @@
         <v>101000</v>
       </c>
       <c r="N109" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="110" spans="1:14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="110" spans="1:17">
       <c r="A110" s="6">
         <v>45416</v>
       </c>
       <c r="B110" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D110" s="6">
         <v>45385</v>
@@ -4637,12 +4777,12 @@
         <v>200000</v>
       </c>
       <c r="N110" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="111" spans="1:14">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="111" spans="1:17">
       <c r="B111" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D111" s="6">
         <v>45387</v>
@@ -4678,15 +4818,15 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="112" spans="1:14">
+    <row r="112" spans="1:17">
       <c r="A112" s="6">
         <v>45417</v>
       </c>
       <c r="B112" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C112" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D112" s="6">
         <v>45381</v>
@@ -4716,12 +4856,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:14">
+    <row r="113" spans="1:17">
       <c r="A113" s="6">
         <v>45420</v>
       </c>
       <c r="B113" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="D113" s="6">
         <v>45399</v>
@@ -4754,12 +4894,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="114" spans="1:14">
+    <row r="114" spans="1:17">
       <c r="A114" s="6">
         <v>45424</v>
       </c>
       <c r="B114" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D114" s="6">
         <v>45404</v>
@@ -4789,12 +4929,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:14">
+    <row r="115" spans="1:17">
       <c r="A115" s="6">
         <v>45427</v>
       </c>
       <c r="B115" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D115" s="6">
         <v>45412</v>
@@ -4827,9 +4967,9 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="116" spans="1:14">
+    <row r="116" spans="1:17">
       <c r="B116" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D116" s="6">
         <v>45387</v>
@@ -4865,12 +5005,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="117" spans="1:14">
+    <row r="117" spans="1:17">
       <c r="A117" s="6">
         <v>45430</v>
       </c>
       <c r="B117" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D117" s="6">
         <v>45415</v>
@@ -4903,9 +5043,9 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="118" spans="1:14">
+    <row r="118" spans="1:17">
       <c r="B118" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D118" s="6">
         <v>45412</v>
@@ -4935,12 +5075,12 @@
         <v>3523000</v>
       </c>
       <c r="N118" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="119" spans="1:14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="119" spans="1:17">
       <c r="B119" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D119" s="6">
         <v>45413</v>
@@ -4976,15 +5116,15 @@
         <v>100000</v>
       </c>
       <c r="N119" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="120" spans="1:14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="120" spans="1:17">
       <c r="A120" s="6">
         <v>45434</v>
       </c>
       <c r="B120" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D120" s="6">
         <v>45419</v>
@@ -5017,9 +5157,9 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="121" spans="1:14">
+    <row r="121" spans="1:17">
       <c r="B121" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="D121" s="6">
         <v>45408</v>
@@ -5052,9 +5192,9 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="122" spans="1:14">
+    <row r="122" spans="1:17">
       <c r="B122" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D122" s="6">
         <v>45410</v>
@@ -5087,12 +5227,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="123" spans="1:14">
+    <row r="123" spans="1:17">
       <c r="A123" s="6">
         <v>45437</v>
       </c>
       <c r="B123" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D123" s="6">
         <v>45418</v>
@@ -5122,12 +5262,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:14">
+    <row r="124" spans="1:17">
       <c r="A124" s="6">
         <v>45443</v>
       </c>
       <c r="B124" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D124" s="6">
         <v>45423</v>
@@ -5157,12 +5297,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:14">
+    <row r="125" spans="1:17">
       <c r="A125" s="6">
         <v>45444</v>
       </c>
       <c r="B125" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D125" s="6">
         <v>45429</v>
@@ -5194,13 +5334,20 @@
       <c r="M125" s="1">
         <v>100000</v>
       </c>
-    </row>
-    <row r="126" spans="1:14">
+      <c r="P125" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q125" s="1">
+        <f>SUM(J125:J154)</f>
+        <v>158777000</v>
+      </c>
+    </row>
+    <row r="126" spans="1:17">
       <c r="B126" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C126" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D126" s="6">
         <v>45412</v>
@@ -5229,13 +5376,20 @@
         <f t="shared" si="12"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="127" spans="1:14">
+      <c r="P126" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q126" s="1">
+        <f>SUM(M125:M154)</f>
+        <v>1764000</v>
+      </c>
+    </row>
+    <row r="127" spans="1:17">
       <c r="B127" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C127" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D127" s="6">
         <v>191509</v>
@@ -5265,15 +5419,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:14">
+    <row r="128" spans="1:17">
       <c r="C128" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="F128" s="1">
         <v>2441000</v>
@@ -5299,7 +5453,7 @@
     </row>
     <row r="129" spans="1:14">
       <c r="B129" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D129" s="6">
         <v>45424</v>
@@ -5335,12 +5489,12 @@
         <v>100000</v>
       </c>
       <c r="N129" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="130" spans="1:14">
       <c r="B130" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D130" s="6">
         <v>45401</v>
@@ -5372,10 +5526,10 @@
     </row>
     <row r="131" spans="1:14">
       <c r="B131" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C131" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D131" s="6">
         <v>45412</v>
@@ -5405,12 +5559,12 @@
         <v>429000</v>
       </c>
       <c r="N131" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="132" spans="1:14">
       <c r="B132" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="D132" s="6">
         <v>45431</v>
@@ -5445,7 +5599,7 @@
         <v>45450</v>
       </c>
       <c r="B133" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="D133" s="6">
         <v>45423</v>
@@ -5480,7 +5634,7 @@
     </row>
     <row r="134" spans="1:14">
       <c r="B134" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D134" s="6">
         <v>45422</v>
@@ -5516,7 +5670,7 @@
         <v>100000</v>
       </c>
       <c r="N134" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
     </row>
     <row r="135" spans="1:14">
@@ -5524,7 +5678,7 @@
         <v>45453</v>
       </c>
       <c r="B135" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D135" s="6">
         <v>45424</v>
@@ -5562,7 +5716,7 @@
         <v>45456</v>
       </c>
       <c r="B136" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D136" s="6">
         <v>45431</v>
@@ -5597,7 +5751,7 @@
     </row>
     <row r="137" spans="1:14">
       <c r="B137" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D137" s="6">
         <v>45437</v>
@@ -5630,7 +5784,7 @@
         <v>100000</v>
       </c>
       <c r="N137" t="s">
-        <v>70</v>
+        <v>107</v>
       </c>
     </row>
     <row r="138" spans="1:14">
@@ -5638,7 +5792,7 @@
         <v>45457</v>
       </c>
       <c r="B138" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D138" s="6">
         <v>45443</v>
@@ -5673,10 +5827,10 @@
     </row>
     <row r="139" spans="1:14">
       <c r="B139" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C139" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="D139" s="6">
         <v>45231</v>
@@ -5706,7 +5860,7 @@
         <v>1014000</v>
       </c>
       <c r="N139" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
     </row>
     <row r="140" spans="1:14">
@@ -5714,7 +5868,7 @@
         <v>45458</v>
       </c>
       <c r="B140" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D140" s="6">
         <v>45416</v>
@@ -5752,7 +5906,7 @@
         <v>45459</v>
       </c>
       <c r="B141" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D141" s="6">
         <v>45443</v>
@@ -5788,7 +5942,7 @@
         <v>100000</v>
       </c>
       <c r="N141" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
     </row>
     <row r="142" spans="1:14">
@@ -5796,7 +5950,7 @@
         <v>45463</v>
       </c>
       <c r="B142" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D142" s="6">
         <v>45445</v>
@@ -5834,7 +5988,7 @@
         <v>45466</v>
       </c>
       <c r="B143" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="D143" s="6">
         <v>45437</v>
@@ -5867,12 +6021,12 @@
         <v>50000</v>
       </c>
       <c r="N143" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
     </row>
     <row r="144" spans="1:14">
       <c r="B144" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D144" s="6">
         <v>45447</v>
@@ -5902,12 +6056,12 @@
         <v>220000</v>
       </c>
       <c r="N144" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="145" spans="1:14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="145" spans="1:17">
       <c r="B145" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D145" s="6">
         <v>45438</v>
@@ -5940,12 +6094,12 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="146" spans="1:14">
+    <row r="146" spans="1:17">
       <c r="A146" s="6">
         <v>45468</v>
       </c>
       <c r="B146" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D146" s="6">
         <v>45429</v>
@@ -5981,15 +6135,15 @@
         <v>50000</v>
       </c>
       <c r="N146" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="147" spans="1:14">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="147" spans="1:17">
       <c r="A147" s="6">
         <v>45469</v>
       </c>
       <c r="B147" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D147" s="6">
         <v>45443</v>
@@ -6025,12 +6179,12 @@
         <v>150000</v>
       </c>
       <c r="N147" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="148" spans="1:14">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="148" spans="1:17">
       <c r="B148" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="D148" s="6">
         <v>45436</v>
@@ -6066,12 +6220,12 @@
         <v>150000</v>
       </c>
       <c r="N148" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="149" spans="1:14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="149" spans="1:17">
       <c r="B149" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="D149" s="6">
         <v>45437</v>
@@ -6107,15 +6261,15 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="150" spans="1:14">
+    <row r="150" spans="1:17">
       <c r="A150" s="6">
         <v>45470</v>
       </c>
       <c r="B150" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C150" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="D150" s="6">
         <v>45407</v>
@@ -6148,18 +6302,18 @@
         <v>1075000</v>
       </c>
       <c r="N150" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="151" spans="1:14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17">
       <c r="A151" s="6">
         <v>45471</v>
       </c>
       <c r="B151" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C151" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="D151" s="6">
         <v>45463</v>
@@ -6189,9 +6343,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:14">
+    <row r="152" spans="1:17">
       <c r="C152" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="D152" s="6">
         <v>45231</v>
@@ -6227,15 +6381,15 @@
         <v>14000</v>
       </c>
       <c r="N152" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="153" spans="1:14">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="153" spans="1:17">
       <c r="B153" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C153" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D153" s="6">
         <v>45385</v>
@@ -6268,15 +6422,15 @@
         <v>636000</v>
       </c>
       <c r="N153" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="154" spans="1:14">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="154" spans="1:17">
       <c r="A154" s="6">
         <v>45473</v>
       </c>
       <c r="B154" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D154" s="6">
         <v>45457</v>
@@ -6309,12 +6463,12 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="155" spans="1:14">
+    <row r="155" spans="1:17">
       <c r="A155" s="6">
         <v>45474</v>
       </c>
       <c r="B155" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="D155" s="6">
         <v>45459</v>
@@ -6346,13 +6500,20 @@
       <c r="M155" s="1">
         <v>100000</v>
       </c>
-    </row>
-    <row r="156" spans="1:14">
+      <c r="P155" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q155" s="1">
+        <f>SUM(J155:J155)</f>
+        <v>5896000</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17">
       <c r="B156" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C156" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D156" s="6">
         <v>45443</v>
@@ -6384,10 +6545,17 @@
       <c r="M156" s="1">
         <v>50000</v>
       </c>
-    </row>
-    <row r="157" spans="1:14">
+      <c r="P156" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q156" s="1">
+        <f>SUM(M155:M155)</f>
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17">
       <c r="C157" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="D157" s="6">
         <v>45443</v>
@@ -6420,9 +6588,9 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="158" spans="1:14">
+    <row r="158" spans="1:17">
       <c r="C158" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="D158" s="6">
         <v>45443</v>
@@ -6458,9 +6626,9 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="159" spans="1:14">
+    <row r="159" spans="1:17">
       <c r="B159" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D159" s="6">
         <v>45457</v>
@@ -6496,24 +6664,24 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="160" spans="1:14">
+    <row r="160" spans="1:17">
       <c r="A160" s="6">
         <v>45475</v>
       </c>
       <c r="B160" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D160" s="6">
         <v>45448</v>
       </c>
       <c r="E160" s="8">
-        <v>45465</v>
+        <v>45464</v>
       </c>
       <c r="F160" s="1">
-        <v>15148000</v>
+        <v>14382000</v>
       </c>
       <c r="G160" s="1">
-        <v>15148000</v>
+        <v>14382000</v>
       </c>
       <c r="H160" s="1">
         <v>6606000</v>
@@ -6527,14 +6695,415 @@
       </c>
       <c r="K160" s="1">
         <f>G160-J160</f>
-        <v>-4852000</v>
+        <v>-5618000</v>
       </c>
       <c r="L160" s="1">
         <f>G160-J160+H160</f>
-        <v>1754000</v>
+        <v>988000</v>
       </c>
       <c r="M160" s="1">
         <v>150000</v>
+      </c>
+    </row>
+    <row r="161" spans="1:14">
+      <c r="A161" s="6">
+        <v>45476</v>
+      </c>
+      <c r="B161" t="s">
+        <v>26</v>
+      </c>
+      <c r="C161" t="s">
+        <v>29</v>
+      </c>
+      <c r="D161" s="6">
+        <v>45311</v>
+      </c>
+      <c r="E161" s="8">
+        <v>45471</v>
+      </c>
+      <c r="F161" s="1">
+        <v>3039000</v>
+      </c>
+      <c r="G161" s="1">
+        <v>3039000</v>
+      </c>
+      <c r="H161" s="1">
+        <v>251000</v>
+      </c>
+      <c r="I161" s="1">
+        <f>G161-F161</f>
+        <v>0</v>
+      </c>
+      <c r="J161" s="1">
+        <v>200000</v>
+      </c>
+      <c r="K161" s="1">
+        <f>G161-J161</f>
+        <v>2839000</v>
+      </c>
+      <c r="L161" s="1">
+        <f>G161-J161+H161</f>
+        <v>3090000</v>
+      </c>
+      <c r="M161" s="1">
+        <v>0</v>
+      </c>
+      <c r="N161" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14">
+      <c r="C162" t="s">
+        <v>27</v>
+      </c>
+      <c r="D162" s="6">
+        <v>45471</v>
+      </c>
+      <c r="E162" s="8">
+        <v>45471</v>
+      </c>
+      <c r="F162" s="1">
+        <v>0</v>
+      </c>
+      <c r="G162" s="1">
+        <v>0</v>
+      </c>
+      <c r="H162" s="1">
+        <v>636000</v>
+      </c>
+      <c r="I162" s="1">
+        <f>G162-F162</f>
+        <v>0</v>
+      </c>
+      <c r="J162" s="1">
+        <v>200000</v>
+      </c>
+      <c r="K162" s="1">
+        <f>G162-J162</f>
+        <v>-200000</v>
+      </c>
+      <c r="L162" s="1">
+        <f>G162-J162+H162</f>
+        <v>436000</v>
+      </c>
+      <c r="M162" s="1">
+        <v>0</v>
+      </c>
+      <c r="N162" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14">
+      <c r="C163" t="s">
+        <v>28</v>
+      </c>
+      <c r="D163" s="6">
+        <v>45443</v>
+      </c>
+      <c r="E163" s="8">
+        <v>45471</v>
+      </c>
+      <c r="F163" s="1">
+        <v>572000</v>
+      </c>
+      <c r="G163" s="1">
+        <v>572000</v>
+      </c>
+      <c r="H163" s="1">
+        <v>0</v>
+      </c>
+      <c r="I163" s="1">
+        <f>G163-F163</f>
+        <v>0</v>
+      </c>
+      <c r="J163" s="1">
+        <v>572000</v>
+      </c>
+      <c r="K163" s="1">
+        <f>G163-J163</f>
+        <v>0</v>
+      </c>
+      <c r="L163" s="1">
+        <f>G163-J163+H163</f>
+        <v>0</v>
+      </c>
+      <c r="M163" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14">
+      <c r="C164" t="s">
+        <v>81</v>
+      </c>
+      <c r="D164" s="6">
+        <v>45381</v>
+      </c>
+      <c r="E164" s="8">
+        <v>45471</v>
+      </c>
+      <c r="F164" s="1">
+        <v>810000</v>
+      </c>
+      <c r="G164" s="1">
+        <v>810000</v>
+      </c>
+      <c r="H164" s="1">
+        <v>0</v>
+      </c>
+      <c r="I164" s="1">
+        <f>G164-F164</f>
+        <v>0</v>
+      </c>
+      <c r="J164" s="1">
+        <v>810000</v>
+      </c>
+      <c r="K164" s="1">
+        <f>G164-J164</f>
+        <v>0</v>
+      </c>
+      <c r="L164" s="1">
+        <f>G164-J164+H164</f>
+        <v>0</v>
+      </c>
+      <c r="M164" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14">
+      <c r="B165" t="s">
+        <v>36</v>
+      </c>
+      <c r="C165" t="s">
+        <v>67</v>
+      </c>
+      <c r="D165" s="6">
+        <v>45412</v>
+      </c>
+      <c r="E165" s="8">
+        <v>45472</v>
+      </c>
+      <c r="F165" s="1">
+        <v>1180000</v>
+      </c>
+      <c r="G165" s="1">
+        <v>1180000</v>
+      </c>
+      <c r="H165" s="1">
+        <v>101000</v>
+      </c>
+      <c r="I165" s="1">
+        <f>G165-F165</f>
+        <v>0</v>
+      </c>
+      <c r="J165" s="1">
+        <v>1081000</v>
+      </c>
+      <c r="K165" s="1">
+        <f>G165-J165</f>
+        <v>99000</v>
+      </c>
+      <c r="L165" s="1">
+        <f>G165-J165+H165</f>
+        <v>200000</v>
+      </c>
+      <c r="M165" s="1">
+        <v>50000</v>
+      </c>
+      <c r="N165" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14">
+      <c r="A166" s="6">
+        <v>45478</v>
+      </c>
+      <c r="B166" t="s">
+        <v>28</v>
+      </c>
+      <c r="C166" t="s">
+        <v>116</v>
+      </c>
+      <c r="D166" s="6">
+        <v>45465</v>
+      </c>
+      <c r="E166" s="8">
+        <v>45472</v>
+      </c>
+      <c r="F166" s="1">
+        <v>132000</v>
+      </c>
+      <c r="G166" s="1">
+        <v>132000</v>
+      </c>
+      <c r="H166" s="1">
+        <v>0</v>
+      </c>
+      <c r="I166" s="1">
+        <f>G166-F166</f>
+        <v>0</v>
+      </c>
+      <c r="J166" s="1">
+        <v>132000</v>
+      </c>
+      <c r="K166" s="1">
+        <f>G166-J166</f>
+        <v>0</v>
+      </c>
+      <c r="L166" s="1">
+        <f>G166-J166+H166</f>
+        <v>0</v>
+      </c>
+      <c r="M166" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14">
+      <c r="C167" t="s">
+        <v>117</v>
+      </c>
+      <c r="D167" s="6">
+        <v>45465</v>
+      </c>
+      <c r="E167" s="8">
+        <v>45472</v>
+      </c>
+      <c r="F167" s="1">
+        <v>136000</v>
+      </c>
+      <c r="G167" s="1">
+        <v>136000</v>
+      </c>
+      <c r="H167" s="1">
+        <v>0</v>
+      </c>
+      <c r="I167" s="1">
+        <f>G167-F167</f>
+        <v>0</v>
+      </c>
+      <c r="J167" s="1">
+        <v>136000</v>
+      </c>
+      <c r="K167" s="1">
+        <f>G167-J167</f>
+        <v>0</v>
+      </c>
+      <c r="L167" s="1">
+        <f>G167-J167+H167</f>
+        <v>0</v>
+      </c>
+      <c r="M167" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14">
+      <c r="A168" s="6">
+        <v>45479</v>
+      </c>
+      <c r="B168" t="s">
+        <v>20</v>
+      </c>
+      <c r="D168" s="6">
+        <v>45465</v>
+      </c>
+      <c r="E168" s="8">
+        <v>45477</v>
+      </c>
+      <c r="G168" s="1">
+        <v>1256000</v>
+      </c>
+      <c r="H168" s="1">
+        <v>220000</v>
+      </c>
+      <c r="I168" s="1">
+        <f>G168-F168</f>
+        <v>1256000</v>
+      </c>
+      <c r="J168" s="1">
+        <v>1256000</v>
+      </c>
+      <c r="K168" s="1">
+        <f>G168-J168</f>
+        <v>0</v>
+      </c>
+      <c r="L168" s="1">
+        <f>G168-J168+H168</f>
+        <v>220000</v>
+      </c>
+      <c r="M168" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14">
+      <c r="A169" s="6">
+        <v>45481</v>
+      </c>
+      <c r="B169" t="s">
+        <v>16</v>
+      </c>
+      <c r="F169" s="1">
+        <v>0</v>
+      </c>
+      <c r="G169" s="1">
+        <v>0</v>
+      </c>
+      <c r="H169" s="1">
+        <v>36200000</v>
+      </c>
+      <c r="I169" s="1">
+        <f>G169-F169</f>
+        <v>0</v>
+      </c>
+      <c r="J169" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="K169" s="1">
+        <f>G169-J169</f>
+        <v>-10000000</v>
+      </c>
+      <c r="L169" s="1">
+        <f>G169-J169+H169</f>
+        <v>26200000</v>
+      </c>
+      <c r="M169" s="1">
+        <v>0</v>
+      </c>
+      <c r="N169" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14">
+      <c r="B170" t="s">
+        <v>96</v>
+      </c>
+      <c r="D170" s="6">
+        <v>45453</v>
+      </c>
+      <c r="E170" s="8">
+        <v>45479</v>
+      </c>
+      <c r="H170" s="1">
+        <v>193000</v>
+      </c>
+      <c r="I170" s="1">
+        <f>G170-F170</f>
+        <v>0</v>
+      </c>
+      <c r="J170" s="1">
+        <v>18880000</v>
+      </c>
+      <c r="K170" s="1">
+        <f>G170-J170</f>
+        <v>-18880000</v>
+      </c>
+      <c r="L170" s="1">
+        <f>G170-J170+H170</f>
+        <v>-18687000</v>
+      </c>
+      <c r="M170" s="1">
+        <v>200000</v>
+      </c>
+      <c r="N170" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update 20 July 2024
</commit_message>
<xml_diff>
--- a/pembayaran/Pembayaran.xlsx
+++ b/pembayaran/Pembayaran.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/277ffa1efc2bfcc1/Apartment Bintaro/Data Harian/BINTARO-APG/pembayaran/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="513" documentId="14_{1E7DE582-8E6A-4088-84FC-1A8DF5B9EF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1664F13B-FFC1-4364-AB55-B066E361A1B4}"/>
+  <xr:revisionPtr revIDLastSave="631" documentId="14_{1E7DE582-8E6A-4088-84FC-1A8DF5B9EF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A80DF21B-F094-4167-A188-E4C189F1EE5E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="133">
   <si>
     <t>Tanggal Pembayaran</t>
   </si>
@@ -332,6 +332,9 @@
     <t>May</t>
   </si>
   <si>
+    <t>gabung tgl 03 juli 2024</t>
+  </si>
+  <si>
     <t>gabung tgl 18 mei 2024</t>
   </si>
   <si>
@@ -341,9 +344,18 @@
     <t>Fatoni</t>
   </si>
   <si>
+    <t>gabung tgl 01 juni 2024</t>
+  </si>
+  <si>
     <t>Haji Skun</t>
   </si>
   <si>
+    <t>gabung tgl 07 juni 2024</t>
+  </si>
+  <si>
+    <t>gabung tgl 25 juni 2024</t>
+  </si>
+  <si>
     <t>Amin</t>
   </si>
   <si>
@@ -356,9 +368,15 @@
     <t>30/05/2024</t>
   </si>
   <si>
+    <t>gabung tgl 16 juni 2024</t>
+  </si>
+  <si>
     <t>lunas tgl 01 juli 2024</t>
   </si>
   <si>
+    <t>salah total, ditagih tgl 23 juni 2024</t>
+  </si>
+  <si>
     <t>gabung  tgl 08 juli 2024</t>
   </si>
   <si>
@@ -368,10 +386,16 @@
     <t>lunas tgl 28 juni 2024</t>
   </si>
   <si>
+    <t>gabunt tgl 2 juli 2024</t>
+  </si>
+  <si>
+    <t>gabung tgl 1 juli 2024</t>
+  </si>
+  <si>
     <t>lunas tgl 26 juni 2024</t>
   </si>
   <si>
-    <t>gabung tgl 25 juni 2024</t>
+    <t>gabung tgl 06 juli 2024</t>
   </si>
   <si>
     <t>gabung tgl 08 juli 2024</t>
@@ -386,10 +410,31 @@
     <t>July</t>
   </si>
   <si>
+    <t>termasuk tgl 1 juli</t>
+  </si>
+  <si>
+    <t>tesmasuk tgl 1 juli</t>
+  </si>
+  <si>
+    <t>gabung tgl 16 juli 2024</t>
+  </si>
+  <si>
     <t>Hasani</t>
   </si>
   <si>
     <t>Jaenudin</t>
+  </si>
+  <si>
+    <t>gabung 21 juli 2024</t>
+  </si>
+  <si>
+    <t>gabung tgl 13 juli 2024</t>
+  </si>
+  <si>
+    <t>gabung tgl 21 juli 2024</t>
+  </si>
+  <si>
+    <t>gabung tgl 15 juli 2024</t>
   </si>
 </sst>
 </file>
@@ -521,8 +566,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}" name="Table1" displayName="Table1" ref="A1:N173" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A1:N173" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}" name="Table1" displayName="Table1" ref="A1:N181" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A1:N181" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{ADAEF761-889D-4642-B4B1-5AD983017E99}" name="Tanggal Pembayaran" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{1D148A0B-5DE6-485F-ABBF-15493C92DBA8}" name="Nama Mandor"/>
@@ -866,10 +911,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q173"/>
+  <dimension ref="A1:Q181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" zoomScale="110" workbookViewId="0">
-      <selection activeCell="N174" sqref="N174"/>
+    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="110" workbookViewId="0">
+      <selection activeCell="E152" sqref="E152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4733,7 +4778,7 @@
         <v>101000</v>
       </c>
       <c r="N109" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
     </row>
     <row r="110" spans="1:17">
@@ -4777,7 +4822,7 @@
         <v>200000</v>
       </c>
       <c r="N110" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="111" spans="1:17">
@@ -4861,7 +4906,7 @@
         <v>45420</v>
       </c>
       <c r="B113" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D113" s="6">
         <v>45399</v>
@@ -4899,7 +4944,7 @@
         <v>45424</v>
       </c>
       <c r="B114" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D114" s="6">
         <v>45404</v>
@@ -5004,6 +5049,9 @@
       <c r="M116" s="1">
         <v>100000</v>
       </c>
+      <c r="N116" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="117" spans="1:17">
       <c r="A117" s="6">
@@ -5045,7 +5093,7 @@
     </row>
     <row r="118" spans="1:17">
       <c r="B118" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D118" s="6">
         <v>45412</v>
@@ -5075,7 +5123,7 @@
         <v>3523000</v>
       </c>
       <c r="N118" t="s">
-        <v>75</v>
+        <v>104</v>
       </c>
     </row>
     <row r="119" spans="1:17">
@@ -5116,7 +5164,7 @@
         <v>100000</v>
       </c>
       <c r="N119" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
     </row>
     <row r="120" spans="1:17">
@@ -5124,7 +5172,7 @@
         <v>45434</v>
       </c>
       <c r="B120" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D120" s="6">
         <v>45419</v>
@@ -5159,7 +5207,7 @@
     </row>
     <row r="121" spans="1:17">
       <c r="B121" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D121" s="6">
         <v>45408</v>
@@ -5232,7 +5280,7 @@
         <v>45437</v>
       </c>
       <c r="B123" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D123" s="6">
         <v>45418</v>
@@ -5335,7 +5383,7 @@
         <v>100000</v>
       </c>
       <c r="P125" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="Q125" s="1">
         <f>SUM(J125:J154)</f>
@@ -5424,10 +5472,10 @@
         <v>70</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="E128" s="8" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="F128" s="1">
         <v>2441000</v>
@@ -5489,7 +5537,7 @@
         <v>100000</v>
       </c>
       <c r="N129" t="s">
-        <v>75</v>
+        <v>110</v>
       </c>
     </row>
     <row r="130" spans="1:14">
@@ -5559,12 +5607,12 @@
         <v>429000</v>
       </c>
       <c r="N131" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
     </row>
     <row r="132" spans="1:14">
       <c r="B132" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D132" s="6">
         <v>45431</v>
@@ -5599,7 +5647,7 @@
         <v>45450</v>
       </c>
       <c r="B133" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D133" s="6">
         <v>45423</v>
@@ -5631,10 +5679,13 @@
       <c r="M133" s="1">
         <v>100000</v>
       </c>
+      <c r="N133" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="134" spans="1:14">
       <c r="B134" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D134" s="6">
         <v>45422</v>
@@ -5716,7 +5767,7 @@
         <v>45456</v>
       </c>
       <c r="B136" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D136" s="6">
         <v>45431</v>
@@ -5784,7 +5835,7 @@
         <v>100000</v>
       </c>
       <c r="N137" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
     </row>
     <row r="138" spans="1:14">
@@ -5830,7 +5881,7 @@
         <v>30</v>
       </c>
       <c r="C139" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="D139" s="6">
         <v>45231</v>
@@ -5860,7 +5911,7 @@
         <v>1014000</v>
       </c>
       <c r="N139" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="140" spans="1:14">
@@ -5900,6 +5951,9 @@
       <c r="M140" s="1">
         <v>200000</v>
       </c>
+      <c r="N140" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="141" spans="1:14">
       <c r="A141" s="6">
@@ -5942,7 +5996,7 @@
         <v>100000</v>
       </c>
       <c r="N141" t="s">
-        <v>75</v>
+        <v>117</v>
       </c>
     </row>
     <row r="142" spans="1:14">
@@ -5950,7 +6004,7 @@
         <v>45463</v>
       </c>
       <c r="B142" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D142" s="6">
         <v>45445</v>
@@ -5988,7 +6042,7 @@
         <v>45466</v>
       </c>
       <c r="B143" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D143" s="6">
         <v>45437</v>
@@ -6021,7 +6075,7 @@
         <v>50000</v>
       </c>
       <c r="N143" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="144" spans="1:14">
@@ -6056,7 +6110,7 @@
         <v>220000</v>
       </c>
       <c r="N144" t="s">
-        <v>75</v>
+        <v>119</v>
       </c>
     </row>
     <row r="145" spans="1:17">
@@ -6135,7 +6189,7 @@
         <v>50000</v>
       </c>
       <c r="N146" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="147" spans="1:17">
@@ -6179,12 +6233,12 @@
         <v>150000</v>
       </c>
       <c r="N147" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="148" spans="1:17">
       <c r="B148" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D148" s="6">
         <v>45436</v>
@@ -6225,10 +6279,10 @@
     </row>
     <row r="149" spans="1:17">
       <c r="B149" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D149" s="6">
-        <v>45437</v>
+        <v>45451</v>
       </c>
       <c r="E149" s="8">
         <v>45451</v>
@@ -6313,13 +6367,13 @@
         <v>30</v>
       </c>
       <c r="C151" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="D151" s="6">
         <v>45463</v>
       </c>
       <c r="E151" s="8">
-        <v>45470</v>
+        <v>45472</v>
       </c>
       <c r="F151" s="1">
         <v>314000</v>
@@ -6345,7 +6399,7 @@
     </row>
     <row r="152" spans="1:17">
       <c r="C152" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="D152" s="6">
         <v>45231</v>
@@ -6381,7 +6435,7 @@
         <v>14000</v>
       </c>
       <c r="N152" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="153" spans="1:17">
@@ -6468,7 +6522,7 @@
         <v>45474</v>
       </c>
       <c r="B155" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D155" s="6">
         <v>45459</v>
@@ -6501,7 +6555,7 @@
         <v>100000</v>
       </c>
       <c r="P155" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="Q155" s="1">
         <f>SUM(J155:J155)</f>
@@ -6545,6 +6599,9 @@
       <c r="M156" s="1">
         <v>50000</v>
       </c>
+      <c r="N156" t="s">
+        <v>124</v>
+      </c>
       <c r="P156" t="s">
         <v>12</v>
       </c>
@@ -6587,6 +6644,9 @@
       <c r="M157" s="1">
         <v>50000</v>
       </c>
+      <c r="N157" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="158" spans="1:17">
       <c r="C158" t="s">
@@ -6663,6 +6723,9 @@
       <c r="M159" s="1">
         <v>100000</v>
       </c>
+      <c r="N159" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="160" spans="1:17">
       <c r="A160" s="6">
@@ -6675,13 +6738,13 @@
         <v>45448</v>
       </c>
       <c r="E160" s="8">
-        <v>45464</v>
+        <v>45465</v>
       </c>
       <c r="F160" s="1">
-        <v>14382000</v>
+        <v>15148000</v>
       </c>
       <c r="G160" s="1">
-        <v>14382000</v>
+        <v>15148000</v>
       </c>
       <c r="H160" s="1">
         <v>6606000</v>
@@ -6695,14 +6758,17 @@
       </c>
       <c r="K160" s="1">
         <f>G160-J160</f>
-        <v>-5618000</v>
+        <v>-4852000</v>
       </c>
       <c r="L160" s="1">
         <f>G160-J160+H160</f>
-        <v>988000</v>
+        <v>1754000</v>
       </c>
       <c r="M160" s="1">
         <v>150000</v>
+      </c>
+      <c r="N160" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="161" spans="1:14">
@@ -6921,7 +6987,7 @@
         <v>28</v>
       </c>
       <c r="C166" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="D166" s="6">
         <v>45465</v>
@@ -6959,7 +7025,7 @@
     </row>
     <row r="167" spans="1:14">
       <c r="C167" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="D167" s="6">
         <v>45465</v>
@@ -7035,6 +7101,9 @@
       <c r="M168" s="1">
         <v>0</v>
       </c>
+      <c r="N168" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="169" spans="1:14">
       <c r="A169" s="6">
@@ -7077,7 +7146,7 @@
         <v>0</v>
       </c>
       <c r="N169" t="s">
-        <v>75</v>
+        <v>130</v>
       </c>
     </row>
     <row r="170" spans="1:14">
@@ -7118,7 +7187,7 @@
         <v>200000</v>
       </c>
       <c r="N170" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
     </row>
     <row r="171" spans="1:14">
@@ -7161,7 +7230,7 @@
     </row>
     <row r="172" spans="1:14">
       <c r="B172" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D172" s="6">
         <v>45452</v>
@@ -7196,7 +7265,7 @@
     </row>
     <row r="173" spans="1:14">
       <c r="B173" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="D173" s="6">
         <v>45457</v>
@@ -7225,7 +7294,347 @@
         <f>G173-J173+H173</f>
         <v>565000</v>
       </c>
+      <c r="M173" s="1">
+        <v>0</v>
+      </c>
       <c r="N173" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14">
+      <c r="A174" s="6">
+        <v>45486</v>
+      </c>
+      <c r="B174" t="s">
+        <v>16</v>
+      </c>
+      <c r="D174" s="6">
+        <v>45467</v>
+      </c>
+      <c r="E174" s="8">
+        <v>45467</v>
+      </c>
+      <c r="F174" s="1">
+        <v>0</v>
+      </c>
+      <c r="G174" s="1">
+        <v>0</v>
+      </c>
+      <c r="H174" s="1">
+        <v>26200000</v>
+      </c>
+      <c r="I174" s="1">
+        <f>G174-F174</f>
+        <v>0</v>
+      </c>
+      <c r="J174" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="K174" s="1">
+        <f>G174-J174</f>
+        <v>-10000000</v>
+      </c>
+      <c r="L174" s="1">
+        <f>G174-J174+H174</f>
+        <v>16200000</v>
+      </c>
+      <c r="M174" s="1">
+        <v>0</v>
+      </c>
+      <c r="N174" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14">
+      <c r="B175" t="s">
+        <v>106</v>
+      </c>
+      <c r="D175" s="6">
+        <v>45443</v>
+      </c>
+      <c r="E175" s="8">
+        <v>45456</v>
+      </c>
+      <c r="F175" s="1">
+        <v>2675000</v>
+      </c>
+      <c r="G175" s="1">
+        <v>2675000</v>
+      </c>
+      <c r="H175" s="1">
+        <v>565000</v>
+      </c>
+      <c r="I175" s="1">
+        <f>G175-F175</f>
+        <v>0</v>
+      </c>
+      <c r="J175" s="1">
+        <v>2675000</v>
+      </c>
+      <c r="K175" s="1">
+        <f>G175-J175</f>
+        <v>0</v>
+      </c>
+      <c r="L175" s="1">
+        <f>G175-J175+H175</f>
+        <v>565000</v>
+      </c>
+      <c r="M175" s="1">
+        <v>100000</v>
+      </c>
+      <c r="N175" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14">
+      <c r="A176" s="6">
+        <v>45488</v>
+      </c>
+      <c r="B176" t="s">
+        <v>16</v>
+      </c>
+      <c r="D176" s="6">
+        <v>45468</v>
+      </c>
+      <c r="E176" s="8">
+        <v>45485</v>
+      </c>
+      <c r="F176" s="1">
+        <v>2992000</v>
+      </c>
+      <c r="G176" s="1">
+        <v>2992000</v>
+      </c>
+      <c r="H176" s="1">
+        <v>16200000</v>
+      </c>
+      <c r="I176" s="1">
+        <f>G176-F176</f>
+        <v>0</v>
+      </c>
+      <c r="J176" s="1">
+        <v>2565000</v>
+      </c>
+      <c r="K176" s="1">
+        <f>G176-J176</f>
+        <v>427000</v>
+      </c>
+      <c r="L176" s="1">
+        <f>G176-J176+H176</f>
+        <v>16627000</v>
+      </c>
+      <c r="M176" s="1">
+        <v>45000</v>
+      </c>
+      <c r="N176" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="177" spans="1:14">
+      <c r="B177" t="s">
+        <v>101</v>
+      </c>
+      <c r="D177" s="6">
+        <v>45473</v>
+      </c>
+      <c r="E177" s="8">
+        <v>45486</v>
+      </c>
+      <c r="F177" s="1">
+        <v>6732000</v>
+      </c>
+      <c r="G177" s="1">
+        <v>6732000</v>
+      </c>
+      <c r="H177" s="1">
+        <v>0</v>
+      </c>
+      <c r="I177" s="1">
+        <f>G177-F177</f>
+        <v>0</v>
+      </c>
+      <c r="J177" s="1">
+        <v>6031000</v>
+      </c>
+      <c r="K177" s="1">
+        <f>G177-J177</f>
+        <v>701000</v>
+      </c>
+      <c r="L177" s="1">
+        <f>G177-J177+H177</f>
+        <v>701000</v>
+      </c>
+      <c r="M177" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="178" spans="1:14">
+      <c r="A178" s="6">
+        <v>45489</v>
+      </c>
+      <c r="B178" t="s">
+        <v>84</v>
+      </c>
+      <c r="D178" s="6">
+        <v>45474</v>
+      </c>
+      <c r="E178" s="8">
+        <v>45487</v>
+      </c>
+      <c r="F178" s="1">
+        <v>5359000</v>
+      </c>
+      <c r="G178" s="1">
+        <v>5359000</v>
+      </c>
+      <c r="H178" s="1">
+        <v>1733000</v>
+      </c>
+      <c r="I178" s="1">
+        <f>G178-F178</f>
+        <v>0</v>
+      </c>
+      <c r="J178" s="1">
+        <v>6500000</v>
+      </c>
+      <c r="K178" s="1">
+        <f>G178-J178</f>
+        <v>-1141000</v>
+      </c>
+      <c r="L178" s="1">
+        <f>G178-J178+H178</f>
+        <v>592000</v>
+      </c>
+      <c r="M178" s="1">
+        <v>100000</v>
+      </c>
+      <c r="N178" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="179" spans="1:14">
+      <c r="B179" t="s">
+        <v>64</v>
+      </c>
+      <c r="D179" s="6">
+        <v>45466</v>
+      </c>
+      <c r="E179" s="8">
+        <v>45478</v>
+      </c>
+      <c r="F179" s="1">
+        <v>13163000</v>
+      </c>
+      <c r="G179" s="1">
+        <v>13163000</v>
+      </c>
+      <c r="H179" s="1">
+        <v>1754000</v>
+      </c>
+      <c r="I179" s="1">
+        <f>G179-F179</f>
+        <v>0</v>
+      </c>
+      <c r="J179" s="1">
+        <v>14917000</v>
+      </c>
+      <c r="K179" s="1">
+        <f>G179-J179</f>
+        <v>-1754000</v>
+      </c>
+      <c r="L179" s="1">
+        <f>G179-J179+H179</f>
+        <v>0</v>
+      </c>
+      <c r="M179" s="1">
+        <v>100000</v>
+      </c>
+      <c r="N179" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="180" spans="1:14">
+      <c r="A180" s="6">
+        <v>45494</v>
+      </c>
+      <c r="B180" t="s">
+        <v>96</v>
+      </c>
+      <c r="D180" s="6">
+        <v>45480</v>
+      </c>
+      <c r="E180" s="8">
+        <v>45492</v>
+      </c>
+      <c r="F180" s="1">
+        <v>12105000</v>
+      </c>
+      <c r="G180" s="1">
+        <v>12105000</v>
+      </c>
+      <c r="H180" s="1">
+        <v>68000</v>
+      </c>
+      <c r="I180" s="1">
+        <f>G180-F180</f>
+        <v>0</v>
+      </c>
+      <c r="J180" s="1">
+        <v>12105000</v>
+      </c>
+      <c r="K180" s="1">
+        <f>G180-J180</f>
+        <v>0</v>
+      </c>
+      <c r="L180" s="1">
+        <f>G180-J180+H180</f>
+        <v>68000</v>
+      </c>
+      <c r="M180" s="1">
+        <v>100000</v>
+      </c>
+      <c r="N180" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="181" spans="1:14">
+      <c r="B181" t="s">
+        <v>20</v>
+      </c>
+      <c r="D181" s="6">
+        <v>45478</v>
+      </c>
+      <c r="E181" s="8">
+        <v>45492</v>
+      </c>
+      <c r="F181" s="1">
+        <v>2916000</v>
+      </c>
+      <c r="G181" s="1">
+        <v>2916000</v>
+      </c>
+      <c r="H181" s="1">
+        <v>220000</v>
+      </c>
+      <c r="I181" s="1">
+        <f>G181-F181</f>
+        <v>0</v>
+      </c>
+      <c r="J181" s="1">
+        <v>2916000</v>
+      </c>
+      <c r="K181" s="1">
+        <f>G181-J181</f>
+        <v>0</v>
+      </c>
+      <c r="L181" s="1">
+        <f>G181-J181+H181</f>
+        <v>220000</v>
+      </c>
+      <c r="M181" s="1">
+        <v>100000</v>
+      </c>
+      <c r="N181" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update 25 July 2024
</commit_message>
<xml_diff>
--- a/pembayaran/Pembayaran.xlsx
+++ b/pembayaran/Pembayaran.xlsx
@@ -913,8 +913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" zoomScale="110" workbookViewId="0">
-      <selection activeCell="E152" sqref="E152"/>
+    <sheetView tabSelected="1" topLeftCell="A143" zoomScale="110" workbookViewId="0">
+      <selection activeCell="B178" sqref="B178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
update list hutang 12 agustus
</commit_message>
<xml_diff>
--- a/pembayaran/Pembayaran.xlsx
+++ b/pembayaran/Pembayaran.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/277ffa1efc2bfcc1/Apartment Bintaro/Data Harian/BINTARO-APG/pembayaran/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="714" documentId="14_{1E7DE582-8E6A-4088-84FC-1A8DF5B9EF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A921AD26-C823-4D53-86DB-230F1B83E0F6}"/>
+  <xr:revisionPtr revIDLastSave="715" documentId="14_{1E7DE582-8E6A-4088-84FC-1A8DF5B9EF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B703E1D0-A30F-4F67-B09D-5E6E51AF4025}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="9030" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -929,8 +929,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A174" zoomScale="110" workbookViewId="0">
-      <selection activeCell="G202" sqref="G202"/>
+    <sheetView tabSelected="1" topLeftCell="A176" zoomScale="110" workbookViewId="0">
+      <selection activeCell="H197" sqref="H197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8229,7 +8229,7 @@
         <v>10323000</v>
       </c>
       <c r="H196" s="1">
-        <v>565000</v>
+        <v>222000</v>
       </c>
       <c r="I196" s="1">
         <f>G196-F196</f>
@@ -8244,7 +8244,7 @@
       </c>
       <c r="L196" s="1">
         <f>G196-J196+H196</f>
-        <v>5888000</v>
+        <v>5545000</v>
       </c>
       <c r="M196" s="1">
         <v>50000</v>

</xml_diff>

<commit_message>
update 26 agustus 2024
</commit_message>
<xml_diff>
--- a/pembayaran/Pembayaran.xlsx
+++ b/pembayaran/Pembayaran.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28019"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28020"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/277ffa1efc2bfcc1/Apartment Bintaro/Data Harian/BINTARO-APG/pembayaran/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="749" documentId="14_{1E7DE582-8E6A-4088-84FC-1A8DF5B9EF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F8D79AD-C19E-4358-BA86-AB0B43F48DF3}"/>
+  <xr:revisionPtr revIDLastSave="867" documentId="14_{1E7DE582-8E6A-4088-84FC-1A8DF5B9EF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15395474-CE5B-4AC5-ADB2-F3831331AC12}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="9030" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="143">
   <si>
     <t>Tanggal Pembayaran</t>
   </si>
@@ -452,16 +452,19 @@
     <t>Sunar</t>
   </si>
   <si>
-    <t>8/17/2024</t>
-  </si>
-  <si>
     <t>E'es</t>
   </si>
   <si>
-    <t>8/19/2024</t>
-  </si>
-  <si>
-    <t>8/21/2024</t>
+    <t>Wanto</t>
+  </si>
+  <si>
+    <t>Indra</t>
+  </si>
+  <si>
+    <t>gabung tgl 27 agustus 2024</t>
+  </si>
+  <si>
+    <t>Rudi</t>
   </si>
 </sst>
 </file>
@@ -597,8 +600,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}" name="Table1" displayName="Table1" ref="A1:N206" totalsRowShown="0" headerRowDxfId="11">
-  <autoFilter ref="A1:N206" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}" name="Table1" displayName="Table1" ref="A1:N217" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="A1:N217" xr:uid="{20A85D36-285B-4CAB-A76B-A1422EA21A9B}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{ADAEF761-889D-4642-B4B1-5AD983017E99}" name="Tanggal Pembayaran" dataDxfId="10"/>
     <tableColumn id="2" xr3:uid="{1D148A0B-5DE6-485F-ABBF-15493C92DBA8}" name="Nama Mandor"/>
@@ -942,10 +945,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q206"/>
+  <dimension ref="A1:Q217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A190" zoomScale="110" workbookViewId="0">
-      <selection activeCell="F198" sqref="F198"/>
+    <sheetView tabSelected="1" topLeftCell="A194" zoomScale="110" workbookViewId="0">
+      <selection activeCell="I207" sqref="I207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8544,11 +8547,11 @@
       </c>
     </row>
     <row r="204" spans="1:14">
-      <c r="A204" s="9" t="s">
+      <c r="A204" s="9">
+        <v>45521</v>
+      </c>
+      <c r="B204" t="s">
         <v>138</v>
-      </c>
-      <c r="B204" t="s">
-        <v>139</v>
       </c>
       <c r="D204" s="9">
         <v>45467</v>
@@ -8585,8 +8588,8 @@
       </c>
     </row>
     <row r="205" spans="1:14">
-      <c r="A205" s="9" t="s">
-        <v>140</v>
+      <c r="A205" s="9">
+        <v>45523</v>
       </c>
       <c r="B205" t="s">
         <v>135</v>
@@ -8623,8 +8626,8 @@
       </c>
     </row>
     <row r="206" spans="1:14">
-      <c r="A206" s="9" t="s">
-        <v>141</v>
+      <c r="A206" s="9">
+        <v>45525</v>
       </c>
       <c r="B206" t="s">
         <v>106</v>
@@ -8664,6 +8667,440 @@
       </c>
       <c r="N206" t="s">
         <v>75</v>
+      </c>
+    </row>
+    <row r="207" spans="1:14">
+      <c r="A207" s="9">
+        <v>45526</v>
+      </c>
+      <c r="B207" t="s">
+        <v>96</v>
+      </c>
+      <c r="D207" s="9">
+        <v>45507</v>
+      </c>
+      <c r="E207" s="8">
+        <v>45520</v>
+      </c>
+      <c r="F207" s="1">
+        <v>9335000</v>
+      </c>
+      <c r="G207" s="1">
+        <v>9085000</v>
+      </c>
+      <c r="H207" s="1">
+        <v>0</v>
+      </c>
+      <c r="I207" s="1">
+        <f>G207-F207</f>
+        <v>-250000</v>
+      </c>
+      <c r="J207" s="1">
+        <v>9085000</v>
+      </c>
+      <c r="K207" s="1">
+        <f>G207-J207</f>
+        <v>0</v>
+      </c>
+      <c r="L207" s="1">
+        <f>G207-J207+H207</f>
+        <v>0</v>
+      </c>
+      <c r="M207" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="208" spans="1:14">
+      <c r="A208" s="9">
+        <v>45527</v>
+      </c>
+      <c r="B208" t="s">
+        <v>16</v>
+      </c>
+      <c r="D208" s="9">
+        <v>45486</v>
+      </c>
+      <c r="E208" s="8">
+        <v>45505</v>
+      </c>
+      <c r="F208" s="1">
+        <v>0</v>
+      </c>
+      <c r="G208" s="1">
+        <v>0</v>
+      </c>
+      <c r="H208" s="1">
+        <v>16627000</v>
+      </c>
+      <c r="I208" s="1">
+        <f>G208-F208</f>
+        <v>0</v>
+      </c>
+      <c r="J208" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="K208" s="1">
+        <f>G208-J208</f>
+        <v>-10000000</v>
+      </c>
+      <c r="L208" s="1">
+        <f>G208-J208+H208</f>
+        <v>6627000</v>
+      </c>
+      <c r="N208" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="209" spans="1:14">
+      <c r="A209" s="9"/>
+      <c r="B209" t="s">
+        <v>101</v>
+      </c>
+      <c r="D209" s="9">
+        <v>45501</v>
+      </c>
+      <c r="E209" s="8">
+        <v>45519</v>
+      </c>
+      <c r="F209" s="1">
+        <v>10977000</v>
+      </c>
+      <c r="G209" s="1">
+        <v>10977000</v>
+      </c>
+      <c r="I209" s="1">
+        <f>G209-F209</f>
+        <v>0</v>
+      </c>
+      <c r="J209" s="1">
+        <v>10977000</v>
+      </c>
+      <c r="K209" s="1">
+        <f>G209-J209</f>
+        <v>0</v>
+      </c>
+      <c r="L209" s="1">
+        <f>G209-J209+H209</f>
+        <v>0</v>
+      </c>
+      <c r="M209" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="210" spans="1:14">
+      <c r="A210" s="9">
+        <v>45528</v>
+      </c>
+      <c r="B210" t="s">
+        <v>30</v>
+      </c>
+      <c r="C210" t="s">
+        <v>139</v>
+      </c>
+      <c r="D210" s="9">
+        <v>45509</v>
+      </c>
+      <c r="E210" s="8">
+        <v>45514</v>
+      </c>
+      <c r="F210" s="1">
+        <v>72000</v>
+      </c>
+      <c r="G210" s="1">
+        <v>72000</v>
+      </c>
+      <c r="I210" s="1">
+        <f>G210-F210</f>
+        <v>0</v>
+      </c>
+      <c r="J210" s="1">
+        <v>72000</v>
+      </c>
+      <c r="K210" s="1">
+        <f>G210-J210</f>
+        <v>0</v>
+      </c>
+      <c r="L210" s="1">
+        <f>G210-J210+H210</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:14">
+      <c r="A211" s="9">
+        <v>45529</v>
+      </c>
+      <c r="B211" t="s">
+        <v>140</v>
+      </c>
+      <c r="D211" s="9">
+        <v>45509</v>
+      </c>
+      <c r="E211" s="8">
+        <v>45524</v>
+      </c>
+      <c r="F211" s="1">
+        <v>4863000</v>
+      </c>
+      <c r="G211" s="1">
+        <v>4863000</v>
+      </c>
+      <c r="I211" s="1">
+        <f>G211-F211</f>
+        <v>0</v>
+      </c>
+      <c r="J211" s="1">
+        <v>3615000</v>
+      </c>
+      <c r="K211" s="1">
+        <f>G211-J211</f>
+        <v>1248000</v>
+      </c>
+      <c r="L211" s="1">
+        <f>G211-J211+H211</f>
+        <v>1248000</v>
+      </c>
+      <c r="M211" s="1">
+        <v>100000</v>
+      </c>
+      <c r="N211" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="212" spans="1:14">
+      <c r="A212" s="9">
+        <v>45530</v>
+      </c>
+      <c r="B212" t="s">
+        <v>142</v>
+      </c>
+      <c r="D212" s="9">
+        <v>45506</v>
+      </c>
+      <c r="E212" s="8">
+        <v>45525</v>
+      </c>
+      <c r="F212" s="1">
+        <v>880000</v>
+      </c>
+      <c r="G212" s="1">
+        <v>880000</v>
+      </c>
+      <c r="I212" s="1">
+        <f>G212-F212</f>
+        <v>0</v>
+      </c>
+      <c r="J212" s="1">
+        <v>475000</v>
+      </c>
+      <c r="K212" s="1">
+        <f>G212-J212</f>
+        <v>405000</v>
+      </c>
+      <c r="L212" s="1">
+        <f>G212-J212+H212</f>
+        <v>405000</v>
+      </c>
+      <c r="N212" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="213" spans="1:14">
+      <c r="A213" s="9">
+        <v>45531</v>
+      </c>
+      <c r="B213" t="s">
+        <v>140</v>
+      </c>
+      <c r="D213" s="9">
+        <v>45509</v>
+      </c>
+      <c r="E213" s="8">
+        <v>45524</v>
+      </c>
+      <c r="F213" s="1">
+        <v>0</v>
+      </c>
+      <c r="G213" s="1">
+        <v>0</v>
+      </c>
+      <c r="H213" s="1">
+        <v>1248000</v>
+      </c>
+      <c r="I213" s="1">
+        <f>G213-F213</f>
+        <v>0</v>
+      </c>
+      <c r="J213" s="1">
+        <v>1248000</v>
+      </c>
+      <c r="K213" s="1">
+        <f>G213-J213</f>
+        <v>-1248000</v>
+      </c>
+      <c r="L213" s="1">
+        <f>G213-J213+H213</f>
+        <v>0</v>
+      </c>
+      <c r="N213" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="214" spans="1:14">
+      <c r="A214" s="9">
+        <v>45532</v>
+      </c>
+      <c r="B214" t="s">
+        <v>103</v>
+      </c>
+      <c r="D214" s="9">
+        <v>45492</v>
+      </c>
+      <c r="E214" s="8">
+        <v>45505</v>
+      </c>
+      <c r="F214" s="1">
+        <v>10890000</v>
+      </c>
+      <c r="G214" s="1">
+        <v>12924000</v>
+      </c>
+      <c r="H214" s="1">
+        <v>7500000</v>
+      </c>
+      <c r="I214" s="1">
+        <f>G214-F214</f>
+        <v>2034000</v>
+      </c>
+      <c r="J214" s="1">
+        <v>15000000</v>
+      </c>
+      <c r="K214" s="1">
+        <f>G214-J214</f>
+        <v>-2076000</v>
+      </c>
+      <c r="L214" s="1">
+        <f>G214-J214+H214</f>
+        <v>5424000</v>
+      </c>
+      <c r="M214" s="1">
+        <v>150000</v>
+      </c>
+      <c r="N214" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="215" spans="1:14">
+      <c r="A215" s="9"/>
+      <c r="B215" t="s">
+        <v>138</v>
+      </c>
+      <c r="D215" s="9">
+        <v>45500</v>
+      </c>
+      <c r="E215" s="8">
+        <v>45530</v>
+      </c>
+      <c r="F215" s="1">
+        <v>6207000</v>
+      </c>
+      <c r="G215" s="1">
+        <v>6207000</v>
+      </c>
+      <c r="H215" s="1">
+        <v>23942000</v>
+      </c>
+      <c r="I215" s="1">
+        <f>G215-F215</f>
+        <v>0</v>
+      </c>
+      <c r="J215" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="K215" s="1">
+        <f>G215-J215</f>
+        <v>-3793000</v>
+      </c>
+      <c r="L215" s="1">
+        <f>G215-J215+H215</f>
+        <v>20149000</v>
+      </c>
+      <c r="M215" s="1">
+        <v>100000</v>
+      </c>
+      <c r="N215" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="216" spans="1:14">
+      <c r="A216" s="9"/>
+      <c r="B216" t="s">
+        <v>26</v>
+      </c>
+      <c r="C216" t="s">
+        <v>27</v>
+      </c>
+      <c r="D216" s="9">
+        <v>45499</v>
+      </c>
+      <c r="E216" s="8">
+        <v>45523</v>
+      </c>
+      <c r="F216" s="1">
+        <v>36000</v>
+      </c>
+      <c r="G216" s="1">
+        <v>36000</v>
+      </c>
+      <c r="I216" s="1">
+        <f>G216-F216</f>
+        <v>0</v>
+      </c>
+      <c r="J216" s="1">
+        <v>36000</v>
+      </c>
+      <c r="K216" s="1">
+        <f>G216-J216</f>
+        <v>0</v>
+      </c>
+      <c r="L216" s="1">
+        <f>G216-J216+H216</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:14">
+      <c r="A217" s="9"/>
+      <c r="B217" t="s">
+        <v>100</v>
+      </c>
+      <c r="D217" s="9">
+        <v>45499</v>
+      </c>
+      <c r="E217" s="8">
+        <v>45507</v>
+      </c>
+      <c r="F217" s="1">
+        <v>2178000</v>
+      </c>
+      <c r="G217" s="1">
+        <v>2178000</v>
+      </c>
+      <c r="I217" s="1">
+        <f>G217-F217</f>
+        <v>0</v>
+      </c>
+      <c r="J217" s="1">
+        <v>2178000</v>
+      </c>
+      <c r="K217" s="1">
+        <f>G217-J217</f>
+        <v>0</v>
+      </c>
+      <c r="L217" s="1">
+        <f>G217-J217+H217</f>
+        <v>0</v>
+      </c>
+      <c r="M217" s="1">
+        <v>50000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update 29 agustus 2024
</commit_message>
<xml_diff>
--- a/pembayaran/Pembayaran.xlsx
+++ b/pembayaran/Pembayaran.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="867" documentId="14_{1E7DE582-8E6A-4088-84FC-1A8DF5B9EF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15395474-CE5B-4AC5-ADB2-F3831331AC12}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="9030" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,11 +471,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
-    <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -534,9 +533,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -568,15 +564,15 @@
       <numFmt numFmtId="164" formatCode="#,##0.00_ ;[Red]\-#,##0.00\ "/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="right"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="left"/>
     </dxf>
     <dxf>
@@ -947,11 +943,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q217"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" zoomScale="110" workbookViewId="0">
-      <selection activeCell="I207" sqref="I207"/>
+    <sheetView tabSelected="1" topLeftCell="A201" zoomScale="110" workbookViewId="0">
+      <selection activeCell="B214" sqref="B214"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" style="6" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
@@ -965,7 +961,7 @@
     <col min="17" max="17" width="16.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1009,7 +1005,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>45233</v>
       </c>
@@ -1048,7 +1044,7 @@
         <v>41282000</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>45234</v>
       </c>
@@ -1087,7 +1083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>45248</v>
       </c>
@@ -1122,7 +1118,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>18</v>
       </c>
@@ -1154,7 +1150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>20</v>
       </c>
@@ -1183,7 +1179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>21</v>
       </c>
@@ -1212,7 +1208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>22</v>
       </c>
@@ -1241,7 +1237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>16</v>
       </c>
@@ -1273,7 +1269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -1302,7 +1298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>14</v>
       </c>
@@ -1334,7 +1330,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>26</v>
       </c>
@@ -1370,7 +1366,7 @@
       </c>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>28</v>
       </c>
@@ -1403,7 +1399,7 @@
       </c>
       <c r="N13" s="1"/>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>29</v>
       </c>
@@ -1433,7 +1429,7 @@
       </c>
       <c r="N14" s="1"/>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>45252</v>
       </c>
@@ -1470,7 +1466,7 @@
       <c r="N15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>45261</v>
       </c>
@@ -1513,7 +1509,7 @@
         <v>109612000</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>14</v>
       </c>
@@ -1558,7 +1554,7 @@
         <v>700000</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>45273</v>
       </c>
@@ -1597,7 +1593,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>45275</v>
       </c>
@@ -1638,7 +1634,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>24</v>
       </c>
@@ -1671,7 +1667,7 @@
       </c>
       <c r="N20" s="1"/>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>36</v>
       </c>
@@ -1706,7 +1702,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>39</v>
       </c>
@@ -1738,7 +1734,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>45277</v>
       </c>
@@ -1774,7 +1770,7 @@
       </c>
       <c r="N23" s="1"/>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>26</v>
       </c>
@@ -1807,7 +1803,7 @@
       </c>
       <c r="N24" s="1"/>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>18</v>
       </c>
@@ -1840,7 +1836,7 @@
       </c>
       <c r="N25" s="1"/>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>41</v>
       </c>
@@ -1870,7 +1866,7 @@
       </c>
       <c r="N26" s="1"/>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>42</v>
       </c>
@@ -1900,7 +1896,7 @@
       </c>
       <c r="N27" s="1"/>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>16</v>
       </c>
@@ -1938,7 +1934,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="6">
         <v>45289</v>
       </c>
@@ -1976,7 +1972,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>14</v>
       </c>
@@ -2015,7 +2011,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>45290</v>
       </c>
@@ -2051,7 +2047,7 @@
       </c>
       <c r="N31" s="1"/>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C32" t="s">
         <v>46</v>
       </c>
@@ -2081,7 +2077,7 @@
       </c>
       <c r="N32" s="1"/>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>47</v>
       </c>
@@ -2111,7 +2107,7 @@
       </c>
       <c r="N33" s="1"/>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>48</v>
       </c>
@@ -2141,7 +2137,7 @@
       </c>
       <c r="N34" s="1"/>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>49</v>
       </c>
@@ -2171,7 +2167,7 @@
       </c>
       <c r="N35" s="1"/>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
         <v>50</v>
       </c>
@@ -2202,7 +2198,7 @@
       <c r="N36" s="1"/>
       <c r="P36" s="1"/>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>45305</v>
       </c>
@@ -2251,7 +2247,7 @@
         <v>93256000</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>45309</v>
       </c>
@@ -2294,7 +2290,7 @@
         <v>400000</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>45312</v>
       </c>
@@ -2330,7 +2326,7 @@
       </c>
       <c r="N39" s="1"/>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
         <v>49</v>
       </c>
@@ -2360,7 +2356,7 @@
       </c>
       <c r="N40" s="1"/>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
         <v>48</v>
       </c>
@@ -2390,7 +2386,7 @@
       </c>
       <c r="N41" s="1"/>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>50</v>
       </c>
@@ -2420,7 +2416,7 @@
       </c>
       <c r="N42" s="1"/>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>47</v>
       </c>
@@ -2450,7 +2446,7 @@
       </c>
       <c r="N43" s="1"/>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>46</v>
       </c>
@@ -2480,7 +2476,7 @@
       </c>
       <c r="N44" s="1"/>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C45" t="s">
         <v>41</v>
       </c>
@@ -2510,7 +2506,7 @@
       </c>
       <c r="N45" s="1"/>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C46" t="s">
         <v>52</v>
       </c>
@@ -2540,7 +2536,7 @@
       </c>
       <c r="N46" s="1"/>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>16</v>
       </c>
@@ -2579,7 +2575,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>45316</v>
       </c>
@@ -2615,7 +2611,7 @@
       </c>
       <c r="N48" s="1"/>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>54</v>
       </c>
@@ -2645,7 +2641,7 @@
       </c>
       <c r="N49" s="1"/>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C50" t="s">
         <v>55</v>
       </c>
@@ -2675,7 +2671,7 @@
       </c>
       <c r="N50" s="1"/>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C51" t="s">
         <v>57</v>
       </c>
@@ -2705,7 +2701,7 @@
       </c>
       <c r="N51" s="1"/>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C52" t="s">
         <v>58</v>
       </c>
@@ -2732,7 +2728,7 @@
       </c>
       <c r="N52" s="1"/>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C53" t="s">
         <v>40</v>
       </c>
@@ -2756,7 +2752,7 @@
       </c>
       <c r="N53" s="1"/>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>20</v>
       </c>
@@ -2780,7 +2776,7 @@
       </c>
       <c r="N54" s="1"/>
     </row>
-    <row r="55" spans="1:17">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
         <v>19</v>
       </c>
@@ -2804,7 +2800,7 @@
       </c>
       <c r="N55" s="1"/>
     </row>
-    <row r="56" spans="1:17">
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A56" s="6">
         <v>45318</v>
       </c>
@@ -2844,7 +2840,7 @@
       </c>
       <c r="N56" s="1"/>
     </row>
-    <row r="57" spans="1:17">
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>36</v>
       </c>
@@ -2871,7 +2867,7 @@
       </c>
       <c r="N57" s="1"/>
     </row>
-    <row r="58" spans="1:17">
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C58" t="s">
         <v>39</v>
       </c>
@@ -2895,7 +2891,7 @@
       </c>
       <c r="N58" s="1"/>
     </row>
-    <row r="59" spans="1:17">
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A59" s="6">
         <v>45319</v>
       </c>
@@ -2931,7 +2927,7 @@
       </c>
       <c r="N59" s="1"/>
     </row>
-    <row r="60" spans="1:17">
+    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C60" t="s">
         <v>52</v>
       </c>
@@ -2962,7 +2958,7 @@
       <c r="N60" s="1"/>
       <c r="P60" s="1"/>
     </row>
-    <row r="61" spans="1:17">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A61" s="6">
         <v>45327</v>
       </c>
@@ -3010,7 +3006,7 @@
         <v>79356000</v>
       </c>
     </row>
-    <row r="62" spans="1:17">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A62" s="6">
         <v>45332</v>
       </c>
@@ -3055,7 +3051,7 @@
         <v>550000</v>
       </c>
     </row>
-    <row r="63" spans="1:17">
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="6">
         <v>45339</v>
       </c>
@@ -3088,7 +3084,7 @@
       </c>
       <c r="N63" s="1"/>
     </row>
-    <row r="64" spans="1:17">
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>30</v>
       </c>
@@ -3124,7 +3120,7 @@
       </c>
       <c r="N64" s="1"/>
     </row>
-    <row r="65" spans="1:17">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="6">
         <v>45341</v>
       </c>
@@ -3159,7 +3155,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="66" spans="1:17">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="6">
         <v>45347</v>
       </c>
@@ -3200,7 +3196,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="67" spans="1:17">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>61</v>
       </c>
@@ -3238,7 +3234,7 @@
       <c r="N67" s="1"/>
       <c r="P67" s="1"/>
     </row>
-    <row r="68" spans="1:17">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A68" s="6">
         <v>45352</v>
       </c>
@@ -3283,7 +3279,7 @@
         <v>74431000</v>
       </c>
     </row>
-    <row r="69" spans="1:17">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>36</v>
       </c>
@@ -3323,7 +3319,7 @@
         <v>600000</v>
       </c>
     </row>
-    <row r="70" spans="1:17">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C70" t="s">
         <v>71</v>
       </c>
@@ -3353,7 +3349,7 @@
       </c>
       <c r="N70" s="1"/>
     </row>
-    <row r="71" spans="1:17">
+    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C71" t="s">
         <v>72</v>
       </c>
@@ -3383,7 +3379,7 @@
       </c>
       <c r="N71" s="1"/>
     </row>
-    <row r="72" spans="1:17">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
         <v>73</v>
       </c>
@@ -3413,7 +3409,7 @@
       </c>
       <c r="N72" s="1"/>
     </row>
-    <row r="73" spans="1:17">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A73" s="6">
         <v>45354</v>
       </c>
@@ -3451,7 +3447,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="74" spans="1:17">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A74" s="6">
         <v>45358</v>
       </c>
@@ -3490,7 +3486,7 @@
       </c>
       <c r="N74" s="1"/>
     </row>
-    <row r="75" spans="1:17">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="6">
         <v>45361</v>
       </c>
@@ -3523,7 +3519,7 @@
       </c>
       <c r="N75" s="1"/>
     </row>
-    <row r="76" spans="1:17">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A76" s="6">
         <v>45362</v>
       </c>
@@ -3564,7 +3560,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="77" spans="1:17">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="6">
         <v>45366</v>
       </c>
@@ -3599,7 +3595,7 @@
       </c>
       <c r="N77" s="1"/>
     </row>
-    <row r="78" spans="1:17">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C78" t="s">
         <v>79</v>
       </c>
@@ -3633,7 +3629,7 @@
       <c r="N78" s="1"/>
       <c r="P78" s="1"/>
     </row>
-    <row r="79" spans="1:17">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A79" s="6">
         <v>45368</v>
       </c>
@@ -3673,7 +3669,7 @@
       </c>
       <c r="N79" s="1"/>
     </row>
-    <row r="80" spans="1:17">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
         <v>45374</v>
       </c>
@@ -3712,7 +3708,7 @@
       </c>
       <c r="N80" s="1"/>
     </row>
-    <row r="81" spans="1:17">
+    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
         <v>28</v>
       </c>
@@ -3745,7 +3741,7 @@
       </c>
       <c r="N81" s="1"/>
     </row>
-    <row r="82" spans="1:17">
+    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
         <v>81</v>
       </c>
@@ -3778,7 +3774,7 @@
       </c>
       <c r="N82" s="1"/>
     </row>
-    <row r="83" spans="1:17">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>61</v>
       </c>
@@ -3814,7 +3810,7 @@
       </c>
       <c r="N83" s="1"/>
     </row>
-    <row r="84" spans="1:17">
+    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>36</v>
       </c>
@@ -3852,7 +3848,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="85" spans="1:17">
+    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A85" s="6">
         <v>45376</v>
       </c>
@@ -3888,7 +3884,7 @@
       </c>
       <c r="N85" s="1"/>
     </row>
-    <row r="86" spans="1:17">
+    <row r="86" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>84</v>
       </c>
@@ -3926,7 +3922,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="87" spans="1:17">
+    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="6">
         <v>45380</v>
       </c>
@@ -3965,7 +3961,7 @@
       </c>
       <c r="N87" s="1"/>
     </row>
-    <row r="88" spans="1:17">
+    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>30</v>
       </c>
@@ -4001,7 +3997,7 @@
       </c>
       <c r="N88" s="1"/>
     </row>
-    <row r="89" spans="1:17">
+    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C89" t="s">
         <v>67</v>
       </c>
@@ -4040,7 +4036,7 @@
       </c>
       <c r="P89" s="1"/>
     </row>
-    <row r="90" spans="1:17">
+    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="6">
         <v>45383</v>
       </c>
@@ -4086,7 +4082,7 @@
         <v>89108000</v>
       </c>
     </row>
-    <row r="91" spans="1:17">
+    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>36</v>
       </c>
@@ -4129,7 +4125,7 @@
         <v>250000</v>
       </c>
     </row>
-    <row r="92" spans="1:17">
+    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C92" t="s">
         <v>72</v>
       </c>
@@ -4162,7 +4158,7 @@
       </c>
       <c r="N92" s="1"/>
     </row>
-    <row r="93" spans="1:17">
+    <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
         <v>73</v>
       </c>
@@ -4195,7 +4191,7 @@
       </c>
       <c r="N93" s="1"/>
     </row>
-    <row r="94" spans="1:17">
+    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>26</v>
       </c>
@@ -4230,7 +4226,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="95" spans="1:17">
+    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
         <v>29</v>
       </c>
@@ -4266,7 +4262,7 @@
       </c>
       <c r="P95" s="1"/>
     </row>
-    <row r="96" spans="1:17">
+    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A96" s="6">
         <v>45385</v>
       </c>
@@ -4310,7 +4306,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="97" spans="1:17">
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A97" s="6">
         <v>45386</v>
       </c>
@@ -4348,7 +4344,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="1:17">
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>16</v>
       </c>
@@ -4389,7 +4385,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="99" spans="1:17">
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="6">
         <v>45387</v>
       </c>
@@ -4430,7 +4426,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="100" spans="1:17">
+    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>30</v>
       </c>
@@ -4465,7 +4461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:17">
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>84</v>
       </c>
@@ -4503,7 +4499,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="102" spans="1:17">
+    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="6">
         <v>45408</v>
       </c>
@@ -4547,7 +4543,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="103" spans="1:17">
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A103" s="6">
         <v>45409</v>
       </c>
@@ -4585,7 +4581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:17">
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="6">
         <v>45410</v>
       </c>
@@ -4620,7 +4616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:17">
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="6">
         <v>45412</v>
       </c>
@@ -4655,7 +4651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:17">
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A106" s="6">
         <v>45413</v>
       </c>
@@ -4700,7 +4696,7 @@
         <v>118948000</v>
       </c>
     </row>
-    <row r="107" spans="1:17">
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C107" t="s">
         <v>72</v>
       </c>
@@ -4739,7 +4735,7 @@
         <v>1100000</v>
       </c>
     </row>
-    <row r="108" spans="1:17">
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C108" t="s">
         <v>73</v>
       </c>
@@ -4771,7 +4767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:17">
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A109" s="6">
         <v>45414</v>
       </c>
@@ -4815,7 +4811,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="110" spans="1:17">
+    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A110" s="6">
         <v>45416</v>
       </c>
@@ -4859,7 +4855,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="111" spans="1:17">
+    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>61</v>
       </c>
@@ -4897,7 +4893,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="112" spans="1:17">
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A112" s="6">
         <v>45417</v>
       </c>
@@ -4935,7 +4931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:17">
+    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="6">
         <v>45420</v>
       </c>
@@ -4973,7 +4969,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="114" spans="1:17">
+    <row r="114" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A114" s="6">
         <v>45424</v>
       </c>
@@ -5008,7 +5004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:17">
+    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A115" s="6">
         <v>45427</v>
       </c>
@@ -5046,7 +5042,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="116" spans="1:17">
+    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>84</v>
       </c>
@@ -5087,7 +5083,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="117" spans="1:17">
+    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" s="6">
         <v>45430</v>
       </c>
@@ -5125,7 +5121,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="118" spans="1:17">
+    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>103</v>
       </c>
@@ -5160,7 +5156,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="119" spans="1:17">
+    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>16</v>
       </c>
@@ -5201,7 +5197,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="120" spans="1:17">
+    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A120" s="6">
         <v>45434</v>
       </c>
@@ -5239,7 +5235,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="121" spans="1:17">
+    <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>100</v>
       </c>
@@ -5274,7 +5270,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="122" spans="1:17">
+    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>28</v>
       </c>
@@ -5309,7 +5305,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="123" spans="1:17">
+    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" s="6">
         <v>45437</v>
       </c>
@@ -5344,7 +5340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:17">
+    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A124" s="6">
         <v>45443</v>
       </c>
@@ -5379,7 +5375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:17">
+    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A125" s="6">
         <v>45444</v>
       </c>
@@ -5424,7 +5420,7 @@
         <v>158777000</v>
       </c>
     </row>
-    <row r="126" spans="1:17">
+    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>26</v>
       </c>
@@ -5466,7 +5462,7 @@
         <v>1764000</v>
       </c>
     </row>
-    <row r="127" spans="1:17">
+    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>36</v>
       </c>
@@ -5501,7 +5497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:17">
+    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C128" t="s">
         <v>70</v>
       </c>
@@ -5533,7 +5529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:14">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
         <v>84</v>
       </c>
@@ -5574,7 +5570,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="130" spans="1:14">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>64</v>
       </c>
@@ -5606,7 +5602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:14">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
         <v>36</v>
       </c>
@@ -5644,7 +5640,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="132" spans="1:14">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B132" t="s">
         <v>106</v>
       </c>
@@ -5676,7 +5672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:14">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="6">
         <v>45450</v>
       </c>
@@ -5717,7 +5713,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="134" spans="1:14">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
         <v>103</v>
       </c>
@@ -5758,7 +5754,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="135" spans="1:14">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="6">
         <v>45453</v>
       </c>
@@ -5796,7 +5792,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="136" spans="1:14">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="6">
         <v>45456</v>
       </c>
@@ -5834,7 +5830,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="137" spans="1:14">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B137" t="s">
         <v>96</v>
       </c>
@@ -5872,7 +5868,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="138" spans="1:14">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" s="6">
         <v>45457</v>
       </c>
@@ -5910,7 +5906,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="139" spans="1:14">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B139" t="s">
         <v>30</v>
       </c>
@@ -5948,7 +5944,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="140" spans="1:14">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" s="6">
         <v>45458</v>
       </c>
@@ -5989,7 +5985,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="141" spans="1:14">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" s="6">
         <v>45459</v>
       </c>
@@ -6033,7 +6029,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="142" spans="1:14">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142" s="6">
         <v>45463</v>
       </c>
@@ -6071,7 +6067,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="143" spans="1:14">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" s="6">
         <v>45466</v>
       </c>
@@ -6112,7 +6108,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="144" spans="1:14">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
         <v>20</v>
       </c>
@@ -6147,7 +6143,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="145" spans="1:17">
+    <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
         <v>28</v>
       </c>
@@ -6182,7 +6178,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="146" spans="1:17">
+    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146" s="6">
         <v>45468</v>
       </c>
@@ -6226,7 +6222,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="147" spans="1:17">
+    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147" s="6">
         <v>45469</v>
       </c>
@@ -6270,7 +6266,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="148" spans="1:17">
+    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
         <v>103</v>
       </c>
@@ -6311,7 +6307,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="149" spans="1:17">
+    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
         <v>100</v>
       </c>
@@ -6349,7 +6345,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="150" spans="1:17">
+    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A150" s="6">
         <v>45470</v>
       </c>
@@ -6393,7 +6389,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="151" spans="1:17">
+    <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151" s="6">
         <v>45471</v>
       </c>
@@ -6431,7 +6427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:17">
+    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C152" t="s">
         <v>114</v>
       </c>
@@ -6472,7 +6468,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="153" spans="1:17">
+    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
         <v>26</v>
       </c>
@@ -6513,7 +6509,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="154" spans="1:17">
+    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A154" s="6">
         <v>45473</v>
       </c>
@@ -6551,7 +6547,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="155" spans="1:17">
+    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A155" s="6">
         <v>45474</v>
       </c>
@@ -6596,7 +6592,7 @@
         <v>5896000</v>
       </c>
     </row>
-    <row r="156" spans="1:17">
+    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B156" t="s">
         <v>36</v>
       </c>
@@ -6644,7 +6640,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="157" spans="1:17">
+    <row r="157" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C157" t="s">
         <v>70</v>
       </c>
@@ -6682,7 +6678,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="158" spans="1:17">
+    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C158" t="s">
         <v>73</v>
       </c>
@@ -6720,7 +6716,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="159" spans="1:17">
+    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B159" t="s">
         <v>84</v>
       </c>
@@ -6761,7 +6757,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="160" spans="1:17">
+    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A160" s="6">
         <v>45475</v>
       </c>
@@ -6805,7 +6801,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="161" spans="1:14">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161" s="6">
         <v>45476</v>
       </c>
@@ -6852,7 +6848,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="162" spans="1:14">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C162" t="s">
         <v>27</v>
       </c>
@@ -6893,7 +6889,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="163" spans="1:14">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C163" t="s">
         <v>28</v>
       </c>
@@ -6931,7 +6927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:14">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C164" t="s">
         <v>81</v>
       </c>
@@ -6969,7 +6965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:14">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
         <v>36</v>
       </c>
@@ -7013,7 +7009,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="166" spans="1:14">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166" s="6">
         <v>45478</v>
       </c>
@@ -7057,7 +7053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:14">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C167" t="s">
         <v>128</v>
       </c>
@@ -7095,7 +7091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:14">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A168" s="6">
         <v>45479</v>
       </c>
@@ -7139,7 +7135,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="169" spans="1:14">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A169" s="6">
         <v>45481</v>
       </c>
@@ -7183,7 +7179,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="170" spans="1:14">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B170" t="s">
         <v>96</v>
       </c>
@@ -7224,7 +7220,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="171" spans="1:14">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A171" s="6">
         <v>45482</v>
       </c>
@@ -7262,7 +7258,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="172" spans="1:14">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B172" t="s">
         <v>100</v>
       </c>
@@ -7297,7 +7293,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="173" spans="1:14">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B173" t="s">
         <v>106</v>
       </c>
@@ -7335,7 +7331,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="174" spans="1:14">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174" s="6">
         <v>45486</v>
       </c>
@@ -7379,7 +7375,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="175" spans="1:14">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B175" t="s">
         <v>106</v>
       </c>
@@ -7420,7 +7416,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="176" spans="1:14">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176" s="6">
         <v>45488</v>
       </c>
@@ -7464,7 +7460,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="177" spans="1:14">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B177" t="s">
         <v>101</v>
       </c>
@@ -7502,7 +7498,7 @@
         <v>100000</v>
       </c>
     </row>
-    <row r="178" spans="1:14">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A178" s="6">
         <v>45489</v>
       </c>
@@ -7546,7 +7542,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="179" spans="1:14">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B179" t="s">
         <v>64</v>
       </c>
@@ -7587,7 +7583,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="180" spans="1:14">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A180" s="6">
         <v>45494</v>
       </c>
@@ -7631,7 +7627,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="181" spans="1:14">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B181" t="s">
         <v>20</v>
       </c>
@@ -7672,7 +7668,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="182" spans="1:14">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A182" s="6">
         <v>45499</v>
       </c>
@@ -7698,25 +7694,25 @@
         <v>1075000</v>
       </c>
       <c r="I182" s="1">
-        <f>G182-F182</f>
+        <f t="shared" ref="I182:I217" si="22">G182-F182</f>
         <v>0</v>
       </c>
       <c r="J182" s="1">
         <v>250000</v>
       </c>
       <c r="K182" s="1">
-        <f>G182-J182</f>
+        <f t="shared" ref="K182:K217" si="23">G182-J182</f>
         <v>-250000</v>
       </c>
       <c r="L182" s="1">
-        <f>G182-J182+H182</f>
+        <f t="shared" ref="L182:L217" si="24">G182-J182+H182</f>
         <v>825000</v>
       </c>
       <c r="N182" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="183" spans="1:14">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C183" t="s">
         <v>27</v>
       </c>
@@ -7736,25 +7732,25 @@
         <v>436000</v>
       </c>
       <c r="I183" s="1">
-        <f>G183-F183</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J183" s="1">
         <v>436000</v>
       </c>
       <c r="K183" s="1">
-        <f>G183-J183</f>
+        <f t="shared" si="23"/>
         <v>-436000</v>
       </c>
       <c r="L183" s="1">
-        <f>G183-J183+H183</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="N183" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="184" spans="1:14">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B184" t="s">
         <v>30</v>
       </c>
@@ -7777,22 +7773,22 @@
         <v>0</v>
       </c>
       <c r="I184" s="1">
-        <f>G184-F184</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J184" s="1">
         <v>586000</v>
       </c>
       <c r="K184" s="1">
-        <f>G184-J184</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L184" s="1">
-        <f>G184-J184+H184</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="185" spans="1:14">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B185" t="s">
         <v>61</v>
       </c>
@@ -7809,25 +7805,25 @@
         <v>164000</v>
       </c>
       <c r="I185" s="1">
-        <f>G185-F185</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J185" s="1">
         <v>164000</v>
       </c>
       <c r="K185" s="1">
-        <f>G185-J185</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L185" s="1">
-        <f>G185-J185+H185</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M185" s="1">
         <v>6000</v>
       </c>
     </row>
-    <row r="186" spans="1:14">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A186" s="6">
         <v>45500</v>
       </c>
@@ -7847,18 +7843,18 @@
         <v>30121000</v>
       </c>
       <c r="I186" s="1">
-        <f>G186-F186</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J186" s="1">
         <v>30093000</v>
       </c>
       <c r="K186" s="1">
-        <f>G186-J186</f>
+        <f t="shared" si="23"/>
         <v>28000</v>
       </c>
       <c r="L186" s="1">
-        <f>G186-J186+H186</f>
+        <f t="shared" si="24"/>
         <v>28000</v>
       </c>
       <c r="M186" s="1">
@@ -7868,7 +7864,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="187" spans="1:14">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B187" t="s">
         <v>26</v>
       </c>
@@ -7888,25 +7884,25 @@
         <v>419000</v>
       </c>
       <c r="I187" s="1">
-        <f>G187-F187</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J187" s="1">
         <v>400000</v>
       </c>
       <c r="K187" s="1">
-        <f>G187-J187</f>
+        <f t="shared" si="23"/>
         <v>19000</v>
       </c>
       <c r="L187" s="1">
-        <f>G187-J187+H187</f>
+        <f t="shared" si="24"/>
         <v>19000</v>
       </c>
       <c r="N187" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="188" spans="1:14">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A188" s="6">
         <v>45501</v>
       </c>
@@ -7926,25 +7922,25 @@
         <v>2029000</v>
       </c>
       <c r="I188" s="1">
-        <f>G188-F188</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J188" s="1">
         <v>2029000</v>
       </c>
       <c r="K188" s="1">
-        <f>G188-J188</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L188" s="1">
-        <f>G188-J188+H188</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M188" s="1">
         <v>50000</v>
       </c>
     </row>
-    <row r="189" spans="1:14">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B189" t="s">
         <v>26</v>
       </c>
@@ -7964,22 +7960,22 @@
         <v>379000</v>
       </c>
       <c r="I189" s="1">
-        <f>G189-F189</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J189" s="1">
         <v>379000</v>
       </c>
       <c r="K189" s="1">
-        <f>G189-J189</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L189" s="1">
-        <f>G189-J189+H189</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="190" spans="1:14">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A190" s="6">
         <v>45503</v>
       </c>
@@ -8002,25 +7998,25 @@
         <v>565000</v>
       </c>
       <c r="I190" s="1">
-        <f>G190-F190</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J190" s="1">
         <v>4000000</v>
       </c>
       <c r="K190" s="1">
-        <f>G190-J190</f>
+        <f t="shared" si="23"/>
         <v>-343000</v>
       </c>
       <c r="L190" s="1">
-        <f>G190-J190+H190</f>
+        <f t="shared" si="24"/>
         <v>222000</v>
       </c>
       <c r="N190" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="191" spans="1:14">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B191" t="s">
         <v>103</v>
       </c>
@@ -8041,18 +8037,18 @@
         <v>1500000</v>
       </c>
       <c r="I191" s="1">
-        <f>G191-F191</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J191" s="1">
         <v>24096000</v>
       </c>
       <c r="K191" s="1">
-        <f>G191-J191</f>
+        <f t="shared" si="23"/>
         <v>10000000</v>
       </c>
       <c r="L191" s="1">
-        <f>G191-J191+H191</f>
+        <f t="shared" si="24"/>
         <v>11500000</v>
       </c>
       <c r="M191" s="1">
@@ -8062,7 +8058,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="192" spans="1:14">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A192" s="6">
         <v>45506</v>
       </c>
@@ -8086,18 +8082,18 @@
         <v>701000</v>
       </c>
       <c r="I192" s="1">
-        <f>G192-F192</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J192" s="1">
         <v>9865000</v>
       </c>
       <c r="K192" s="1">
-        <f>G192-J192</f>
+        <f t="shared" si="23"/>
         <v>-701000</v>
       </c>
       <c r="L192" s="1">
-        <f>G192-J192+H192</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M192" s="1">
@@ -8107,7 +8103,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="193" spans="1:14">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A193" s="6">
         <v>45510</v>
       </c>
@@ -8127,25 +8123,25 @@
         <v>3909000</v>
       </c>
       <c r="I193" s="1">
-        <f>G193-F193</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J193" s="1">
         <v>3909000</v>
       </c>
       <c r="K193" s="1">
-        <f>G193-J193</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L193" s="1">
-        <f>G193-J193+H193</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M193" s="1">
         <v>100000</v>
       </c>
     </row>
-    <row r="194" spans="1:14">
+    <row r="194" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B194" t="s">
         <v>16</v>
       </c>
@@ -8165,25 +8161,25 @@
         <v>16627000</v>
       </c>
       <c r="I194" s="1">
-        <f>G194-F194</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J194" s="1">
         <v>3325000</v>
       </c>
       <c r="K194" s="1">
-        <f>G194-J194</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L194" s="1">
-        <f>G194-J194+H194</f>
+        <f t="shared" si="24"/>
         <v>16627000</v>
       </c>
       <c r="M194" s="1">
         <v>100000</v>
       </c>
     </row>
-    <row r="195" spans="1:14">
+    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A195" s="6">
         <v>45511</v>
       </c>
@@ -8206,18 +8202,18 @@
         <v>68000</v>
       </c>
       <c r="I195" s="1">
-        <f>G195-F195</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J195" s="1">
         <v>11804000</v>
       </c>
       <c r="K195" s="1">
-        <f>G195-J195</f>
+        <f t="shared" si="23"/>
         <v>-68000</v>
       </c>
       <c r="L195" s="1">
-        <f>G195-J195+H195</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M195" s="1">
@@ -8227,14 +8223,14 @@
         <v>122</v>
       </c>
     </row>
-    <row r="196" spans="1:14">
-      <c r="A196" s="9">
+    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A196" s="6">
         <v>45516</v>
       </c>
       <c r="B196" t="s">
         <v>106</v>
       </c>
-      <c r="D196" s="9">
+      <c r="D196" s="6">
         <v>45480</v>
       </c>
       <c r="E196" s="8">
@@ -8250,18 +8246,18 @@
         <v>222000</v>
       </c>
       <c r="I196" s="1">
-        <f>G196-F196</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J196" s="1">
         <v>5000000</v>
       </c>
       <c r="K196" s="1">
-        <f>G196-J196</f>
+        <f t="shared" si="23"/>
         <v>5101000</v>
       </c>
       <c r="L196" s="1">
-        <f>G196-J196+H196</f>
+        <f t="shared" si="24"/>
         <v>5323000</v>
       </c>
       <c r="M196" s="1">
@@ -8271,12 +8267,11 @@
         <v>136</v>
       </c>
     </row>
-    <row r="197" spans="1:14">
-      <c r="A197" s="9"/>
+    <row r="197" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B197" t="s">
         <v>103</v>
       </c>
-      <c r="D197" s="9">
+      <c r="D197" s="6">
         <v>45478</v>
       </c>
       <c r="E197" s="8">
@@ -8292,18 +8287,18 @@
         <v>11500000</v>
       </c>
       <c r="I197" s="1">
-        <f>G197-F197</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J197" s="1">
         <v>20993000</v>
       </c>
       <c r="K197" s="1">
-        <f>G197-J197</f>
+        <f t="shared" si="23"/>
         <v>-4000000</v>
       </c>
       <c r="L197" s="1">
-        <f>G197-J197+H197</f>
+        <f t="shared" si="24"/>
         <v>7500000</v>
       </c>
       <c r="M197" s="1">
@@ -8313,14 +8308,14 @@
         <v>75</v>
       </c>
     </row>
-    <row r="198" spans="1:14">
-      <c r="A198" s="9">
+    <row r="198" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A198" s="6">
         <v>45517</v>
       </c>
       <c r="B198" t="s">
         <v>100</v>
       </c>
-      <c r="D198" s="9">
+      <c r="D198" s="6">
         <v>45480</v>
       </c>
       <c r="E198" s="8">
@@ -8333,30 +8328,29 @@
         <v>4204000</v>
       </c>
       <c r="I198" s="1">
-        <f>G198-F198</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J198" s="1">
         <v>4204000</v>
       </c>
       <c r="K198" s="1">
-        <f>G198-J198</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L198" s="1">
-        <f>G198-J198+H198</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M198" s="1">
         <v>100000</v>
       </c>
     </row>
-    <row r="199" spans="1:14">
-      <c r="A199" s="9"/>
+    <row r="199" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B199" t="s">
         <v>28</v>
       </c>
-      <c r="D199" s="9">
+      <c r="D199" s="6">
         <v>45501</v>
       </c>
       <c r="E199" s="8">
@@ -8369,27 +8363,26 @@
         <v>651000</v>
       </c>
       <c r="I199" s="1">
-        <f>G199-F199</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J199" s="1">
         <v>651000</v>
       </c>
       <c r="K199" s="1">
-        <f>G199-J199</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L199" s="1">
-        <f>G199-J199+H199</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="200" spans="1:14">
-      <c r="A200" s="9"/>
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B200" t="s">
         <v>137</v>
       </c>
-      <c r="D200" s="9">
+      <c r="D200" s="6">
         <v>45423</v>
       </c>
       <c r="E200" s="8">
@@ -8402,18 +8395,18 @@
         <v>2291000</v>
       </c>
       <c r="I200" s="1">
-        <f>G200-F200</f>
+        <f t="shared" si="22"/>
         <v>59000</v>
       </c>
       <c r="J200" s="1">
         <v>1280000</v>
       </c>
       <c r="K200" s="1">
-        <f>G200-J200</f>
+        <f t="shared" si="23"/>
         <v>1011000</v>
       </c>
       <c r="L200" s="1">
-        <f>G200-J200+H200</f>
+        <f t="shared" si="24"/>
         <v>1011000</v>
       </c>
       <c r="M200" s="1">
@@ -8423,15 +8416,14 @@
         <v>75</v>
       </c>
     </row>
-    <row r="201" spans="1:14">
-      <c r="A201" s="9"/>
+    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B201" t="s">
         <v>26</v>
       </c>
       <c r="C201" t="s">
         <v>81</v>
       </c>
-      <c r="D201" s="9">
+      <c r="D201" s="6">
         <v>45497</v>
       </c>
       <c r="E201" s="8">
@@ -8447,30 +8439,29 @@
         <v>19000</v>
       </c>
       <c r="I201" s="1">
-        <f>G201-F201</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J201" s="1">
         <v>300000</v>
       </c>
       <c r="K201" s="1">
-        <f>G201-J201</f>
+        <f t="shared" si="23"/>
         <v>-3000</v>
       </c>
       <c r="L201" s="1">
-        <f>G201-J201+H201</f>
+        <f t="shared" si="24"/>
         <v>16000</v>
       </c>
       <c r="N201" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="202" spans="1:14">
-      <c r="A202" s="9"/>
+    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C202" t="s">
         <v>29</v>
       </c>
-      <c r="D202" s="9">
+      <c r="D202" s="6">
         <v>45471</v>
       </c>
       <c r="E202" s="8">
@@ -8486,33 +8477,32 @@
         <v>3090000</v>
       </c>
       <c r="I202" s="1">
-        <f>G202-F202</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J202" s="1">
         <v>570000</v>
       </c>
       <c r="K202" s="1">
-        <f>G202-J202</f>
+        <f t="shared" si="23"/>
         <v>-570000</v>
       </c>
       <c r="L202" s="1">
-        <f>G202-J202+H202</f>
+        <f t="shared" si="24"/>
         <v>2520000</v>
       </c>
       <c r="N202" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="203" spans="1:14">
-      <c r="A203" s="9"/>
+    <row r="203" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B203" t="s">
         <v>30</v>
       </c>
       <c r="C203" t="s">
         <v>67</v>
       </c>
-      <c r="D203" s="9">
+      <c r="D203" s="6">
         <v>45473</v>
       </c>
       <c r="E203" s="8">
@@ -8528,32 +8518,32 @@
         <v>200000</v>
       </c>
       <c r="I203" s="1">
-        <f>G203-F203</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J203" s="1">
         <v>551000</v>
       </c>
       <c r="K203" s="1">
-        <f>G203-J203</f>
+        <f t="shared" si="23"/>
         <v>-180000</v>
       </c>
       <c r="L203" s="1">
-        <f>G203-J203+H203</f>
+        <f t="shared" si="24"/>
         <v>20000</v>
       </c>
       <c r="N203" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="204" spans="1:14">
-      <c r="A204" s="9">
+    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A204" s="6">
         <v>45521</v>
       </c>
       <c r="B204" t="s">
         <v>138</v>
       </c>
-      <c r="D204" s="9">
+      <c r="D204" s="6">
         <v>45467</v>
       </c>
       <c r="E204" s="8">
@@ -8566,18 +8556,18 @@
         <v>33942000</v>
       </c>
       <c r="I204" s="1">
-        <f>G204-F204</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J204" s="1">
         <v>10000000</v>
       </c>
       <c r="K204" s="1">
-        <f>G204-J204</f>
+        <f t="shared" si="23"/>
         <v>23942000</v>
       </c>
       <c r="L204" s="1">
-        <f>G204-J204+H204</f>
+        <f t="shared" si="24"/>
         <v>23942000</v>
       </c>
       <c r="M204" s="1">
@@ -8587,14 +8577,14 @@
         <v>75</v>
       </c>
     </row>
-    <row r="205" spans="1:14">
-      <c r="A205" s="9">
+    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A205" s="6">
         <v>45523</v>
       </c>
       <c r="B205" t="s">
         <v>135</v>
       </c>
-      <c r="D205" s="9">
+      <c r="D205" s="6">
         <v>45507</v>
       </c>
       <c r="E205" s="8">
@@ -8607,32 +8597,32 @@
         <v>4782000</v>
       </c>
       <c r="I205" s="1">
-        <f>G205-F205</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J205" s="1">
         <v>4782000</v>
       </c>
       <c r="K205" s="1">
-        <f>G205-J205</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L205" s="1">
-        <f>G205-J205+H205</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M205" s="1">
         <v>100000</v>
       </c>
     </row>
-    <row r="206" spans="1:14">
-      <c r="A206" s="9">
+    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A206" s="6">
         <v>45525</v>
       </c>
       <c r="B206" t="s">
         <v>106</v>
       </c>
-      <c r="D206" s="9">
+      <c r="D206" s="6">
         <v>45480</v>
       </c>
       <c r="E206" s="8">
@@ -8648,18 +8638,18 @@
         <v>5323000</v>
       </c>
       <c r="I206" s="1">
-        <f>G206-F206</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J206" s="1">
         <v>5000000</v>
       </c>
       <c r="K206" s="1">
-        <f>G206-J206</f>
+        <f t="shared" si="23"/>
         <v>-5000000</v>
       </c>
       <c r="L206" s="1">
-        <f>G206-J206+H206</f>
+        <f t="shared" si="24"/>
         <v>323000</v>
       </c>
       <c r="M206" s="1">
@@ -8669,14 +8659,14 @@
         <v>75</v>
       </c>
     </row>
-    <row r="207" spans="1:14">
-      <c r="A207" s="9">
+    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A207" s="6">
         <v>45526</v>
       </c>
       <c r="B207" t="s">
         <v>96</v>
       </c>
-      <c r="D207" s="9">
+      <c r="D207" s="6">
         <v>45507</v>
       </c>
       <c r="E207" s="8">
@@ -8692,32 +8682,32 @@
         <v>0</v>
       </c>
       <c r="I207" s="1">
-        <f>G207-F207</f>
+        <f t="shared" si="22"/>
         <v>-250000</v>
       </c>
       <c r="J207" s="1">
         <v>9085000</v>
       </c>
       <c r="K207" s="1">
-        <f>G207-J207</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L207" s="1">
-        <f>G207-J207+H207</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M207" s="1">
         <v>100000</v>
       </c>
     </row>
-    <row r="208" spans="1:14">
-      <c r="A208" s="9">
+    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A208" s="6">
         <v>45527</v>
       </c>
       <c r="B208" t="s">
         <v>16</v>
       </c>
-      <c r="D208" s="9">
+      <c r="D208" s="6">
         <v>45486</v>
       </c>
       <c r="E208" s="8">
@@ -8733,30 +8723,29 @@
         <v>16627000</v>
       </c>
       <c r="I208" s="1">
-        <f>G208-F208</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J208" s="1">
         <v>10000000</v>
       </c>
       <c r="K208" s="1">
-        <f>G208-J208</f>
+        <f t="shared" si="23"/>
         <v>-10000000</v>
       </c>
       <c r="L208" s="1">
-        <f>G208-J208+H208</f>
+        <f t="shared" si="24"/>
         <v>6627000</v>
       </c>
       <c r="N208" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="209" spans="1:14">
-      <c r="A209" s="9"/>
+    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B209" t="s">
         <v>101</v>
       </c>
-      <c r="D209" s="9">
+      <c r="D209" s="6">
         <v>45501</v>
       </c>
       <c r="E209" s="8">
@@ -8769,26 +8758,26 @@
         <v>10977000</v>
       </c>
       <c r="I209" s="1">
-        <f>G209-F209</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J209" s="1">
         <v>10977000</v>
       </c>
       <c r="K209" s="1">
-        <f>G209-J209</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L209" s="1">
-        <f>G209-J209+H209</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M209" s="1">
         <v>100000</v>
       </c>
     </row>
-    <row r="210" spans="1:14">
-      <c r="A210" s="9">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A210" s="6">
         <v>45528</v>
       </c>
       <c r="B210" t="s">
@@ -8797,7 +8786,7 @@
       <c r="C210" t="s">
         <v>139</v>
       </c>
-      <c r="D210" s="9">
+      <c r="D210" s="6">
         <v>45509</v>
       </c>
       <c r="E210" s="8">
@@ -8810,29 +8799,29 @@
         <v>72000</v>
       </c>
       <c r="I210" s="1">
-        <f>G210-F210</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J210" s="1">
         <v>72000</v>
       </c>
       <c r="K210" s="1">
-        <f>G210-J210</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L210" s="1">
-        <f>G210-J210+H210</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="211" spans="1:14">
-      <c r="A211" s="9">
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A211" s="6">
         <v>45529</v>
       </c>
       <c r="B211" t="s">
         <v>140</v>
       </c>
-      <c r="D211" s="9">
+      <c r="D211" s="6">
         <v>45509</v>
       </c>
       <c r="E211" s="8">
@@ -8845,18 +8834,18 @@
         <v>4863000</v>
       </c>
       <c r="I211" s="1">
-        <f>G211-F211</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J211" s="1">
         <v>3615000</v>
       </c>
       <c r="K211" s="1">
-        <f>G211-J211</f>
+        <f t="shared" si="23"/>
         <v>1248000</v>
       </c>
       <c r="L211" s="1">
-        <f>G211-J211+H211</f>
+        <f t="shared" si="24"/>
         <v>1248000</v>
       </c>
       <c r="M211" s="1">
@@ -8866,14 +8855,14 @@
         <v>141</v>
       </c>
     </row>
-    <row r="212" spans="1:14">
-      <c r="A212" s="9">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A212" s="6">
         <v>45530</v>
       </c>
       <c r="B212" t="s">
         <v>142</v>
       </c>
-      <c r="D212" s="9">
+      <c r="D212" s="6">
         <v>45506</v>
       </c>
       <c r="E212" s="8">
@@ -8886,32 +8875,32 @@
         <v>880000</v>
       </c>
       <c r="I212" s="1">
-        <f>G212-F212</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J212" s="1">
         <v>475000</v>
       </c>
       <c r="K212" s="1">
-        <f>G212-J212</f>
+        <f t="shared" si="23"/>
         <v>405000</v>
       </c>
       <c r="L212" s="1">
-        <f>G212-J212+H212</f>
+        <f t="shared" si="24"/>
         <v>405000</v>
       </c>
       <c r="N212" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="213" spans="1:14">
-      <c r="A213" s="9">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A213" s="6">
         <v>45531</v>
       </c>
       <c r="B213" t="s">
         <v>140</v>
       </c>
-      <c r="D213" s="9">
+      <c r="D213" s="6">
         <v>45509</v>
       </c>
       <c r="E213" s="8">
@@ -8927,32 +8916,32 @@
         <v>1248000</v>
       </c>
       <c r="I213" s="1">
-        <f>G213-F213</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J213" s="1">
         <v>1248000</v>
       </c>
       <c r="K213" s="1">
-        <f>G213-J213</f>
+        <f t="shared" si="23"/>
         <v>-1248000</v>
       </c>
       <c r="L213" s="1">
-        <f>G213-J213+H213</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="N213" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="214" spans="1:14">
-      <c r="A214" s="9">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A214" s="6">
         <v>45532</v>
       </c>
       <c r="B214" t="s">
         <v>103</v>
       </c>
-      <c r="D214" s="9">
+      <c r="D214" s="6">
         <v>45492</v>
       </c>
       <c r="E214" s="8">
@@ -8968,18 +8957,18 @@
         <v>7500000</v>
       </c>
       <c r="I214" s="1">
-        <f>G214-F214</f>
+        <f t="shared" si="22"/>
         <v>2034000</v>
       </c>
       <c r="J214" s="1">
         <v>15000000</v>
       </c>
       <c r="K214" s="1">
-        <f>G214-J214</f>
+        <f t="shared" si="23"/>
         <v>-2076000</v>
       </c>
       <c r="L214" s="1">
-        <f>G214-J214+H214</f>
+        <f t="shared" si="24"/>
         <v>5424000</v>
       </c>
       <c r="M214" s="1">
@@ -8989,12 +8978,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="215" spans="1:14">
-      <c r="A215" s="9"/>
+    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B215" t="s">
         <v>138</v>
       </c>
-      <c r="D215" s="9">
+      <c r="D215" s="6">
         <v>45500</v>
       </c>
       <c r="E215" s="8">
@@ -9010,18 +8998,18 @@
         <v>23942000</v>
       </c>
       <c r="I215" s="1">
-        <f>G215-F215</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J215" s="1">
         <v>10000000</v>
       </c>
       <c r="K215" s="1">
-        <f>G215-J215</f>
+        <f t="shared" si="23"/>
         <v>-3793000</v>
       </c>
       <c r="L215" s="1">
-        <f>G215-J215+H215</f>
+        <f t="shared" si="24"/>
         <v>20149000</v>
       </c>
       <c r="M215" s="1">
@@ -9031,15 +9019,14 @@
         <v>75</v>
       </c>
     </row>
-    <row r="216" spans="1:14">
-      <c r="A216" s="9"/>
+    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B216" t="s">
         <v>26</v>
       </c>
       <c r="C216" t="s">
         <v>27</v>
       </c>
-      <c r="D216" s="9">
+      <c r="D216" s="6">
         <v>45499</v>
       </c>
       <c r="E216" s="8">
@@ -9052,27 +9039,26 @@
         <v>36000</v>
       </c>
       <c r="I216" s="1">
-        <f>G216-F216</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J216" s="1">
         <v>36000</v>
       </c>
       <c r="K216" s="1">
-        <f>G216-J216</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L216" s="1">
-        <f>G216-J216+H216</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="217" spans="1:14">
-      <c r="A217" s="9"/>
+        <f t="shared" si="24"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B217" t="s">
         <v>100</v>
       </c>
-      <c r="D217" s="9">
+      <c r="D217" s="6">
         <v>45499</v>
       </c>
       <c r="E217" s="8">
@@ -9085,18 +9071,18 @@
         <v>2178000</v>
       </c>
       <c r="I217" s="1">
-        <f>G217-F217</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J217" s="1">
         <v>2178000</v>
       </c>
       <c r="K217" s="1">
-        <f>G217-J217</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="L217" s="1">
-        <f>G217-J217+H217</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M217" s="1">

</xml_diff>

<commit_message>
updae erik 14 nov
</commit_message>
<xml_diff>
--- a/pembayaran/Pembayaran.xlsx
+++ b/pembayaran/Pembayaran.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/277ffa1efc2bfcc1/Apartment Bintaro/Data Harian/BINTARO-APG/pembayaran/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1909" documentId="14_{1E7DE582-8E6A-4088-84FC-1A8DF5B9EF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{420673BD-C4A3-4CAD-89D4-72D7F2611D77}"/>
+  <xr:revisionPtr revIDLastSave="1955" documentId="14_{1E7DE582-8E6A-4088-84FC-1A8DF5B9EF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7063151-327C-4CAA-88AB-3977504341CF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="115">
   <si>
     <t>Tanggal Pembayaran</t>
   </si>
@@ -363,6 +363,9 @@
   </si>
   <si>
     <t>Rohim</t>
+  </si>
+  <si>
+    <t>kurang jay &amp; robi</t>
   </si>
   <si>
     <t>Bulan</t>
@@ -899,8 +902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q271"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D238" zoomScale="110" workbookViewId="0">
-      <selection activeCell="F258" sqref="F258"/>
+    <sheetView tabSelected="1" topLeftCell="A241" zoomScale="110" workbookViewId="0">
+      <selection activeCell="K266" sqref="K266"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9664,7 +9667,7 @@
    IFERROR(INDEX(Table1[Tanggal Pembayaran], MATCH(1,
    (Table1[[#This Row],[Nama Mandor]] = Table1[Nama Mandor]) * (Table1[[#This Row],[Nama Pekerja]] = Table1[Nama Pekerja]) * (Table1[[#This Row],[Tanggal Pembayaran]] &lt; Table1[Tanggal Pembayaran]), 0)), "No Next Payment"),
    "")</f>
-        <v>45527</v>
+        <v>45528</v>
       </c>
     </row>
     <row r="183" spans="1:17">
@@ -10160,7 +10163,7 @@
       </c>
       <c r="Q192" s="1">
         <f>SUM(J192:J220)</f>
-        <v>146770000</v>
+        <v>146345000</v>
       </c>
     </row>
     <row r="193" spans="1:17">
@@ -11049,7 +11052,7 @@
     </row>
     <row r="211" spans="1:17">
       <c r="A211" s="6">
-        <v>45527</v>
+        <v>45528</v>
       </c>
       <c r="B211" t="s">
         <v>24</v>
@@ -11078,15 +11081,15 @@
         <v>0</v>
       </c>
       <c r="J211" s="1">
-        <v>625000</v>
+        <v>200000</v>
       </c>
       <c r="K211" s="1">
         <f>G211-J211</f>
-        <v>-625000</v>
+        <v>-200000</v>
       </c>
       <c r="L211" s="1">
         <f>G211-J211+H211</f>
-        <v>200000</v>
+        <v>625000</v>
       </c>
       <c r="N211" s="9" cm="1">
         <f t="array" ref="N211">IF(Table1[[#This Row],[Total Kurang Bayar]] &lt;&gt; 0,
@@ -12662,7 +12665,7 @@
       </c>
       <c r="H243" s="1" cm="1">
         <f t="array" ref="H243">IFERROR(LOOKUP(2,1/(($B$2:B242=B243)*($C$2:C242=C243)), $L$2:L242), 0)</f>
-        <v>200000</v>
+        <v>625000</v>
       </c>
       <c r="I243" s="1">
         <f t="shared" ref="I243:I245" si="28">G243-F243</f>
@@ -12677,14 +12680,14 @@
       </c>
       <c r="L243" s="1">
         <f t="shared" ref="L243:L245" si="30">G243-J243+H243</f>
-        <v>0</v>
+        <v>425000</v>
       </c>
       <c r="N243" s="9" t="str" cm="1">
         <f t="array" ref="N243">IF(Table1[[#This Row],[Total Kurang Bayar]] &lt;&gt; 0,
    IFERROR(INDEX(Table1[Tanggal Pembayaran], MATCH(1,
    (Table1[[#This Row],[Nama Mandor]] = Table1[Nama Mandor]) * (Table1[[#This Row],[Nama Pekerja]] = Table1[Nama Pekerja]) * (Table1[[#This Row],[Tanggal Pembayaran]] &lt; Table1[Tanggal Pembayaran]), 0)), "No Next Payment"),
    "")</f>
-        <v/>
+        <v>No Next Payment</v>
       </c>
     </row>
     <row r="244" spans="1:17">
@@ -13354,13 +13357,13 @@
         <v>100</v>
       </c>
       <c r="D257" s="10">
-        <v>45556</v>
+        <v>45554</v>
       </c>
       <c r="E257" s="8">
-        <v>45575</v>
+        <v>45573</v>
       </c>
       <c r="F257" s="1">
-        <v>484000</v>
+        <v>460000</v>
       </c>
       <c r="G257" s="1">
         <v>460000</v>
@@ -13371,7 +13374,7 @@
       </c>
       <c r="I257" s="1">
         <f>G257-F257</f>
-        <v>-24000</v>
+        <v>0</v>
       </c>
       <c r="J257" s="1">
         <v>460000</v>
@@ -13399,14 +13402,17 @@
       <c r="B258" t="s">
         <v>92</v>
       </c>
-      <c r="D258" s="6">
-        <v>45534</v>
+      <c r="D258" s="10">
+        <v>45525</v>
       </c>
       <c r="E258" s="8">
         <v>45557</v>
       </c>
+      <c r="F258" s="1">
+        <v>3938000</v>
+      </c>
       <c r="G258" s="1">
-        <v>4564000</v>
+        <v>3938000</v>
       </c>
       <c r="H258" s="1" cm="1">
         <f t="array" ref="H258">IFERROR(LOOKUP(2,1/(($B$2:B257=B258)*($C$2:C257=C258)), $L$2:L257), 0)</f>
@@ -13414,28 +13420,28 @@
       </c>
       <c r="I258" s="1">
         <f>G258-F258</f>
-        <v>4564000</v>
+        <v>0</v>
       </c>
       <c r="J258" s="1">
         <v>3938000</v>
       </c>
       <c r="K258" s="1">
         <f>G258-J258</f>
-        <v>626000</v>
+        <v>0</v>
       </c>
       <c r="L258" s="1">
         <f>G258-J258+H258</f>
-        <v>626000</v>
+        <v>0</v>
       </c>
       <c r="M258" s="1">
         <v>100000</v>
       </c>
-      <c r="N258" s="9" cm="1">
+      <c r="N258" s="9" t="str" cm="1">
         <f t="array" ref="N258">IF(Table1[[#This Row],[Total Kurang Bayar]] &lt;&gt; 0,
    IFERROR(INDEX(Table1[Tanggal Pembayaran], MATCH(1,
    (Table1[[#This Row],[Nama Mandor]] = Table1[Nama Mandor]) * (Table1[[#This Row],[Nama Pekerja]] = Table1[Nama Pekerja]) * (Table1[[#This Row],[Tanggal Pembayaran]] &lt; Table1[Tanggal Pembayaran]), 0)), "No Next Payment"),
    "")</f>
-        <v>45590</v>
+        <v/>
       </c>
     </row>
     <row r="259" spans="1:14">
@@ -13498,8 +13504,11 @@
       <c r="E260" s="8">
         <v>45575</v>
       </c>
+      <c r="F260" s="1">
+        <v>1563000</v>
+      </c>
       <c r="G260" s="1">
-        <v>1788000</v>
+        <v>1563000</v>
       </c>
       <c r="H260" s="1" cm="1">
         <f t="array" ref="H260">IFERROR(LOOKUP(2,1/(($B$2:B259=B260)*($C$2:C259=C260)), $L$2:L259), 0)</f>
@@ -13507,18 +13516,18 @@
       </c>
       <c r="I260" s="1">
         <f>G260-F260</f>
-        <v>1788000</v>
+        <v>0</v>
       </c>
       <c r="J260" s="1">
         <v>1744000</v>
       </c>
       <c r="K260" s="1">
         <f>G260-J260</f>
-        <v>44000</v>
+        <v>-181000</v>
       </c>
       <c r="L260" s="1">
         <f>G260-J260+H260</f>
-        <v>269000</v>
+        <v>44000</v>
       </c>
       <c r="M260" s="1">
         <v>44000</v>
@@ -13548,8 +13557,11 @@
       <c r="E261" s="8">
         <v>45572</v>
       </c>
+      <c r="F261" s="1">
+        <v>361000</v>
+      </c>
       <c r="G261" s="1">
-        <v>430000</v>
+        <v>361000</v>
       </c>
       <c r="H261" s="1" cm="1">
         <f t="array" ref="H261">IFERROR(LOOKUP(2,1/(($B$2:B260=B261)*($C$2:C260=C261)), $L$2:L260), 0)</f>
@@ -13557,18 +13569,18 @@
       </c>
       <c r="I261" s="1">
         <f>G261-F261</f>
-        <v>430000</v>
+        <v>0</v>
       </c>
       <c r="J261" s="1">
         <v>430000</v>
       </c>
       <c r="K261" s="1">
         <f>G261-J261</f>
-        <v>0</v>
+        <v>-69000</v>
       </c>
       <c r="L261" s="1">
         <f>G261-J261+H261</f>
-        <v>69000</v>
+        <v>0</v>
       </c>
       <c r="M261" s="1">
         <v>30000</v>
@@ -13578,7 +13590,7 @@
    IFERROR(INDEX(Table1[Tanggal Pembayaran], MATCH(1,
    (Table1[[#This Row],[Nama Mandor]] = Table1[Nama Mandor]) * (Table1[[#This Row],[Nama Pekerja]] = Table1[Nama Pekerja]) * (Table1[[#This Row],[Tanggal Pembayaran]] &lt; Table1[Tanggal Pembayaran]), 0)), "No Next Payment"),
    "")</f>
-        <v>No Next Payment</v>
+        <v/>
       </c>
     </row>
     <row r="262" spans="1:14">
@@ -13598,8 +13610,11 @@
       <c r="E262" s="8">
         <v>45572</v>
       </c>
+      <c r="F262" s="1">
+        <v>515000</v>
+      </c>
       <c r="G262" s="1">
-        <v>540000</v>
+        <v>515000</v>
       </c>
       <c r="H262" s="1" cm="1">
         <f t="array" ref="H262">IFERROR(LOOKUP(2,1/(($B$2:B261=B262)*($C$2:C261=C262)), $L$2:L261), 0)</f>
@@ -13607,18 +13622,18 @@
       </c>
       <c r="I262" s="1">
         <f>G262-F262</f>
-        <v>540000</v>
+        <v>0</v>
       </c>
       <c r="J262" s="1">
         <v>540000</v>
       </c>
       <c r="K262" s="1">
         <f>G262-J262</f>
-        <v>0</v>
+        <v>-25000</v>
       </c>
       <c r="L262" s="1">
         <f>G262-J262+H262</f>
-        <v>25000</v>
+        <v>0</v>
       </c>
       <c r="M262" s="1">
         <v>30000</v>
@@ -13628,7 +13643,7 @@
    IFERROR(INDEX(Table1[Tanggal Pembayaran], MATCH(1,
    (Table1[[#This Row],[Nama Mandor]] = Table1[Nama Mandor]) * (Table1[[#This Row],[Nama Pekerja]] = Table1[Nama Pekerja]) * (Table1[[#This Row],[Tanggal Pembayaran]] &lt; Table1[Tanggal Pembayaran]), 0)), "No Next Payment"),
    "")</f>
-        <v>No Next Payment</v>
+        <v/>
       </c>
     </row>
     <row r="263" spans="1:14">
@@ -13688,12 +13703,16 @@
       <c r="B264" t="s">
         <v>87</v>
       </c>
-      <c r="D264" s="6">
-        <v>45537</v>
+      <c r="D264" s="6" cm="1">
+        <f t="array" ref="D264">IFERROR(LOOKUP(2,1/(($B$2:B263=B264)*($C$2:C263=C264)), $E$2:E263)+1, 0)</f>
+        <v>45563</v>
       </c>
       <c r="E264" s="8">
         <v>45576</v>
       </c>
+      <c r="F264" s="1">
+        <v>197000</v>
+      </c>
       <c r="G264" s="1">
         <v>197000</v>
       </c>
@@ -13703,7 +13722,7 @@
       </c>
       <c r="I264" s="1">
         <f>G264-F264</f>
-        <v>197000</v>
+        <v>0</v>
       </c>
       <c r="J264" s="1">
         <v>197000</v>
@@ -13832,8 +13851,11 @@
       <c r="E267" s="8">
         <v>45579</v>
       </c>
+      <c r="F267" s="1">
+        <v>1077000</v>
+      </c>
       <c r="G267" s="1">
-        <v>1167000</v>
+        <v>1077000</v>
       </c>
       <c r="H267" s="1" cm="1">
         <f t="array" ref="H267">IFERROR(LOOKUP(2,1/(($B$2:B266=B267)*($C$2:C266=C267)), $L$2:L266), 0)</f>
@@ -13841,18 +13863,18 @@
       </c>
       <c r="I267" s="1">
         <f>G267-F267</f>
-        <v>1167000</v>
+        <v>0</v>
       </c>
       <c r="J267" s="1">
         <v>1100000</v>
       </c>
       <c r="K267" s="1">
         <f>G267-J267</f>
-        <v>67000</v>
+        <v>-23000</v>
       </c>
       <c r="L267" s="1">
         <f>G267-J267+H267</f>
-        <v>157000</v>
+        <v>67000</v>
       </c>
       <c r="M267" s="1">
         <v>50000</v>
@@ -13929,27 +13951,30 @@
       <c r="E269" s="8">
         <v>45589</v>
       </c>
+      <c r="F269" s="1">
+        <v>1397000</v>
+      </c>
       <c r="G269" s="1">
-        <v>1441000</v>
+        <v>1397000</v>
       </c>
       <c r="H269" s="1" cm="1">
         <f t="array" ref="H269">IFERROR(LOOKUP(2,1/(($B$2:B268=B269)*($C$2:C268=C269)), $L$2:L268), 0)</f>
-        <v>269000</v>
+        <v>44000</v>
       </c>
       <c r="I269" s="1">
         <f>G269-F269</f>
-        <v>1441000</v>
+        <v>0</v>
       </c>
       <c r="J269" s="1">
         <v>1441000</v>
       </c>
       <c r="K269" s="1">
         <f>G269-J269</f>
-        <v>0</v>
+        <v>-44000</v>
       </c>
       <c r="L269" s="1">
         <f>G269-J269+H269</f>
-        <v>269000</v>
+        <v>0</v>
       </c>
       <c r="M269" s="1">
         <v>40000</v>
@@ -13959,7 +13984,7 @@
    IFERROR(INDEX(Table1[Tanggal Pembayaran], MATCH(1,
    (Table1[[#This Row],[Nama Mandor]] = Table1[Nama Mandor]) * (Table1[[#This Row],[Nama Pekerja]] = Table1[Nama Pekerja]) * (Table1[[#This Row],[Tanggal Pembayaran]] &lt; Table1[Tanggal Pembayaran]), 0)), "No Next Payment"),
    "")</f>
-        <v>No Next Payment</v>
+        <v/>
       </c>
     </row>
     <row r="270" spans="1:14">
@@ -13976,37 +14001,36 @@
       <c r="E270" s="8">
         <v>45584</v>
       </c>
+      <c r="F270" s="1">
+        <v>6423000</v>
+      </c>
       <c r="G270" s="1">
-        <v>9540000</v>
+        <v>6423000</v>
       </c>
       <c r="H270" s="1" cm="1">
         <f t="array" ref="H270">IFERROR(LOOKUP(2,1/(($B$2:B269=B270)*($C$2:C269=C270)), $L$2:L269), 0)</f>
-        <v>626000</v>
+        <v>0</v>
       </c>
       <c r="I270" s="1">
         <f>G270-F270</f>
-        <v>9540000</v>
+        <v>0</v>
       </c>
       <c r="J270" s="1">
         <v>6423000</v>
       </c>
       <c r="K270" s="1">
         <f>G270-J270</f>
-        <v>3117000</v>
+        <v>0</v>
       </c>
       <c r="L270" s="1">
         <f>G270-J270+H270</f>
-        <v>3743000</v>
+        <v>0</v>
       </c>
       <c r="M270" s="1">
         <v>100000</v>
       </c>
-      <c r="N270" s="9" t="str" cm="1">
-        <f t="array" ref="N270">IF(Table1[[#This Row],[Total Kurang Bayar]] &lt;&gt; 0,
-   IFERROR(INDEX(Table1[Tanggal Pembayaran], MATCH(1,
-   (Table1[[#This Row],[Nama Mandor]] = Table1[Nama Mandor]) * (Table1[[#This Row],[Nama Pekerja]] = Table1[Nama Pekerja]) * (Table1[[#This Row],[Tanggal Pembayaran]] &lt; Table1[Tanggal Pembayaran]), 0)), "No Next Payment"),
-   "")</f>
-        <v>No Next Payment</v>
+      <c r="N270" s="9" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="271" spans="1:14">
@@ -14085,36 +14109,36 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K1" t="s">
         <v>102</v>
       </c>
-      <c r="C1" t="s">
+      <c r="L1" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="G1" t="s">
-        <v>104</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="N1" s="11" t="s">
         <v>105</v>
-      </c>
-      <c r="K1" t="s">
-        <v>101</v>
-      </c>
-      <c r="L1" t="s">
-        <v>102</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B2">
         <v>24</v>
@@ -14127,7 +14151,7 @@
         <v>100877</v>
       </c>
       <c r="J2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="K2" t="s">
         <v>55</v>
@@ -14151,7 +14175,7 @@
         <v>1101320</v>
       </c>
       <c r="J3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="N3" s="11">
         <v>50000</v>
@@ -14199,7 +14223,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -14216,7 +14240,7 @@
         <v>4103352</v>
       </c>
       <c r="J6" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="N6" s="11">
         <v>150000</v>
@@ -14234,7 +14258,7 @@
         <v>5103462</v>
       </c>
       <c r="J7" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="N7" s="11">
         <v>300000</v>
@@ -14314,7 +14338,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B14">
         <v>7</v>
@@ -14393,7 +14417,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B20">
         <v>5</v>

</xml_diff>